<commit_message>
Update for Apr 19
</commit_message>
<xml_diff>
--- a/excelsheets/probables.xlsx
+++ b/excelsheets/probables.xlsx
@@ -622,61 +622,64 @@
                   <c:v>274</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>299</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>356</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>399</c:v>
+                  <c:v>401</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>431</c:v>
+                  <c:v>433</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>439</c:v>
+                  <c:v>441</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>446</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>500</c:v>
+                  <c:v>504</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>506</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>528</c:v>
+                  <c:v>529</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>454</c:v>
+                  <c:v>459</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>424</c:v>
+                  <c:v>431</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>396</c:v>
+                  <c:v>412</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>381</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>382</c:v>
+                  <c:v>402</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>354</c:v>
+                  <c:v>385</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>279</c:v>
+                  <c:v>311</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>206</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>119</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>14</c:v>
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -966,101 +969,110 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="8">
+                  <c:v>4.4735729386892178</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.4735729386892178</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.9823819591261453</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.4735729386892178</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.9647639182522907</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.4735729386892178</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16.030303030303031</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.197040169133192</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.012684989429175</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>36.16138125440451</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43.766455250176179</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>62.779140239605354</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>72.844679351656097</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>96.181818181818187</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>96.181818181818187</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>122.50133897110641</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>195.34601832276252</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>195.34601832276252</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>209.95968992248061</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>209.95968992248061</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>265.28287526427061</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>266.77406624383366</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>253.65158562367864</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>260.95842142353769</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>250.6692036645525</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>249.17801268498943</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>257.97603946441154</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>274.0063424947146</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>265.28287526427061</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>199.67047216349542</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>249.17801268498943</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>179.31571529245949</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.4777385159010601</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.4777385159010601</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.9851590106007069</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.4777385159010601</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.9703180212014137</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.4777385159010601</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16.0452296819788</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>13.209328621908128</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>19.030388692579507</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>36.195053003533566</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43.807208480565372</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>62.762968197879857</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>71.569187279151947</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>94.778798586572435</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>94.778798586572435</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>121.12282685512368</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>194.03533568904592</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>194.03533568904592</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>210.15519434628976</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>211.49851590106007</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>268.44042402826852</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>266.94784452296818</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>255.23109540636042</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>268.44042402826852</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>256.72367491166079</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>255.23109540636042</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>265.52989399293284</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>283.06770318021199</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>277.09738515901063</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>215.90162544169613</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>217.39420494699647</c:v>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1076,8 +1088,8 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="476259648"/>
-        <c:axId val="476260208"/>
+        <c:axId val="289900352"/>
+        <c:axId val="296094416"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1618,11 +1630,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="476259648"/>
-        <c:axId val="476260208"/>
+        <c:axId val="289900352"/>
+        <c:axId val="296094416"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="476259648"/>
+        <c:axId val="289900352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1664,7 +1676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476260208"/>
+        <c:crossAx val="296094416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1673,7 +1685,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="476260208"/>
+        <c:axId val="296094416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1723,7 +1735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476259648"/>
+        <c:crossAx val="289900352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2366,7 +2378,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2377,7 +2389,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661400" cy="6290733"/>
+    <xdr:ext cx="8667750" cy="6298406"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2666,7 +2678,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2728,15 +2740,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -2752,8 +2764,11 @@
       <c r="F1">
         <v>418</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2772,8 +2787,11 @@
       <c r="F2">
         <v>7075</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>7095</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2792,33 +2810,36 @@
       <c r="F3">
         <v>528</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>313</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>314</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>315</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>316</v>
       </c>
@@ -2837,8 +2858,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>317</v>
       </c>
@@ -2857,8 +2881,11 @@
       <c r="F10">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>318</v>
       </c>
@@ -2877,8 +2904,11 @@
       <c r="F11">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>319</v>
       </c>
@@ -2897,8 +2927,11 @@
       <c r="F12">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>320</v>
       </c>
@@ -2917,8 +2950,11 @@
       <c r="F13">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>321</v>
       </c>
@@ -2937,8 +2973,11 @@
       <c r="F14">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>322</v>
       </c>
@@ -2957,8 +2996,11 @@
       <c r="F15">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>323</v>
       </c>
@@ -2977,8 +3019,11 @@
       <c r="F16">
         <v>215</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>324</v>
       </c>
@@ -2997,8 +3042,11 @@
       <c r="F17">
         <v>177</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>325</v>
       </c>
@@ -3017,8 +3065,11 @@
       <c r="F18">
         <v>255</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>326</v>
       </c>
@@ -3037,8 +3088,11 @@
       <c r="F19">
         <v>485</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>327</v>
       </c>
@@ -3057,8 +3111,11 @@
       <c r="F20">
         <v>587</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>328</v>
       </c>
@@ -3077,8 +3134,11 @@
       <c r="F21">
         <v>841</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>329</v>
       </c>
@@ -3097,8 +3157,11 @@
       <c r="F22">
         <v>959</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>330</v>
       </c>
@@ -3117,8 +3180,11 @@
       <c r="F23">
         <v>1270</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>331</v>
       </c>
@@ -3137,8 +3203,11 @@
       <c r="F24">
         <v>1270</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>401</v>
       </c>
@@ -3157,8 +3226,11 @@
       <c r="F25">
         <v>1623</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>402</v>
       </c>
@@ -3177,8 +3249,11 @@
       <c r="F26">
         <v>2600</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>403</v>
       </c>
@@ -3197,8 +3272,11 @@
       <c r="F27">
         <v>2600</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>404</v>
       </c>
@@ -3217,8 +3295,11 @@
       <c r="F28">
         <v>2816</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>2816</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>405</v>
       </c>
@@ -3237,8 +3318,11 @@
       <c r="F29">
         <v>2834</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <v>2816</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>406</v>
       </c>
@@ -3257,8 +3341,11 @@
       <c r="F30">
         <v>3597</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>3558</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>407</v>
       </c>
@@ -3277,8 +3364,11 @@
       <c r="F31">
         <v>3577</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <v>3578</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>408</v>
       </c>
@@ -3297,8 +3387,11 @@
       <c r="F32">
         <v>3420</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>3402</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>409</v>
       </c>
@@ -3317,8 +3410,11 @@
       <c r="F33">
         <v>3597</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>410</v>
       </c>
@@ -3337,8 +3433,11 @@
       <c r="F34">
         <v>3440</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>3362</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>411</v>
       </c>
@@ -3357,8 +3456,11 @@
       <c r="F35">
         <v>3420</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <v>3342</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>412</v>
       </c>
@@ -3377,8 +3479,11 @@
       <c r="F36">
         <v>3558</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <v>3460</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>413</v>
       </c>
@@ -3394,8 +3499,11 @@
       <c r="F37">
         <v>3793</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <v>3675</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>414</v>
       </c>
@@ -3408,8 +3516,11 @@
       <c r="F38">
         <v>3713</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <v>3558</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>415</v>
       </c>
@@ -3419,18 +3530,32 @@
       <c r="F39">
         <v>2893</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <v>2678</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>416</v>
       </c>
       <c r="F40">
         <v>2913</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <v>3342</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>417</v>
+      </c>
+      <c r="G41">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -3440,15 +3565,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -3464,795 +3589,959 @@
       <c r="F1">
         <v>418</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>316</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <f>Raw!B9*Raw!B$3/Raw!B$2</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>Raw!C9*Raw!C$3/Raw!C$2</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>Raw!D9*Raw!D$3/Raw!D$2</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>Raw!E9*Raw!E$3/Raw!E$2</f>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f>Raw!F9*Raw!F$3/Raw!F$2</f>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>Raw!G9*Raw!G$3/Raw!G$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>317</v>
       </c>
       <c r="B8">
-        <f>Raw!B9*Raw!B$3/Raw!B$2</f>
-        <v>0</v>
+        <f>Raw!B10*Raw!B$3/Raw!B$2</f>
+        <v>4.4089023010184833</v>
       </c>
       <c r="C8">
-        <f>Raw!C9*Raw!C$3/Raw!C$2</f>
-        <v>0</v>
+        <f>Raw!C10*Raw!C$3/Raw!C$2</f>
+        <v>4.4089023010184833</v>
       </c>
       <c r="D8">
-        <f>Raw!D9*Raw!D$3/Raw!D$2</f>
-        <v>0</v>
+        <f>Raw!D10*Raw!D$3/Raw!D$2</f>
+        <v>4.4095776681506438</v>
       </c>
       <c r="E8">
-        <f>Raw!E9*Raw!E$3/Raw!E$2</f>
-        <v>0</v>
+        <f>Raw!E10*Raw!E$3/Raw!E$2</f>
+        <v>4.4754239724058635</v>
       </c>
       <c r="F8">
-        <f>Raw!F9*Raw!F$3/Raw!F$2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F10*Raw!F$3/Raw!F$2</f>
+        <v>4.4777385159010601</v>
+      </c>
+      <c r="G8">
+        <f>Raw!G10*Raw!G$3/Raw!G$2</f>
+        <v>4.4735729386892178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>318</v>
       </c>
       <c r="B9">
-        <f>Raw!B10*Raw!B$3/Raw!B$2</f>
+        <f>Raw!B11*Raw!B$3/Raw!B$2</f>
         <v>4.4089023010184833</v>
       </c>
       <c r="C9">
-        <f>Raw!C10*Raw!C$3/Raw!C$2</f>
+        <f>Raw!C11*Raw!C$3/Raw!C$2</f>
         <v>4.4089023010184833</v>
       </c>
       <c r="D9">
-        <f>Raw!D10*Raw!D$3/Raw!D$2</f>
+        <f>Raw!D11*Raw!D$3/Raw!D$2</f>
         <v>4.4095776681506438</v>
       </c>
       <c r="E9">
-        <f>Raw!E10*Raw!E$3/Raw!E$2</f>
+        <f>Raw!E11*Raw!E$3/Raw!E$2</f>
         <v>4.4754239724058635</v>
       </c>
       <c r="F9">
-        <f>Raw!F10*Raw!F$3/Raw!F$2</f>
+        <f>Raw!F11*Raw!F$3/Raw!F$2</f>
         <v>4.4777385159010601</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <f>Raw!G11*Raw!G$3/Raw!G$2</f>
+        <v>4.4735729386892178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>319</v>
       </c>
       <c r="B10">
-        <f>Raw!B11*Raw!B$3/Raw!B$2</f>
-        <v>4.4089023010184833</v>
+        <f>Raw!B12*Raw!B$3/Raw!B$2</f>
+        <v>2.9392682006789892</v>
       </c>
       <c r="C10">
-        <f>Raw!C11*Raw!C$3/Raw!C$2</f>
-        <v>4.4089023010184833</v>
+        <f>Raw!C12*Raw!C$3/Raw!C$2</f>
+        <v>2.9392682006789892</v>
       </c>
       <c r="D10">
-        <f>Raw!D11*Raw!D$3/Raw!D$2</f>
-        <v>4.4095776681506438</v>
+        <f>Raw!D12*Raw!D$3/Raw!D$2</f>
+        <v>2.9397184454337624</v>
       </c>
       <c r="E10">
-        <f>Raw!E11*Raw!E$3/Raw!E$2</f>
-        <v>4.4754239724058635</v>
+        <f>Raw!E12*Raw!E$3/Raw!E$2</f>
+        <v>2.9836159816039092</v>
       </c>
       <c r="F10">
-        <f>Raw!F11*Raw!F$3/Raw!F$2</f>
-        <v>4.4777385159010601</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F12*Raw!F$3/Raw!F$2</f>
+        <v>2.9851590106007069</v>
+      </c>
+      <c r="G10">
+        <f>Raw!G12*Raw!G$3/Raw!G$2</f>
+        <v>2.9823819591261453</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>320</v>
       </c>
       <c r="B11">
-        <f>Raw!B12*Raw!B$3/Raw!B$2</f>
-        <v>2.9392682006789892</v>
+        <f>Raw!B13*Raw!B$3/Raw!B$2</f>
+        <v>5.8173016471771657</v>
       </c>
       <c r="C11">
-        <f>Raw!C12*Raw!C$3/Raw!C$2</f>
-        <v>2.9392682006789892</v>
+        <f>Raw!C13*Raw!C$3/Raw!C$2</f>
+        <v>5.8173016471771657</v>
       </c>
       <c r="D11">
-        <f>Raw!D12*Raw!D$3/Raw!D$2</f>
-        <v>2.9397184454337624</v>
+        <f>Raw!D13*Raw!D$3/Raw!D$2</f>
+        <v>4.4095776681506438</v>
       </c>
       <c r="E11">
-        <f>Raw!E12*Raw!E$3/Raw!E$2</f>
-        <v>2.9836159816039092</v>
+        <f>Raw!E13*Raw!E$3/Raw!E$2</f>
+        <v>4.4754239724058635</v>
       </c>
       <c r="F11">
-        <f>Raw!F12*Raw!F$3/Raw!F$2</f>
-        <v>2.9851590106007069</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F13*Raw!F$3/Raw!F$2</f>
+        <v>4.4777385159010601</v>
+      </c>
+      <c r="G11">
+        <f>Raw!G13*Raw!G$3/Raw!G$2</f>
+        <v>4.4735729386892178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>321</v>
       </c>
       <c r="B12">
-        <f>Raw!B13*Raw!B$3/Raw!B$2</f>
-        <v>5.8173016471771657</v>
+        <f>Raw!B14*Raw!B$3/Raw!B$2</f>
+        <v>7.3481705016974725</v>
       </c>
       <c r="C12">
-        <f>Raw!C13*Raw!C$3/Raw!C$2</f>
-        <v>5.8173016471771657</v>
+        <f>Raw!C14*Raw!C$3/Raw!C$2</f>
+        <v>7.3481705016974725</v>
       </c>
       <c r="D12">
-        <f>Raw!D13*Raw!D$3/Raw!D$2</f>
+        <f>Raw!D14*Raw!D$3/Raw!D$2</f>
         <v>4.4095776681506438</v>
       </c>
       <c r="E12">
-        <f>Raw!E13*Raw!E$3/Raw!E$2</f>
-        <v>4.4754239724058635</v>
+        <f>Raw!E14*Raw!E$3/Raw!E$2</f>
+        <v>5.9672319632078183</v>
       </c>
       <c r="F12">
-        <f>Raw!F13*Raw!F$3/Raw!F$2</f>
-        <v>4.4777385159010601</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F14*Raw!F$3/Raw!F$2</f>
+        <v>5.9703180212014137</v>
+      </c>
+      <c r="G12">
+        <f>Raw!G14*Raw!G$3/Raw!G$2</f>
+        <v>5.9647639182522907</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>322</v>
       </c>
       <c r="B13">
-        <f>Raw!B14*Raw!B$3/Raw!B$2</f>
-        <v>7.3481705016974725</v>
+        <f>Raw!B15*Raw!B$3/Raw!B$2</f>
+        <v>4.4089023010184833</v>
       </c>
       <c r="C13">
-        <f>Raw!C14*Raw!C$3/Raw!C$2</f>
-        <v>7.3481705016974725</v>
+        <f>Raw!C15*Raw!C$3/Raw!C$2</f>
+        <v>4.4089023010184833</v>
       </c>
       <c r="D13">
-        <f>Raw!D14*Raw!D$3/Raw!D$2</f>
+        <f>Raw!D15*Raw!D$3/Raw!D$2</f>
         <v>4.4095776681506438</v>
       </c>
       <c r="E13">
-        <f>Raw!E14*Raw!E$3/Raw!E$2</f>
-        <v>5.9672319632078183</v>
+        <f>Raw!E15*Raw!E$3/Raw!E$2</f>
+        <v>4.4754239724058635</v>
       </c>
       <c r="F13">
-        <f>Raw!F14*Raw!F$3/Raw!F$2</f>
-        <v>5.9703180212014137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F15*Raw!F$3/Raw!F$2</f>
+        <v>4.4777385159010601</v>
+      </c>
+      <c r="G13">
+        <f>Raw!G15*Raw!G$3/Raw!G$2</f>
+        <v>4.4735729386892178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>323</v>
       </c>
       <c r="B14">
-        <f>Raw!B15*Raw!B$3/Raw!B$2</f>
-        <v>4.4089023010184833</v>
+        <f>Raw!B16*Raw!B$3/Raw!B$2</f>
+        <v>14.573871495033321</v>
       </c>
       <c r="C14">
-        <f>Raw!C15*Raw!C$3/Raw!C$2</f>
-        <v>4.4089023010184833</v>
+        <f>Raw!C16*Raw!C$3/Raw!C$2</f>
+        <v>14.573871495033321</v>
       </c>
       <c r="D14">
-        <f>Raw!D15*Raw!D$3/Raw!D$2</f>
-        <v>4.4095776681506438</v>
+        <f>Raw!D16*Raw!D$3/Raw!D$2</f>
+        <v>14.576103958609073</v>
       </c>
       <c r="E14">
-        <f>Raw!E15*Raw!E$3/Raw!E$2</f>
-        <v>4.4754239724058635</v>
+        <f>Raw!E16*Raw!E$3/Raw!E$2</f>
+        <v>14.545127910319056</v>
       </c>
       <c r="F14">
-        <f>Raw!F15*Raw!F$3/Raw!F$2</f>
-        <v>4.4777385159010601</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F16*Raw!F$3/Raw!F$2</f>
+        <v>16.0452296819788</v>
+      </c>
+      <c r="G14">
+        <f>Raw!G16*Raw!G$3/Raw!G$2</f>
+        <v>16.030303030303031</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>324</v>
       </c>
       <c r="B15">
-        <f>Raw!B16*Raw!B$3/Raw!B$2</f>
-        <v>14.573871495033321</v>
+        <f>Raw!B17*Raw!B$3/Raw!B$2</f>
+        <v>13.165472148874638</v>
       </c>
       <c r="C15">
-        <f>Raw!C16*Raw!C$3/Raw!C$2</f>
-        <v>14.573871495033321</v>
+        <f>Raw!C17*Raw!C$3/Raw!C$2</f>
+        <v>13.165472148874638</v>
       </c>
       <c r="D15">
-        <f>Raw!D16*Raw!D$3/Raw!D$2</f>
-        <v>14.576103958609073</v>
+        <f>Raw!D17*Raw!D$3/Raw!D$2</f>
+        <v>13.167488870172061</v>
       </c>
       <c r="E15">
-        <f>Raw!E16*Raw!E$3/Raw!E$2</f>
-        <v>14.545127910319056</v>
+        <f>Raw!E17*Raw!E$3/Raw!E$2</f>
+        <v>13.202500718597298</v>
       </c>
       <c r="F15">
-        <f>Raw!F16*Raw!F$3/Raw!F$2</f>
-        <v>16.0452296819788</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F17*Raw!F$3/Raw!F$2</f>
+        <v>13.209328621908128</v>
+      </c>
+      <c r="G15">
+        <f>Raw!G17*Raw!G$3/Raw!G$2</f>
+        <v>13.197040169133192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>325</v>
       </c>
       <c r="B16">
-        <f>Raw!B17*Raw!B$3/Raw!B$2</f>
-        <v>13.165472148874638</v>
+        <f>Raw!B18*Raw!B$3/Raw!B$2</f>
+        <v>21.922041996730794</v>
       </c>
       <c r="C16">
-        <f>Raw!C17*Raw!C$3/Raw!C$2</f>
-        <v>13.165472148874638</v>
+        <f>Raw!C18*Raw!C$3/Raw!C$2</f>
+        <v>21.922041996730794</v>
       </c>
       <c r="D16">
-        <f>Raw!D17*Raw!D$3/Raw!D$2</f>
-        <v>13.167488870172061</v>
+        <f>Raw!D18*Raw!D$3/Raw!D$2</f>
+        <v>17.515822404042837</v>
       </c>
       <c r="E16">
-        <f>Raw!E17*Raw!E$3/Raw!E$2</f>
-        <v>13.202500718597298</v>
+        <f>Raw!E18*Raw!E$3/Raw!E$2</f>
+        <v>19.02055188272492</v>
       </c>
       <c r="F16">
-        <f>Raw!F17*Raw!F$3/Raw!F$2</f>
-        <v>13.209328621908128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F18*Raw!F$3/Raw!F$2</f>
+        <v>19.030388692579507</v>
+      </c>
+      <c r="G16">
+        <f>Raw!G18*Raw!G$3/Raw!G$2</f>
+        <v>19.012684989429175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>326</v>
       </c>
       <c r="B17">
-        <f>Raw!B18*Raw!B$3/Raw!B$2</f>
-        <v>21.922041996730794</v>
+        <f>Raw!B19*Raw!B$3/Raw!B$2</f>
+        <v>45.252483339620269</v>
       </c>
       <c r="C17">
-        <f>Raw!C18*Raw!C$3/Raw!C$2</f>
-        <v>21.922041996730794</v>
+        <f>Raw!C19*Raw!C$3/Raw!C$2</f>
+        <v>45.252483339620269</v>
       </c>
       <c r="D17">
-        <f>Raw!D18*Raw!D$3/Raw!D$2</f>
-        <v>17.515822404042837</v>
+        <f>Raw!D19*Raw!D$3/Raw!D$2</f>
+        <v>36.50150403080255</v>
       </c>
       <c r="E17">
-        <f>Raw!E18*Raw!E$3/Raw!E$2</f>
-        <v>19.02055188272492</v>
+        <f>Raw!E19*Raw!E$3/Raw!E$2</f>
+        <v>36.176343776947398</v>
       </c>
       <c r="F17">
-        <f>Raw!F18*Raw!F$3/Raw!F$2</f>
-        <v>19.030388692579507</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F19*Raw!F$3/Raw!F$2</f>
+        <v>36.195053003533566</v>
+      </c>
+      <c r="G17">
+        <f>Raw!G19*Raw!G$3/Raw!G$2</f>
+        <v>36.16138125440451</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>327</v>
       </c>
       <c r="B18">
-        <f>Raw!B19*Raw!B$3/Raw!B$2</f>
-        <v>45.252483339620269</v>
+        <f>Raw!B20*Raw!B$3/Raw!B$2</f>
+        <v>64.174022381491255</v>
       </c>
       <c r="C18">
-        <f>Raw!C19*Raw!C$3/Raw!C$2</f>
-        <v>45.252483339620269</v>
+        <f>Raw!C20*Raw!C$3/Raw!C$2</f>
+        <v>64.174022381491255</v>
       </c>
       <c r="D18">
-        <f>Raw!D19*Raw!D$3/Raw!D$2</f>
-        <v>36.50150403080255</v>
+        <f>Raw!D20*Raw!D$3/Raw!D$2</f>
+        <v>45.259415232823969</v>
       </c>
       <c r="E18">
-        <f>Raw!E19*Raw!E$3/Raw!E$2</f>
-        <v>36.176343776947398</v>
+        <f>Raw!E20*Raw!E$3/Raw!E$2</f>
+        <v>41.845214141994823</v>
       </c>
       <c r="F18">
-        <f>Raw!F19*Raw!F$3/Raw!F$2</f>
-        <v>36.195053003533566</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F20*Raw!F$3/Raw!F$2</f>
+        <v>43.807208480565372</v>
+      </c>
+      <c r="G18">
+        <f>Raw!G20*Raw!G$3/Raw!G$2</f>
+        <v>43.766455250176179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>328</v>
       </c>
       <c r="B19">
-        <f>Raw!B20*Raw!B$3/Raw!B$2</f>
-        <v>64.174022381491255</v>
+        <f>Raw!B21*Raw!B$3/Raw!B$2</f>
+        <v>78.747893876524586</v>
       </c>
       <c r="C19">
-        <f>Raw!C20*Raw!C$3/Raw!C$2</f>
-        <v>64.174022381491255</v>
+        <f>Raw!C21*Raw!C$3/Raw!C$2</f>
+        <v>77.339494530365897</v>
       </c>
       <c r="D19">
-        <f>Raw!D20*Raw!D$3/Raw!D$2</f>
-        <v>45.259415232823969</v>
+        <f>Raw!D21*Raw!D$3/Raw!D$2</f>
+        <v>65.6537119480207</v>
       </c>
       <c r="E19">
-        <f>Raw!E20*Raw!E$3/Raw!E$2</f>
-        <v>41.845214141994823</v>
+        <f>Raw!E21*Raw!E$3/Raw!E$2</f>
+        <v>65.639551595286008</v>
       </c>
       <c r="F19">
-        <f>Raw!F20*Raw!F$3/Raw!F$2</f>
-        <v>43.807208480565372</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F21*Raw!F$3/Raw!F$2</f>
+        <v>62.762968197879857</v>
+      </c>
+      <c r="G19">
+        <f>Raw!G21*Raw!G$3/Raw!G$2</f>
+        <v>62.779140239605354</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>329</v>
       </c>
       <c r="B20">
-        <f>Raw!B21*Raw!B$3/Raw!B$2</f>
-        <v>78.747893876524586</v>
+        <f>Raw!B22*Raw!B$3/Raw!B$2</f>
+        <v>87.504463724380741</v>
       </c>
       <c r="C20">
-        <f>Raw!C21*Raw!C$3/Raw!C$2</f>
-        <v>77.339494530365897</v>
+        <f>Raw!C22*Raw!C$3/Raw!C$2</f>
+        <v>87.504463724380741</v>
       </c>
       <c r="D20">
-        <f>Raw!D21*Raw!D$3/Raw!D$2</f>
-        <v>65.6537119480207</v>
+        <f>Raw!D22*Raw!D$3/Raw!D$2</f>
+        <v>71.533148838888224</v>
       </c>
       <c r="E20">
-        <f>Raw!E21*Raw!E$3/Raw!E$2</f>
-        <v>65.639551595286008</v>
+        <f>Raw!E22*Raw!E$3/Raw!E$2</f>
+        <v>71.532193158953717</v>
       </c>
       <c r="F20">
-        <f>Raw!F21*Raw!F$3/Raw!F$2</f>
-        <v>62.762968197879857</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F22*Raw!F$3/Raw!F$2</f>
+        <v>71.569187279151947</v>
+      </c>
+      <c r="G20">
+        <f>Raw!G22*Raw!G$3/Raw!G$2</f>
+        <v>72.844679351656097</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>330</v>
       </c>
       <c r="B21">
-        <f>Raw!B22*Raw!B$3/Raw!B$2</f>
-        <v>87.504463724380741</v>
+        <f>Raw!B23*Raw!B$3/Raw!B$2</f>
+        <v>110.83490506727021</v>
       </c>
       <c r="C21">
-        <f>Raw!C22*Raw!C$3/Raw!C$2</f>
-        <v>87.504463724380741</v>
+        <f>Raw!C23*Raw!C$3/Raw!C$2</f>
+        <v>110.83490506727021</v>
       </c>
       <c r="D21">
-        <f>Raw!D22*Raw!D$3/Raw!D$2</f>
-        <v>71.533148838888224</v>
+        <f>Raw!D23*Raw!D$3/Raw!D$2</f>
+        <v>96.275779087955726</v>
       </c>
       <c r="E21">
-        <f>Raw!E22*Raw!E$3/Raw!E$2</f>
-        <v>71.532193158953717</v>
+        <f>Raw!E23*Raw!E$3/Raw!E$2</f>
+        <v>99.205231388329977</v>
       </c>
       <c r="F21">
-        <f>Raw!F22*Raw!F$3/Raw!F$2</f>
-        <v>71.569187279151947</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F23*Raw!F$3/Raw!F$2</f>
+        <v>94.778798586572435</v>
+      </c>
+      <c r="G21">
+        <f>Raw!G23*Raw!G$3/Raw!G$2</f>
+        <v>96.181818181818187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>331</v>
       </c>
       <c r="B22">
-        <f>Raw!B23*Raw!B$3/Raw!B$2</f>
-        <v>110.83490506727021</v>
+        <f>Raw!B24*Raw!B$3/Raw!B$2</f>
+        <v>116.65220671444737</v>
       </c>
       <c r="C22">
-        <f>Raw!C23*Raw!C$3/Raw!C$2</f>
-        <v>110.83490506727021</v>
+        <f>Raw!C24*Raw!C$3/Raw!C$2</f>
+        <v>116.65220671444737</v>
       </c>
       <c r="D22">
-        <f>Raw!D23*Raw!D$3/Raw!D$2</f>
+        <f>Raw!D24*Raw!D$3/Raw!D$2</f>
         <v>96.275779087955726</v>
       </c>
       <c r="E22">
-        <f>Raw!E23*Raw!E$3/Raw!E$2</f>
-        <v>99.205231388329977</v>
+        <f>Raw!E24*Raw!E$3/Raw!E$2</f>
+        <v>96.221615406726073</v>
       </c>
       <c r="F22">
-        <f>Raw!F23*Raw!F$3/Raw!F$2</f>
+        <f>Raw!F24*Raw!F$3/Raw!F$2</f>
         <v>94.778798586572435</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <f>Raw!G24*Raw!G$3/Raw!G$2</f>
+        <v>96.181818181818187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>401</v>
       </c>
       <c r="B23">
-        <f>Raw!B24*Raw!B$3/Raw!B$2</f>
-        <v>116.65220671444737</v>
+        <f>Raw!B25*Raw!B$3/Raw!B$2</f>
+        <v>151.678486105872</v>
       </c>
       <c r="C23">
-        <f>Raw!C24*Raw!C$3/Raw!C$2</f>
-        <v>116.65220671444737</v>
+        <f>Raw!C25*Raw!C$3/Raw!C$2</f>
+        <v>145.79994970451401</v>
       </c>
       <c r="D23">
-        <f>Raw!D24*Raw!D$3/Raw!D$2</f>
-        <v>96.275779087955726</v>
+        <f>Raw!D25*Raw!D$3/Raw!D$2</f>
+        <v>121.07965347130309</v>
       </c>
       <c r="E23">
-        <f>Raw!E24*Raw!E$3/Raw!E$2</f>
-        <v>96.221615406726073</v>
+        <f>Raw!E25*Raw!E$3/Raw!E$2</f>
+        <v>121.06021845357861</v>
       </c>
       <c r="F23">
-        <f>Raw!F24*Raw!F$3/Raw!F$2</f>
-        <v>94.778798586572435</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F25*Raw!F$3/Raw!F$2</f>
+        <v>121.12282685512368</v>
+      </c>
+      <c r="G23">
+        <f>Raw!G25*Raw!G$3/Raw!G$2</f>
+        <v>122.50133897110641</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>402</v>
       </c>
       <c r="B24">
-        <f>Raw!B25*Raw!B$3/Raw!B$2</f>
-        <v>151.678486105872</v>
+        <f>Raw!B26*Raw!B$3/Raw!B$2</f>
+        <v>223.13944423487993</v>
       </c>
       <c r="C24">
-        <f>Raw!C25*Raw!C$3/Raw!C$2</f>
-        <v>145.79994970451401</v>
+        <f>Raw!C26*Raw!C$3/Raw!C$2</f>
+        <v>217.32214258770276</v>
       </c>
       <c r="D24">
-        <f>Raw!D25*Raw!D$3/Raw!D$2</f>
-        <v>121.07965347130309</v>
+        <f>Raw!D26*Raw!D$3/Raw!D$2</f>
+        <v>195.43003248706535</v>
       </c>
       <c r="E24">
-        <f>Raw!E25*Raw!E$3/Raw!E$2</f>
-        <v>121.06021845357861</v>
+        <f>Raw!E26*Raw!E$3/Raw!E$2</f>
+        <v>198.26128197757976</v>
       </c>
       <c r="F24">
-        <f>Raw!F25*Raw!F$3/Raw!F$2</f>
-        <v>121.12282685512368</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F26*Raw!F$3/Raw!F$2</f>
+        <v>194.03533568904592</v>
+      </c>
+      <c r="G24">
+        <f>Raw!G26*Raw!G$3/Raw!G$2</f>
+        <v>195.34601832276252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>403</v>
       </c>
       <c r="B25">
-        <f>Raw!B26*Raw!B$3/Raw!B$2</f>
-        <v>223.13944423487993</v>
+        <f>Raw!B27*Raw!B$3/Raw!B$2</f>
+        <v>205.62630453916762</v>
       </c>
       <c r="C25">
-        <f>Raw!C26*Raw!C$3/Raw!C$2</f>
-        <v>217.32214258770276</v>
+        <f>Raw!C27*Raw!C$3/Raw!C$2</f>
+        <v>207.03470388532628</v>
       </c>
       <c r="D25">
-        <f>Raw!D26*Raw!D$3/Raw!D$2</f>
-        <v>195.43003248706535</v>
+        <f>Raw!D27*Raw!D$3/Raw!D$2</f>
+        <v>194.02141739862833</v>
       </c>
       <c r="E25">
-        <f>Raw!E26*Raw!E$3/Raw!E$2</f>
-        <v>198.26128197757976</v>
+        <f>Raw!E27*Raw!E$3/Raw!E$2</f>
+        <v>195.42684679505604</v>
       </c>
       <c r="F25">
-        <f>Raw!F26*Raw!F$3/Raw!F$2</f>
+        <f>Raw!F27*Raw!F$3/Raw!F$2</f>
         <v>194.03533568904592</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <f>Raw!G27*Raw!G$3/Raw!G$2</f>
+        <v>195.34601832276252</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>404</v>
       </c>
       <c r="B26">
-        <f>Raw!B27*Raw!B$3/Raw!B$2</f>
-        <v>205.62630453916762</v>
+        <f>Raw!B28*Raw!B$3/Raw!B$2</f>
+        <v>230.36514522821577</v>
       </c>
       <c r="C26">
-        <f>Raw!C27*Raw!C$3/Raw!C$2</f>
-        <v>207.03470388532628</v>
+        <f>Raw!C28*Raw!C$3/Raw!C$2</f>
+        <v>226.07871243555891</v>
       </c>
       <c r="D26">
-        <f>Raw!D27*Raw!D$3/Raw!D$2</f>
-        <v>194.02141739862833</v>
+        <f>Raw!D28*Raw!D$3/Raw!D$2</f>
+        <v>210.0061364456744</v>
       </c>
       <c r="E26">
-        <f>Raw!E27*Raw!E$3/Raw!E$2</f>
-        <v>195.42684679505604</v>
+        <f>Raw!E28*Raw!E$3/Raw!E$2</f>
+        <v>211.38919229663696</v>
       </c>
       <c r="F26">
-        <f>Raw!F27*Raw!F$3/Raw!F$2</f>
-        <v>194.03533568904592</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F28*Raw!F$3/Raw!F$2</f>
+        <v>210.15519434628976</v>
+      </c>
+      <c r="G26">
+        <f>Raw!G28*Raw!G$3/Raw!G$2</f>
+        <v>209.95968992248061</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>405</v>
       </c>
       <c r="B27">
-        <f>Raw!B28*Raw!B$3/Raw!B$2</f>
-        <v>230.36514522821577</v>
+        <f>Raw!B29*Raw!B$3/Raw!B$2</f>
+        <v>231.89601408273609</v>
       </c>
       <c r="C27">
-        <f>Raw!C28*Raw!C$3/Raw!C$2</f>
-        <v>226.07871243555891</v>
+        <f>Raw!C29*Raw!C$3/Raw!C$2</f>
+        <v>227.4871117817176</v>
       </c>
       <c r="D27">
-        <f>Raw!D28*Raw!D$3/Raw!D$2</f>
+        <f>Raw!D29*Raw!D$3/Raw!D$2</f>
         <v>210.0061364456744</v>
       </c>
       <c r="E27">
-        <f>Raw!E28*Raw!E$3/Raw!E$2</f>
-        <v>211.38919229663696</v>
+        <f>Raw!E29*Raw!E$3/Raw!E$2</f>
+        <v>214.37280827824088</v>
       </c>
       <c r="F27">
-        <f>Raw!F28*Raw!F$3/Raw!F$2</f>
-        <v>210.15519434628976</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F29*Raw!F$3/Raw!F$2</f>
+        <v>211.49851590106007</v>
+      </c>
+      <c r="G27">
+        <f>Raw!G29*Raw!G$3/Raw!G$2</f>
+        <v>209.95968992248061</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>406</v>
       </c>
       <c r="B28">
-        <f>Raw!B29*Raw!B$3/Raw!B$2</f>
-        <v>231.89601408273609</v>
+        <f>Raw!B30*Raw!B$3/Raw!B$2</f>
+        <v>301.88733811140452</v>
       </c>
       <c r="C28">
-        <f>Raw!C29*Raw!C$3/Raw!C$2</f>
-        <v>227.4871117817176</v>
+        <f>Raw!C30*Raw!C$3/Raw!C$2</f>
+        <v>297.47843581038603</v>
       </c>
       <c r="D28">
-        <f>Raw!D29*Raw!D$3/Raw!D$2</f>
-        <v>210.0061364456744</v>
+        <f>Raw!D30*Raw!D$3/Raw!D$2</f>
+        <v>274.18998917097821</v>
       </c>
       <c r="E28">
-        <f>Raw!E29*Raw!E$3/Raw!E$2</f>
-        <v>214.37280827824088</v>
+        <f>Raw!E30*Raw!E$3/Raw!E$2</f>
+        <v>276.95415349238289</v>
       </c>
       <c r="F28">
-        <f>Raw!F29*Raw!F$3/Raw!F$2</f>
-        <v>211.49851590106007</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F30*Raw!F$3/Raw!F$2</f>
+        <v>268.44042402826852</v>
+      </c>
+      <c r="G28">
+        <f>Raw!G30*Raw!G$3/Raw!G$2</f>
+        <v>265.28287526427061</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>407</v>
       </c>
       <c r="B29">
-        <f>Raw!B30*Raw!B$3/Raw!B$2</f>
-        <v>301.88733811140452</v>
+        <f>Raw!B31*Raw!B$3/Raw!B$2</f>
+        <v>297.47843581038603</v>
       </c>
       <c r="C29">
-        <f>Raw!C30*Raw!C$3/Raw!C$2</f>
+        <f>Raw!C31*Raw!C$3/Raw!C$2</f>
         <v>297.47843581038603</v>
       </c>
       <c r="D29">
-        <f>Raw!D30*Raw!D$3/Raw!D$2</f>
+        <f>Raw!D31*Raw!D$3/Raw!D$2</f>
         <v>274.18998917097821</v>
       </c>
       <c r="E29">
-        <f>Raw!E30*Raw!E$3/Raw!E$2</f>
-        <v>276.95415349238289</v>
+        <f>Raw!E31*Raw!E$3/Raw!E$2</f>
+        <v>274.11971830985914</v>
       </c>
       <c r="F29">
-        <f>Raw!F30*Raw!F$3/Raw!F$2</f>
-        <v>268.44042402826852</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F31*Raw!F$3/Raw!F$2</f>
+        <v>266.94784452296818</v>
+      </c>
+      <c r="G29">
+        <f>Raw!G31*Raw!G$3/Raw!G$2</f>
+        <v>266.77406624383366</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>408</v>
       </c>
       <c r="B30">
-        <f>Raw!B31*Raw!B$3/Raw!B$2</f>
-        <v>297.47843581038603</v>
+        <f>Raw!B32*Raw!B$3/Raw!B$2</f>
+        <v>285.78259776185087</v>
       </c>
       <c r="C30">
-        <f>Raw!C31*Raw!C$3/Raw!C$2</f>
-        <v>297.47843581038603</v>
+        <f>Raw!C32*Raw!C$3/Raw!C$2</f>
+        <v>285.78259776185087</v>
       </c>
       <c r="D30">
-        <f>Raw!D31*Raw!D$3/Raw!D$2</f>
-        <v>274.18998917097821</v>
+        <f>Raw!D32*Raw!D$3/Raw!D$2</f>
+        <v>262.49235952352302</v>
       </c>
       <c r="E30">
-        <f>Raw!E31*Raw!E$3/Raw!E$2</f>
-        <v>274.11971830985914</v>
+        <f>Raw!E32*Raw!E$3/Raw!E$2</f>
+        <v>261.06639839034204</v>
       </c>
       <c r="F30">
-        <f>Raw!F31*Raw!F$3/Raw!F$2</f>
-        <v>266.94784452296818</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F32*Raw!F$3/Raw!F$2</f>
+        <v>255.23109540636042</v>
+      </c>
+      <c r="G30">
+        <f>Raw!G32*Raw!G$3/Raw!G$2</f>
+        <v>253.65158562367864</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>409</v>
       </c>
       <c r="B31">
-        <f>Raw!B32*Raw!B$3/Raw!B$2</f>
-        <v>285.78259776185087</v>
+        <f>Raw!B33*Raw!B$3/Raw!B$2</f>
+        <v>320.80887715327549</v>
       </c>
       <c r="C31">
-        <f>Raw!C32*Raw!C$3/Raw!C$2</f>
-        <v>285.78259776185087</v>
+        <f>Raw!C33*Raw!C$3/Raw!C$2</f>
+        <v>303.29573745756318</v>
       </c>
       <c r="D31">
-        <f>Raw!D32*Raw!D$3/Raw!D$2</f>
-        <v>262.49235952352302</v>
+        <f>Raw!D33*Raw!D$3/Raw!D$2</f>
+        <v>282.94790037299964</v>
       </c>
       <c r="E31">
-        <f>Raw!E32*Raw!E$3/Raw!E$2</f>
-        <v>261.06639839034204</v>
+        <f>Raw!E33*Raw!E$3/Raw!E$2</f>
+        <v>275.61152630066113</v>
       </c>
       <c r="F31">
-        <f>Raw!F32*Raw!F$3/Raw!F$2</f>
-        <v>255.23109540636042</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F33*Raw!F$3/Raw!F$2</f>
+        <v>268.44042402826852</v>
+      </c>
+      <c r="G31">
+        <f>Raw!G33*Raw!G$3/Raw!G$2</f>
+        <v>260.95842142353769</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>410</v>
       </c>
       <c r="B32">
-        <f>Raw!B33*Raw!B$3/Raw!B$2</f>
-        <v>320.80887715327549</v>
+        <f>Raw!B34*Raw!B$3/Raw!B$2</f>
+        <v>296.07003646422731</v>
       </c>
       <c r="C32">
-        <f>Raw!C33*Raw!C$3/Raw!C$2</f>
-        <v>303.29573745756318</v>
+        <f>Raw!C34*Raw!C$3/Raw!C$2</f>
+        <v>304.82660631208347</v>
       </c>
       <c r="D32">
-        <f>Raw!D33*Raw!D$3/Raw!D$2</f>
+        <f>Raw!D34*Raw!D$3/Raw!D$2</f>
         <v>282.94790037299964</v>
       </c>
       <c r="E32">
-        <f>Raw!E33*Raw!E$3/Raw!E$2</f>
-        <v>275.61152630066113</v>
+        <f>Raw!E34*Raw!E$3/Raw!E$2</f>
+        <v>272.62791031905721</v>
       </c>
       <c r="F32">
-        <f>Raw!F33*Raw!F$3/Raw!F$2</f>
-        <v>268.44042402826852</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F34*Raw!F$3/Raw!F$2</f>
+        <v>256.72367491166079</v>
+      </c>
+      <c r="G32">
+        <f>Raw!G34*Raw!G$3/Raw!G$2</f>
+        <v>250.6692036645525</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>411</v>
       </c>
       <c r="B33">
-        <f>Raw!B34*Raw!B$3/Raw!B$2</f>
-        <v>296.07003646422731</v>
+        <f>Raw!B35*Raw!B$3/Raw!B$2</f>
+        <v>303.29573745756318</v>
       </c>
       <c r="C33">
-        <f>Raw!C34*Raw!C$3/Raw!C$2</f>
+        <f>Raw!C35*Raw!C$3/Raw!C$2</f>
         <v>304.82660631208347</v>
       </c>
       <c r="D33">
-        <f>Raw!D34*Raw!D$3/Raw!D$2</f>
-        <v>282.94790037299964</v>
+        <f>Raw!D35*Raw!D$3/Raw!D$2</f>
+        <v>275.65984839369509</v>
       </c>
       <c r="E33">
-        <f>Raw!E34*Raw!E$3/Raw!E$2</f>
-        <v>272.62791031905721</v>
+        <f>Raw!E35*Raw!E$3/Raw!E$2</f>
+        <v>266.88444955446965</v>
       </c>
       <c r="F33">
-        <f>Raw!F34*Raw!F$3/Raw!F$2</f>
-        <v>256.72367491166079</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F35*Raw!F$3/Raw!F$2</f>
+        <v>255.23109540636042</v>
+      </c>
+      <c r="G33">
+        <f>Raw!G35*Raw!G$3/Raw!G$2</f>
+        <v>249.17801268498943</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>412</v>
       </c>
       <c r="B34">
-        <f>Raw!B35*Raw!B$3/Raw!B$2</f>
-        <v>303.29573745756318</v>
+        <f>Raw!B36*Raw!B$3/Raw!B$2</f>
+        <v>297.47843581038603</v>
       </c>
       <c r="C34">
-        <f>Raw!C35*Raw!C$3/Raw!C$2</f>
-        <v>304.82660631208347</v>
+        <f>Raw!C36*Raw!C$3/Raw!C$2</f>
+        <v>320.80887715327549</v>
       </c>
       <c r="D34">
-        <f>Raw!D35*Raw!D$3/Raw!D$2</f>
-        <v>275.65984839369509</v>
+        <f>Raw!D36*Raw!D$3/Raw!D$2</f>
+        <v>290.29719648658403</v>
       </c>
       <c r="E34">
-        <f>Raw!E35*Raw!E$3/Raw!E$2</f>
-        <v>266.88444955446965</v>
+        <f>Raw!E36*Raw!E$3/Raw!E$2</f>
+        <v>287.24762862891635</v>
       </c>
       <c r="F34">
-        <f>Raw!F35*Raw!F$3/Raw!F$2</f>
-        <v>255.23109540636042</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F36*Raw!F$3/Raw!F$2</f>
+        <v>265.52989399293284</v>
+      </c>
+      <c r="G34">
+        <f>Raw!G36*Raw!G$3/Raw!G$2</f>
+        <v>257.97603946441154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>413</v>
       </c>
       <c r="B35">
-        <f>Raw!B36*Raw!B$3/Raw!B$2</f>
-        <v>297.47843581038603</v>
+        <f>Raw!B37*Raw!B$3/Raw!B$2</f>
+        <v>0</v>
       </c>
       <c r="C35">
-        <f>Raw!C36*Raw!C$3/Raw!C$2</f>
-        <v>320.80887715327549</v>
+        <f>Raw!C37*Raw!C$3/Raw!C$2</f>
+        <v>287.31346661637116</v>
       </c>
       <c r="D35">
-        <f>Raw!D36*Raw!D$3/Raw!D$2</f>
-        <v>290.29719648658403</v>
+        <f>Raw!D37*Raw!D$3/Raw!D$2</f>
+        <v>282.94790037299964</v>
       </c>
       <c r="E35">
-        <f>Raw!E36*Raw!E$3/Raw!E$2</f>
-        <v>287.24762862891635</v>
+        <f>Raw!E37*Raw!E$3/Raw!E$2</f>
+        <v>316.41247484909456</v>
       </c>
       <c r="F35">
-        <f>Raw!F36*Raw!F$3/Raw!F$2</f>
-        <v>265.52989399293284</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F37*Raw!F$3/Raw!F$2</f>
+        <v>283.06770318021199</v>
+      </c>
+      <c r="G35">
+        <f>Raw!G37*Raw!G$3/Raw!G$2</f>
+        <v>274.0063424947146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>414</v>
       </c>
       <c r="C36">
-        <f>Raw!C37*Raw!C$3/Raw!C$2</f>
-        <v>287.31346661637116</v>
+        <f>Raw!C38*Raw!C$3/Raw!C$2</f>
+        <v>0</v>
       </c>
       <c r="D36">
-        <f>Raw!D37*Raw!D$3/Raw!D$2</f>
-        <v>282.94790037299964</v>
+        <f>Raw!D38*Raw!D$3/Raw!D$2</f>
+        <v>239.15834436289256</v>
       </c>
       <c r="E36">
-        <f>Raw!E37*Raw!E$3/Raw!E$2</f>
-        <v>316.41247484909456</v>
+        <f>Raw!E38*Raw!E$3/Raw!E$2</f>
+        <v>317.9042828398965</v>
       </c>
       <c r="F36">
-        <f>Raw!F37*Raw!F$3/Raw!F$2</f>
-        <v>283.06770318021199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F38*Raw!F$3/Raw!F$2</f>
+        <v>277.09738515901063</v>
+      </c>
+      <c r="G36">
+        <f>Raw!G38*Raw!G$3/Raw!G$2</f>
+        <v>265.28287526427061</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>415</v>
       </c>
       <c r="D37">
-        <f>Raw!D38*Raw!D$3/Raw!D$2</f>
-        <v>239.15834436289256</v>
+        <f>Raw!D39*Raw!D$3/Raw!D$2</f>
+        <v>0</v>
       </c>
       <c r="E37">
-        <f>Raw!E38*Raw!E$3/Raw!E$2</f>
-        <v>317.9042828398965</v>
+        <f>Raw!E39*Raw!E$3/Raw!E$2</f>
+        <v>278.44596148318482</v>
       </c>
       <c r="F37">
-        <f>Raw!F38*Raw!F$3/Raw!F$2</f>
-        <v>277.09738515901063</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F39*Raw!F$3/Raw!F$2</f>
+        <v>215.90162544169613</v>
+      </c>
+      <c r="G37">
+        <f>Raw!G39*Raw!G$3/Raw!G$2</f>
+        <v>199.67047216349542</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>416</v>
       </c>
       <c r="E38">
-        <f>Raw!E39*Raw!E$3/Raw!E$2</f>
-        <v>278.44596148318482</v>
+        <f>Raw!E40*Raw!E$3/Raw!E$2</f>
+        <v>0</v>
       </c>
       <c r="F38">
-        <f>Raw!F39*Raw!F$3/Raw!F$2</f>
-        <v>215.90162544169613</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <f>Raw!F40*Raw!F$3/Raw!F$2</f>
+        <v>217.39420494699647</v>
+      </c>
+      <c r="G38">
+        <f>Raw!G40*Raw!G$3/Raw!G$2</f>
+        <v>249.17801268498943</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>417</v>
       </c>
       <c r="F39">
-        <f>Raw!F40*Raw!F$3/Raw!F$2</f>
-        <v>217.39420494699647</v>
+        <f>Raw!F41*Raw!F$3/Raw!F$2</f>
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f>Raw!G41*Raw!G$3/Raw!G$2</f>
+        <v>179.31571529245949</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>418</v>
+      </c>
+      <c r="G40">
+        <f>Raw!G42*Raw!G$3/Raw!G$2</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4262,15 +4551,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X48"/>
+  <dimension ref="A1:Y49"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11:X48"/>
+    <sheetView topLeftCell="J31" workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11:Y49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>325</v>
       </c>
@@ -4340,8 +4629,11 @@
       <c r="X1">
         <v>418</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y1">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>302</v>
       </c>
@@ -4414,8 +4706,11 @@
       <c r="X2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>303</v>
       </c>
@@ -4488,8 +4783,11 @@
       <c r="X3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>304</v>
       </c>
@@ -4562,8 +4860,11 @@
       <c r="X4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>305</v>
       </c>
@@ -4636,8 +4937,11 @@
       <c r="X5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>306</v>
       </c>
@@ -4710,8 +5014,11 @@
       <c r="X6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>307</v>
       </c>
@@ -4784,8 +5091,11 @@
       <c r="X7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>308</v>
       </c>
@@ -4858,8 +5168,11 @@
       <c r="X8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>309</v>
       </c>
@@ -4932,8 +5245,11 @@
       <c r="X9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>310</v>
       </c>
@@ -5006,8 +5322,11 @@
       <c r="X10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>311</v>
       </c>
@@ -5080,8 +5399,11 @@
       <c r="X11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>312</v>
       </c>
@@ -5154,8 +5476,11 @@
       <c r="X12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>313</v>
       </c>
@@ -5228,8 +5553,11 @@
       <c r="X13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>314</v>
       </c>
@@ -5302,8 +5630,11 @@
       <c r="X14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>315</v>
       </c>
@@ -5376,8 +5707,11 @@
       <c r="X15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>316</v>
       </c>
@@ -5450,8 +5784,11 @@
       <c r="X16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>317</v>
       </c>
@@ -5524,8 +5861,11 @@
       <c r="X17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>318</v>
       </c>
@@ -5598,8 +5938,11 @@
       <c r="X18">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>319</v>
       </c>
@@ -5672,8 +6015,11 @@
       <c r="X19">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>320</v>
       </c>
@@ -5746,8 +6092,11 @@
       <c r="X20">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y20">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>321</v>
       </c>
@@ -5820,8 +6169,11 @@
       <c r="X21">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>322</v>
       </c>
@@ -5894,8 +6246,11 @@
       <c r="X22">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y22">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>323</v>
       </c>
@@ -5968,8 +6323,11 @@
       <c r="X23">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y23">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>324</v>
       </c>
@@ -6042,8 +6400,11 @@
       <c r="X24">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>325</v>
       </c>
@@ -6116,8 +6477,11 @@
       <c r="X25">
         <v>120</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>326</v>
       </c>
@@ -6187,8 +6551,11 @@
       <c r="X26">
         <v>185</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y26">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>327</v>
       </c>
@@ -6255,8 +6622,11 @@
       <c r="X27">
         <v>205</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y27">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>328</v>
       </c>
@@ -6320,8 +6690,11 @@
       <c r="X28">
         <v>256</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y28">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>329</v>
       </c>
@@ -6385,8 +6758,11 @@
       <c r="X29">
         <v>274</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y29">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>330</v>
       </c>
@@ -6450,8 +6826,11 @@
       <c r="X30">
         <v>299</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y30">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>331</v>
       </c>
@@ -6512,8 +6891,11 @@
       <c r="X31">
         <v>356</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y31">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>401</v>
       </c>
@@ -6571,8 +6953,11 @@
       <c r="X32">
         <v>399</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y32">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>402</v>
       </c>
@@ -6627,8 +7012,11 @@
       <c r="X33">
         <v>431</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y33">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>403</v>
       </c>
@@ -6680,8 +7068,11 @@
       <c r="X34">
         <v>439</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y34">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>404</v>
       </c>
@@ -6730,8 +7121,11 @@
       <c r="X35">
         <v>446</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y35">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>405</v>
       </c>
@@ -6777,8 +7171,11 @@
       <c r="X36">
         <v>500</v>
       </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y36">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>406</v>
       </c>
@@ -6821,8 +7218,11 @@
       <c r="X37">
         <v>506</v>
       </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y37">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>407</v>
       </c>
@@ -6862,8 +7262,11 @@
       <c r="X38">
         <v>528</v>
       </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y38">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>408</v>
       </c>
@@ -6900,8 +7303,11 @@
       <c r="X39">
         <v>454</v>
       </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y39">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>409</v>
       </c>
@@ -6935,8 +7341,11 @@
       <c r="X40">
         <v>424</v>
       </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y40">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>410</v>
       </c>
@@ -6967,8 +7376,11 @@
       <c r="X41">
         <v>396</v>
       </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y41">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>411</v>
       </c>
@@ -6996,8 +7408,11 @@
       <c r="X42">
         <v>381</v>
       </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y42">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>412</v>
       </c>
@@ -7022,8 +7437,11 @@
       <c r="X43">
         <v>382</v>
       </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y43">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>413</v>
       </c>
@@ -7045,8 +7463,11 @@
       <c r="X44">
         <v>354</v>
       </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y44">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>414</v>
       </c>
@@ -7062,8 +7483,11 @@
       <c r="X45">
         <v>279</v>
       </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y45">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>415</v>
       </c>
@@ -7076,8 +7500,11 @@
       <c r="X46">
         <v>206</v>
       </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y46">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>416</v>
       </c>
@@ -7087,13 +7514,27 @@
       <c r="X47">
         <v>119</v>
       </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y47">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>417</v>
       </c>
       <c r="X48">
         <v>14</v>
+      </c>
+      <c r="Y48">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>418</v>
+      </c>
+      <c r="Y49">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -7103,15 +7544,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G40" sqref="G40:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -7127,8 +7568,11 @@
       <c r="F1">
         <v>418</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>311</v>
       </c>
@@ -7152,8 +7596,12 @@
         <f>Confirmed!X11+Daily!F2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <f>Confirmed!Y11+Daily!G2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>312</v>
       </c>
@@ -7177,8 +7625,12 @@
         <f>Confirmed!X12+Daily!F3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <f>Confirmed!Y12+Daily!G3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>313</v>
       </c>
@@ -7202,8 +7654,12 @@
         <f>Confirmed!X13+Daily!F4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <f>Confirmed!Y13+Daily!G4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314</v>
       </c>
@@ -7227,8 +7683,12 @@
         <f>Confirmed!X14+Daily!F5</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <f>Confirmed!Y14+Daily!G5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>315</v>
       </c>
@@ -7252,8 +7712,12 @@
         <f>Confirmed!X15+Daily!F6</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <f>Confirmed!Y15+Daily!G6</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>316</v>
       </c>
@@ -7277,33 +7741,41 @@
         <f>Confirmed!X16+Daily!F7</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <f>Confirmed!Y16+Daily!G7</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>317</v>
       </c>
       <c r="B8">
         <f>Confirmed!T17+Daily!B8</f>
-        <v>7</v>
+        <v>11.408902301018482</v>
       </c>
       <c r="C8">
         <f>Confirmed!U17+Daily!C8</f>
-        <v>7</v>
+        <v>11.408902301018482</v>
       </c>
       <c r="D8">
         <f>Confirmed!V17+Daily!D8</f>
-        <v>7</v>
+        <v>11.409577668150643</v>
       </c>
       <c r="E8">
         <f>Confirmed!W17+Daily!E8</f>
-        <v>7</v>
+        <v>11.475423972405864</v>
       </c>
       <c r="F8">
         <f>Confirmed!X17+Daily!F8</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>11.477738515901059</v>
+      </c>
+      <c r="G8">
+        <f>Confirmed!Y17+Daily!G8</f>
+        <v>11.473572938689218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>318</v>
       </c>
@@ -7327,68 +7799,80 @@
         <f>Confirmed!X18+Daily!F9</f>
         <v>25.477738515901059</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <f>Confirmed!Y18+Daily!G9</f>
+        <v>25.473572938689216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>319</v>
       </c>
       <c r="B10">
         <f>Confirmed!T19+Daily!B10</f>
-        <v>29.408902301018482</v>
+        <v>27.939268200678988</v>
       </c>
       <c r="C10">
         <f>Confirmed!U19+Daily!C10</f>
-        <v>29.408902301018482</v>
+        <v>27.939268200678988</v>
       </c>
       <c r="D10">
         <f>Confirmed!V19+Daily!D10</f>
-        <v>29.409577668150643</v>
+        <v>27.939718445433762</v>
       </c>
       <c r="E10">
         <f>Confirmed!W19+Daily!E10</f>
-        <v>29.475423972405864</v>
+        <v>27.983615981603908</v>
       </c>
       <c r="F10">
         <f>Confirmed!X19+Daily!F10</f>
-        <v>29.477738515901059</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>27.985159010600707</v>
+      </c>
+      <c r="G10">
+        <f>Confirmed!Y19+Daily!G10</f>
+        <v>27.982381959126144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>320</v>
       </c>
       <c r="B11">
         <f>Confirmed!T20+Daily!B11</f>
-        <v>47.939268200678988</v>
+        <v>50.817301647177167</v>
       </c>
       <c r="C11">
         <f>Confirmed!U20+Daily!C11</f>
-        <v>47.939268200678988</v>
+        <v>50.817301647177167</v>
       </c>
       <c r="D11">
         <f>Confirmed!V20+Daily!D11</f>
-        <v>48.939718445433762</v>
+        <v>50.409577668150646</v>
       </c>
       <c r="E11">
         <f>Confirmed!W20+Daily!E11</f>
-        <v>48.983615981603911</v>
+        <v>50.475423972405864</v>
       </c>
       <c r="F11">
         <f>Confirmed!X20+Daily!F11</f>
-        <v>48.985159010600704</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>50.477738515901059</v>
+      </c>
+      <c r="G11">
+        <f>Confirmed!Y20+Daily!G11</f>
+        <v>50.473572938689216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>321</v>
       </c>
       <c r="B12">
         <f>Confirmed!T21+Daily!B12</f>
-        <v>41.817301647177167</v>
+        <v>43.348170501697474</v>
       </c>
       <c r="C12">
         <f>Confirmed!U21+Daily!C12</f>
-        <v>41.817301647177167</v>
+        <v>43.348170501697474</v>
       </c>
       <c r="D12">
         <f>Confirmed!V21+Daily!D12</f>
@@ -7396,24 +7880,28 @@
       </c>
       <c r="E12">
         <f>Confirmed!W21+Daily!E12</f>
-        <v>44.475423972405864</v>
+        <v>45.967231963207816</v>
       </c>
       <c r="F12">
         <f>Confirmed!X21+Daily!F12</f>
-        <v>44.477738515901059</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>45.970318021201415</v>
+      </c>
+      <c r="G12">
+        <f>Confirmed!Y21+Daily!G12</f>
+        <v>45.964763918252288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>322</v>
       </c>
       <c r="B13">
         <f>Confirmed!T22+Daily!B13</f>
-        <v>52.348170501697474</v>
+        <v>49.408902301018486</v>
       </c>
       <c r="C13">
         <f>Confirmed!U22+Daily!C13</f>
-        <v>52.348170501697474</v>
+        <v>49.408902301018486</v>
       </c>
       <c r="D13">
         <f>Confirmed!V22+Daily!D13</f>
@@ -7421,224 +7909,260 @@
       </c>
       <c r="E13">
         <f>Confirmed!W22+Daily!E13</f>
-        <v>51.967231963207816</v>
+        <v>50.475423972405864</v>
       </c>
       <c r="F13">
         <f>Confirmed!X22+Daily!F13</f>
-        <v>53.970318021201415</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>52.477738515901059</v>
+      </c>
+      <c r="G13">
+        <f>Confirmed!Y22+Daily!G13</f>
+        <v>52.473572938689216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>323</v>
       </c>
       <c r="B14">
         <f>Confirmed!T23+Daily!B14</f>
-        <v>84.408902301018486</v>
+        <v>94.573871495033316</v>
       </c>
       <c r="C14">
         <f>Confirmed!U23+Daily!C14</f>
-        <v>84.408902301018486</v>
+        <v>94.573871495033316</v>
       </c>
       <c r="D14">
         <f>Confirmed!V23+Daily!D14</f>
-        <v>85.409577668150646</v>
+        <v>95.576103958609067</v>
       </c>
       <c r="E14">
         <f>Confirmed!W23+Daily!E14</f>
-        <v>85.475423972405864</v>
+        <v>95.545127910319053</v>
       </c>
       <c r="F14">
         <f>Confirmed!X23+Daily!F14</f>
-        <v>85.477738515901066</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>97.045229681978796</v>
+      </c>
+      <c r="G14">
+        <f>Confirmed!Y23+Daily!G14</f>
+        <v>97.030303030303031</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>324</v>
       </c>
       <c r="B15">
         <f>Confirmed!T24+Daily!B15</f>
-        <v>104.57387149503332</v>
+        <v>103.16547214887464</v>
       </c>
       <c r="C15">
         <f>Confirmed!U24+Daily!C15</f>
-        <v>104.57387149503332</v>
+        <v>103.16547214887464</v>
       </c>
       <c r="D15">
         <f>Confirmed!V24+Daily!D15</f>
-        <v>106.57610395860907</v>
+        <v>105.16748887017206</v>
       </c>
       <c r="E15">
         <f>Confirmed!W24+Daily!E15</f>
-        <v>106.54512791031905</v>
+        <v>105.20250071859729</v>
       </c>
       <c r="F15">
         <f>Confirmed!X24+Daily!F15</f>
-        <v>108.0452296819788</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>105.20932862190813</v>
+      </c>
+      <c r="G15">
+        <f>Confirmed!Y24+Daily!G15</f>
+        <v>105.19704016913319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>325</v>
       </c>
       <c r="B16">
         <f>Confirmed!T25+Daily!B16</f>
-        <v>126.16547214887464</v>
+        <v>134.9220419967308</v>
       </c>
       <c r="C16">
         <f>Confirmed!U25+Daily!C16</f>
-        <v>126.16547214887464</v>
+        <v>134.9220419967308</v>
       </c>
       <c r="D16">
         <f>Confirmed!V25+Daily!D16</f>
-        <v>128.16748887017206</v>
+        <v>132.51582240404284</v>
       </c>
       <c r="E16">
         <f>Confirmed!W25+Daily!E16</f>
-        <v>132.20250071859729</v>
+        <v>138.02055188272493</v>
       </c>
       <c r="F16">
         <f>Confirmed!X25+Daily!F16</f>
-        <v>133.20932862190813</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>139.03038869257949</v>
+      </c>
+      <c r="G16">
+        <f>Confirmed!Y25+Daily!G16</f>
+        <v>139.01268498942918</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>326</v>
       </c>
       <c r="B17">
         <f>Confirmed!T26+Daily!B17</f>
-        <v>194.9220419967308</v>
+        <v>218.25248333962026</v>
       </c>
       <c r="C17">
         <f>Confirmed!U26+Daily!C17</f>
-        <v>194.9220419967308</v>
+        <v>218.25248333962026</v>
       </c>
       <c r="D17">
         <f>Confirmed!V26+Daily!D17</f>
-        <v>195.51582240404284</v>
+        <v>214.50150403080255</v>
       </c>
       <c r="E17">
         <f>Confirmed!W26+Daily!E17</f>
-        <v>203.02055188272493</v>
+        <v>220.17634377694739</v>
       </c>
       <c r="F17">
         <f>Confirmed!X26+Daily!F17</f>
-        <v>204.03038869257949</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>221.19505300353356</v>
+      </c>
+      <c r="G17">
+        <f>Confirmed!Y26+Daily!G17</f>
+        <v>221.16138125440452</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>327</v>
       </c>
       <c r="B18">
         <f>Confirmed!T27+Daily!B18</f>
-        <v>229.25248333962026</v>
+        <v>248.17402238149126</v>
       </c>
       <c r="C18">
         <f>Confirmed!U27+Daily!C18</f>
-        <v>229.25248333962026</v>
+        <v>248.17402238149126</v>
       </c>
       <c r="D18">
         <f>Confirmed!V27+Daily!D18</f>
-        <v>234.50150403080255</v>
+        <v>243.25941523282398</v>
       </c>
       <c r="E18">
         <f>Confirmed!W27+Daily!E18</f>
-        <v>239.17634377694739</v>
+        <v>244.84521414199483</v>
       </c>
       <c r="F18">
         <f>Confirmed!X27+Daily!F18</f>
-        <v>241.19505300353356</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>248.80720848056538</v>
+      </c>
+      <c r="G18">
+        <f>Confirmed!Y27+Daily!G18</f>
+        <v>248.76645525017619</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>328</v>
       </c>
       <c r="B19">
         <f>Confirmed!T28+Daily!B19</f>
-        <v>300.17402238149123</v>
+        <v>314.74789387652459</v>
       </c>
       <c r="C19">
         <f>Confirmed!U28+Daily!C19</f>
-        <v>300.17402238149123</v>
+        <v>313.33949453036587</v>
       </c>
       <c r="D19">
         <f>Confirmed!V28+Daily!D19</f>
-        <v>292.25941523282398</v>
+        <v>312.65371194802071</v>
       </c>
       <c r="E19">
         <f>Confirmed!W28+Daily!E19</f>
-        <v>294.8452141419948</v>
+        <v>318.63955159528598</v>
       </c>
       <c r="F19">
         <f>Confirmed!X28+Daily!F19</f>
-        <v>299.80720848056535</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>318.76296819787984</v>
+      </c>
+      <c r="G19">
+        <f>Confirmed!Y28+Daily!G19</f>
+        <v>318.77914023960534</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>329</v>
       </c>
       <c r="B20">
         <f>Confirmed!T29+Daily!B20</f>
-        <v>333.74789387652459</v>
+        <v>342.50446372438074</v>
       </c>
       <c r="C20">
         <f>Confirmed!U29+Daily!C20</f>
-        <v>332.33949453036587</v>
+        <v>342.50446372438074</v>
       </c>
       <c r="D20">
         <f>Confirmed!V29+Daily!D20</f>
-        <v>328.65371194802071</v>
+        <v>334.53314883888822</v>
       </c>
       <c r="E20">
         <f>Confirmed!W29+Daily!E20</f>
-        <v>339.63955159528598</v>
+        <v>345.5321931589537</v>
       </c>
       <c r="F20">
         <f>Confirmed!X29+Daily!F20</f>
-        <v>336.76296819787984</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>345.56918727915195</v>
+      </c>
+      <c r="G20">
+        <f>Confirmed!Y29+Daily!G20</f>
+        <v>346.84467935165611</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>330</v>
       </c>
       <c r="B21">
         <f>Confirmed!T30+Daily!B21</f>
-        <v>364.50446372438074</v>
+        <v>387.8349050672702</v>
       </c>
       <c r="C21">
         <f>Confirmed!U30+Daily!C21</f>
-        <v>364.50446372438074</v>
+        <v>387.8349050672702</v>
       </c>
       <c r="D21">
         <f>Confirmed!V30+Daily!D21</f>
-        <v>358.53314883888822</v>
+        <v>383.2757790879557</v>
       </c>
       <c r="E21">
         <f>Confirmed!W30+Daily!E21</f>
-        <v>366.5321931589537</v>
+        <v>394.20523138832999</v>
       </c>
       <c r="F21">
         <f>Confirmed!X30+Daily!F21</f>
-        <v>370.56918727915195</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>393.77879858657241</v>
+      </c>
+      <c r="G21">
+        <f>Confirmed!Y30+Daily!G21</f>
+        <v>396.18181818181819</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>331</v>
       </c>
       <c r="B22">
         <f>Confirmed!T31+Daily!B22</f>
-        <v>439.8349050672702</v>
+        <v>445.6522067144474</v>
       </c>
       <c r="C22">
         <f>Confirmed!U31+Daily!C22</f>
-        <v>439.8349050672702</v>
+        <v>445.6522067144474</v>
       </c>
       <c r="D22">
         <f>Confirmed!V31+Daily!D22</f>
@@ -7646,124 +8170,144 @@
       </c>
       <c r="E22">
         <f>Confirmed!W31+Daily!E22</f>
-        <v>454.20523138832999</v>
+        <v>451.22161540672607</v>
       </c>
       <c r="F22">
         <f>Confirmed!X31+Daily!F22</f>
         <v>450.77879858657241</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <f>Confirmed!Y31+Daily!G22</f>
+        <v>452.18181818181819</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>401</v>
       </c>
       <c r="B23">
         <f>Confirmed!T32+Daily!B23</f>
-        <v>482.6522067144474</v>
+        <v>517.67848610587203</v>
       </c>
       <c r="C23">
         <f>Confirmed!U32+Daily!C23</f>
-        <v>482.6522067144474</v>
+        <v>511.79994970451401</v>
       </c>
       <c r="D23">
         <f>Confirmed!V32+Daily!D23</f>
-        <v>479.2757790879557</v>
+        <v>504.07965347130312</v>
       </c>
       <c r="E23">
         <f>Confirmed!W32+Daily!E23</f>
-        <v>492.22161540672607</v>
+        <v>517.06021845357861</v>
       </c>
       <c r="F23">
         <f>Confirmed!X32+Daily!F23</f>
-        <v>493.77879858657241</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>520.12282685512366</v>
+      </c>
+      <c r="G23">
+        <f>Confirmed!Y32+Daily!G23</f>
+        <v>523.50133897110641</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>402</v>
       </c>
       <c r="B24">
         <f>Confirmed!T33+Daily!B24</f>
-        <v>549.67848610587203</v>
+        <v>621.13944423487987</v>
       </c>
       <c r="C24">
         <f>Confirmed!U33+Daily!C24</f>
-        <v>544.79994970451401</v>
+        <v>616.32214258770273</v>
       </c>
       <c r="D24">
         <f>Confirmed!V33+Daily!D24</f>
-        <v>532.07965347130312</v>
+        <v>606.43003248706532</v>
       </c>
       <c r="E24">
         <f>Confirmed!W33+Daily!E24</f>
-        <v>548.06021845357861</v>
+        <v>625.26128197757976</v>
       </c>
       <c r="F24">
         <f>Confirmed!X33+Daily!F24</f>
-        <v>552.12282685512366</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>625.03533568904595</v>
+      </c>
+      <c r="G24">
+        <f>Confirmed!Y33+Daily!G24</f>
+        <v>628.34601832276257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>403</v>
       </c>
       <c r="B25">
         <f>Confirmed!T34+Daily!B25</f>
-        <v>643.13944423487987</v>
+        <v>625.62630453916768</v>
       </c>
       <c r="C25">
         <f>Confirmed!U34+Daily!C25</f>
-        <v>638.32214258770273</v>
+        <v>628.03470388532628</v>
       </c>
       <c r="D25">
         <f>Confirmed!V34+Daily!D25</f>
-        <v>624.43003248706532</v>
+        <v>623.02141739862827</v>
       </c>
       <c r="E25">
         <f>Confirmed!W34+Daily!E25</f>
-        <v>634.26128197757976</v>
+        <v>631.42684679505601</v>
       </c>
       <c r="F25">
         <f>Confirmed!X34+Daily!F25</f>
         <v>633.03533568904595</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <f>Confirmed!Y34+Daily!G25</f>
+        <v>636.34601832276257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>404</v>
       </c>
       <c r="B26">
         <f>Confirmed!T35+Daily!B26</f>
-        <v>626.62630453916768</v>
+        <v>651.36514522821574</v>
       </c>
       <c r="C26">
         <f>Confirmed!U35+Daily!C26</f>
-        <v>628.03470388532628</v>
+        <v>647.07871243555894</v>
       </c>
       <c r="D26">
         <f>Confirmed!V35+Daily!D26</f>
-        <v>628.02141739862827</v>
+        <v>644.00613644567443</v>
       </c>
       <c r="E26">
         <f>Confirmed!W35+Daily!E26</f>
-        <v>638.42684679505601</v>
+        <v>654.38919229663702</v>
       </c>
       <c r="F26">
         <f>Confirmed!X35+Daily!F26</f>
-        <v>640.03533568904595</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>656.15519434628982</v>
+      </c>
+      <c r="G26">
+        <f>Confirmed!Y35+Daily!G26</f>
+        <v>655.95968992248061</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>405</v>
       </c>
       <c r="B27">
         <f>Confirmed!T36+Daily!B27</f>
-        <v>703.36514522821574</v>
+        <v>704.89601408273609</v>
       </c>
       <c r="C27">
         <f>Confirmed!U36+Daily!C27</f>
-        <v>698.07871243555894</v>
+        <v>699.48711178171766</v>
       </c>
       <c r="D27">
         <f>Confirmed!V36+Daily!D27</f>
@@ -7771,45 +8315,53 @@
       </c>
       <c r="E27">
         <f>Confirmed!W36+Daily!E27</f>
-        <v>707.38919229663702</v>
+        <v>710.37280827824088</v>
       </c>
       <c r="F27">
         <f>Confirmed!X36+Daily!F27</f>
-        <v>710.15519434628982</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>711.49851590106005</v>
+      </c>
+      <c r="G27">
+        <f>Confirmed!Y36+Daily!G27</f>
+        <v>713.95968992248061</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>406</v>
       </c>
       <c r="B28">
         <f>Confirmed!T37+Daily!B28</f>
-        <v>694.89601408273609</v>
+        <v>764.88733811140446</v>
       </c>
       <c r="C28">
         <f>Confirmed!U37+Daily!C28</f>
-        <v>690.48711178171766</v>
+        <v>760.47843581038603</v>
       </c>
       <c r="D28">
         <f>Confirmed!V37+Daily!D28</f>
-        <v>700.00613644567443</v>
+        <v>764.18998917097815</v>
       </c>
       <c r="E28">
         <f>Confirmed!W37+Daily!E28</f>
-        <v>713.37280827824088</v>
+        <v>775.95415349238283</v>
       </c>
       <c r="F28">
         <f>Confirmed!X37+Daily!F28</f>
-        <v>717.49851590106005</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>774.44042402826858</v>
+      </c>
+      <c r="G28">
+        <f>Confirmed!Y37+Daily!G28</f>
+        <v>775.28287526427061</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>407</v>
       </c>
       <c r="B29">
         <f>Confirmed!T38+Daily!B29</f>
-        <v>788.88733811140446</v>
+        <v>784.47843581038603</v>
       </c>
       <c r="C29">
         <f>Confirmed!U38+Daily!C29</f>
@@ -7821,74 +8373,86 @@
       </c>
       <c r="E29">
         <f>Confirmed!W38+Daily!E29</f>
-        <v>795.95415349238283</v>
+        <v>793.11971830985908</v>
       </c>
       <c r="F29">
         <f>Confirmed!X38+Daily!F29</f>
-        <v>796.44042402826858</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>794.94784452296813</v>
+      </c>
+      <c r="G29">
+        <f>Confirmed!Y38+Daily!G29</f>
+        <v>795.77406624383366</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>408</v>
       </c>
       <c r="B30">
         <f>Confirmed!T39+Daily!B30</f>
-        <v>708.47843581038603</v>
+        <v>696.78259776185087</v>
       </c>
       <c r="C30">
         <f>Confirmed!U39+Daily!C30</f>
-        <v>708.47843581038603</v>
+        <v>696.78259776185087</v>
       </c>
       <c r="D30">
         <f>Confirmed!V39+Daily!D30</f>
-        <v>704.18998917097815</v>
+        <v>692.49235952352296</v>
       </c>
       <c r="E30">
         <f>Confirmed!W39+Daily!E30</f>
-        <v>717.11971830985908</v>
+        <v>704.0663983903421</v>
       </c>
       <c r="F30">
         <f>Confirmed!X39+Daily!F30</f>
-        <v>720.94784452296813</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>709.2310954063604</v>
+      </c>
+      <c r="G30">
+        <f>Confirmed!Y39+Daily!G30</f>
+        <v>712.65158562367867</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>409</v>
       </c>
       <c r="B31">
         <f>Confirmed!T40+Daily!B31</f>
-        <v>643.78259776185087</v>
+        <v>678.80887715327549</v>
       </c>
       <c r="C31">
         <f>Confirmed!U40+Daily!C31</f>
-        <v>648.78259776185087</v>
+        <v>666.29573745756318</v>
       </c>
       <c r="D31">
         <f>Confirmed!V40+Daily!D31</f>
-        <v>653.49235952352296</v>
+        <v>673.94790037299958</v>
       </c>
       <c r="E31">
         <f>Confirmed!W40+Daily!E31</f>
-        <v>670.0663983903421</v>
+        <v>684.61152630066113</v>
       </c>
       <c r="F31">
         <f>Confirmed!X40+Daily!F31</f>
-        <v>679.2310954063604</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>692.44042402826858</v>
+      </c>
+      <c r="G31">
+        <f>Confirmed!Y40+Daily!G31</f>
+        <v>691.95842142353763</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>410</v>
       </c>
       <c r="B32">
         <f>Confirmed!T41+Daily!B32</f>
-        <v>636.80887715327549</v>
+        <v>612.07003646422731</v>
       </c>
       <c r="C32">
         <f>Confirmed!U41+Daily!C32</f>
-        <v>631.29573745756318</v>
+        <v>632.82660631208341</v>
       </c>
       <c r="D32">
         <f>Confirmed!V41+Daily!D32</f>
@@ -7896,20 +8460,24 @@
       </c>
       <c r="E32">
         <f>Confirmed!W41+Daily!E32</f>
-        <v>648.61152630066113</v>
+        <v>645.62791031905726</v>
       </c>
       <c r="F32">
         <f>Confirmed!X41+Daily!F32</f>
-        <v>664.44042402826858</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>652.72367491166074</v>
+      </c>
+      <c r="G32">
+        <f>Confirmed!Y41+Daily!G32</f>
+        <v>662.66920366455247</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>411</v>
       </c>
       <c r="B33">
         <f>Confirmed!T42+Daily!B33</f>
-        <v>560.07003646422731</v>
+        <v>567.29573745756318</v>
       </c>
       <c r="C33">
         <f>Confirmed!U42+Daily!C33</f>
@@ -7917,68 +8485,80 @@
       </c>
       <c r="D33">
         <f>Confirmed!V42+Daily!D33</f>
-        <v>611.94790037299958</v>
+        <v>604.65984839369503</v>
       </c>
       <c r="E33">
         <f>Confirmed!W42+Daily!E33</f>
-        <v>622.62791031905726</v>
+        <v>616.88444955446971</v>
       </c>
       <c r="F33">
         <f>Confirmed!X42+Daily!F33</f>
-        <v>637.72367491166074</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>636.2310954063604</v>
+      </c>
+      <c r="G33">
+        <f>Confirmed!Y42+Daily!G33</f>
+        <v>642.17801268498943</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>412</v>
       </c>
       <c r="B34">
         <f>Confirmed!T43+Daily!B34</f>
-        <v>498.29573745756318</v>
+        <v>492.47843581038603</v>
       </c>
       <c r="C34">
         <f>Confirmed!U43+Daily!C34</f>
-        <v>545.82660631208341</v>
+        <v>561.80887715327549</v>
       </c>
       <c r="D34">
         <f>Confirmed!V43+Daily!D34</f>
-        <v>578.65984839369503</v>
+        <v>593.29719648658397</v>
       </c>
       <c r="E34">
         <f>Confirmed!W43+Daily!E34</f>
-        <v>598.88444955446971</v>
+        <v>619.24762862891635</v>
       </c>
       <c r="F34">
         <f>Confirmed!X43+Daily!F34</f>
-        <v>637.2310954063604</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>647.52989399293278</v>
+      </c>
+      <c r="G34">
+        <f>Confirmed!Y43+Daily!G34</f>
+        <v>659.97603946441154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>413</v>
       </c>
       <c r="B35">
         <f>Confirmed!T44+Daily!B35</f>
-        <v>326.47843581038603</v>
+        <v>29</v>
       </c>
       <c r="C35">
         <f>Confirmed!U44+Daily!C35</f>
-        <v>476.80887715327549</v>
+        <v>443.31346661637116</v>
       </c>
       <c r="D35">
         <f>Confirmed!V44+Daily!D35</f>
-        <v>569.29719648658397</v>
+        <v>561.94790037299958</v>
       </c>
       <c r="E35">
         <f>Confirmed!W44+Daily!E35</f>
-        <v>601.24762862891635</v>
+        <v>630.41247484909456</v>
       </c>
       <c r="F35">
         <f>Confirmed!X44+Daily!F35</f>
-        <v>619.52989399293278</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>637.06770318021199</v>
+      </c>
+      <c r="G35">
+        <f>Confirmed!Y44+Daily!G35</f>
+        <v>659.00634249471454</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>414</v>
       </c>
@@ -7988,22 +8568,26 @@
       </c>
       <c r="C36">
         <f>Confirmed!U45+Daily!C36</f>
-        <v>330.31346661637116</v>
+        <v>43</v>
       </c>
       <c r="D36">
         <f>Confirmed!V45+Daily!D36</f>
-        <v>434.94790037299964</v>
+        <v>391.15834436289254</v>
       </c>
       <c r="E36">
         <f>Confirmed!W45+Daily!E36</f>
-        <v>530.41247484909456</v>
+        <v>531.9042828398965</v>
       </c>
       <c r="F36">
         <f>Confirmed!X45+Daily!F36</f>
-        <v>562.06770318021199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>556.09738515901063</v>
+      </c>
+      <c r="G36">
+        <f>Confirmed!Y45+Daily!G36</f>
+        <v>576.28287526427061</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>415</v>
       </c>
@@ -8017,18 +8601,22 @@
       </c>
       <c r="D37">
         <f>Confirmed!V46+Daily!D37</f>
-        <v>252.15834436289256</v>
+        <v>13</v>
       </c>
       <c r="E37">
         <f>Confirmed!W46+Daily!E37</f>
-        <v>354.9042828398965</v>
+        <v>315.44596148318482</v>
       </c>
       <c r="F37">
         <f>Confirmed!X46+Daily!F37</f>
-        <v>483.09738515901063</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>421.90162544169613</v>
+      </c>
+      <c r="G37">
+        <f>Confirmed!Y46+Daily!G37</f>
+        <v>460.67047216349545</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>416</v>
       </c>
@@ -8046,14 +8634,18 @@
       </c>
       <c r="E38">
         <f>Confirmed!W47+Daily!E38</f>
-        <v>278.44596148318482</v>
+        <v>0</v>
       </c>
       <c r="F38">
         <f>Confirmed!X47+Daily!F38</f>
-        <v>334.90162544169613</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>336.39420494699647</v>
+      </c>
+      <c r="G38">
+        <f>Confirmed!Y47+Daily!G38</f>
+        <v>445.17801268498943</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>417</v>
       </c>
@@ -8075,7 +8667,29 @@
       </c>
       <c r="F39">
         <f>Confirmed!X48+Daily!F39</f>
-        <v>231.39420494699647</v>
+        <v>14</v>
+      </c>
+      <c r="G39">
+        <f>Confirmed!Y48+Daily!G39</f>
+        <v>273.31571529245946</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>418</v>
+      </c>
+      <c r="G40">
+        <f>Confirmed!Y49+Daily!G40</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>419</v>
+      </c>
+      <c r="G41">
+        <f>Confirmed!Y50+Daily!G41</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8259,8 +8873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8329,7 +8943,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E41" si="1">E4+1</f>
+        <f t="shared" ref="E5:E43" si="1">E4+1</f>
         <v>43902</v>
       </c>
     </row>
@@ -8392,6 +9006,9 @@
       <c r="C9">
         <v>9</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
       <c r="E9" s="2">
         <f t="shared" si="1"/>
         <v>43906</v>
@@ -8409,7 +9026,7 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>4.4735729386892178</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="1"/>
@@ -8428,7 +9045,7 @@
         <v>21</v>
       </c>
       <c r="D11">
-        <v>4.4777385159010601</v>
+        <v>4.4735729386892178</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="1"/>
@@ -8447,7 +9064,7 @@
         <v>25</v>
       </c>
       <c r="D12">
-        <v>4.4777385159010601</v>
+        <v>2.9823819591261453</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="1"/>
@@ -8466,7 +9083,7 @@
         <v>46</v>
       </c>
       <c r="D13">
-        <v>2.9851590106007069</v>
+        <v>4.4735729386892178</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="1"/>
@@ -8485,7 +9102,7 @@
         <v>40</v>
       </c>
       <c r="D14">
-        <v>4.4777385159010601</v>
+        <v>5.9647639182522907</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="1"/>
@@ -8504,7 +9121,7 @@
         <v>48</v>
       </c>
       <c r="D15">
-        <v>5.9703180212014137</v>
+        <v>4.4735729386892178</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
@@ -8523,7 +9140,7 @@
         <v>81</v>
       </c>
       <c r="D16">
-        <v>4.4777385159010601</v>
+        <v>16.030303030303031</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="1"/>
@@ -8542,7 +9159,7 @@
         <v>92</v>
       </c>
       <c r="D17">
-        <v>16.0452296819788</v>
+        <v>13.197040169133192</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="1"/>
@@ -8561,7 +9178,7 @@
         <v>120</v>
       </c>
       <c r="D18">
-        <v>13.209328621908128</v>
+        <v>19.012684989429175</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="1"/>
@@ -8580,7 +9197,7 @@
         <v>185</v>
       </c>
       <c r="D19">
-        <v>19.030388692579507</v>
+        <v>36.16138125440451</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="1"/>
@@ -8599,7 +9216,7 @@
         <v>205</v>
       </c>
       <c r="D20">
-        <v>36.195053003533566</v>
+        <v>43.766455250176179</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="1"/>
@@ -8618,7 +9235,7 @@
         <v>256</v>
       </c>
       <c r="D21">
-        <v>43.807208480565372</v>
+        <v>62.779140239605354</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="1"/>
@@ -8637,7 +9254,7 @@
         <v>274</v>
       </c>
       <c r="D22">
-        <v>62.762968197879857</v>
+        <v>72.844679351656097</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="1"/>
@@ -8653,10 +9270,10 @@
         <v>270</v>
       </c>
       <c r="C23">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D23">
-        <v>71.569187279151947</v>
+        <v>96.181818181818187</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="1"/>
@@ -8675,7 +9292,7 @@
         <v>356</v>
       </c>
       <c r="D24">
-        <v>94.778798586572435</v>
+        <v>96.181818181818187</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="1"/>
@@ -8691,10 +9308,10 @@
         <v>319</v>
       </c>
       <c r="C25">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="D25">
-        <v>94.778798586572435</v>
+        <v>122.50133897110641</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="1"/>
@@ -8710,10 +9327,10 @@
         <v>374</v>
       </c>
       <c r="C26">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D26">
-        <v>121.12282685512368</v>
+        <v>195.34601832276252</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="1"/>
@@ -8729,10 +9346,10 @@
         <v>450</v>
       </c>
       <c r="C27">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D27">
-        <v>194.03533568904592</v>
+        <v>195.34601832276252</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="1"/>
@@ -8751,7 +9368,7 @@
         <v>446</v>
       </c>
       <c r="D28">
-        <v>194.03533568904592</v>
+        <v>209.95968992248061</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="1"/>
@@ -8767,10 +9384,10 @@
         <v>549</v>
       </c>
       <c r="C29">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="D29">
-        <v>210.15519434628976</v>
+        <v>209.95968992248061</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="1"/>
@@ -8786,10 +9403,10 @@
         <v>624</v>
       </c>
       <c r="C30">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="D30">
-        <v>211.49851590106007</v>
+        <v>265.28287526427061</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="1"/>
@@ -8805,10 +9422,10 @@
         <v>599</v>
       </c>
       <c r="C31">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D31">
-        <v>268.44042402826852</v>
+        <v>266.77406624383366</v>
       </c>
       <c r="E31" s="2">
         <f t="shared" si="1"/>
@@ -8824,10 +9441,10 @@
         <v>628</v>
       </c>
       <c r="C32">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="D32">
-        <v>266.94784452296818</v>
+        <v>253.65158562367864</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" si="1"/>
@@ -8843,10 +9460,10 @@
         <v>757</v>
       </c>
       <c r="C33">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="D33">
-        <v>255.23109540636042</v>
+        <v>260.95842142353769</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" si="1"/>
@@ -8862,10 +9479,10 @@
         <v>789</v>
       </c>
       <c r="C34">
-        <v>396</v>
+        <v>412</v>
       </c>
       <c r="D34">
-        <v>268.44042402826852</v>
+        <v>250.6692036645525</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="1"/>
@@ -8881,10 +9498,10 @@
         <v>797</v>
       </c>
       <c r="C35">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="D35">
-        <v>256.72367491166079</v>
+        <v>249.17801268498943</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="1"/>
@@ -8900,10 +9517,10 @@
         <v>729</v>
       </c>
       <c r="C36">
-        <v>382</v>
+        <v>402</v>
       </c>
       <c r="D36">
-        <v>255.23109540636042</v>
+        <v>257.97603946441154</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="1"/>
@@ -8919,10 +9536,10 @@
         <v>804</v>
       </c>
       <c r="C37">
-        <v>354</v>
+        <v>385</v>
       </c>
       <c r="D37">
-        <v>265.52989399293284</v>
+        <v>274.0063424947146</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="1"/>
@@ -8938,10 +9555,10 @@
         <v>755</v>
       </c>
       <c r="C38">
-        <v>279</v>
+        <v>311</v>
       </c>
       <c r="D38">
-        <v>283.06770318021199</v>
+        <v>265.28287526427061</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="1"/>
@@ -8957,10 +9574,10 @@
         <v>742</v>
       </c>
       <c r="C39">
-        <v>206</v>
+        <v>261</v>
       </c>
       <c r="D39">
-        <v>277.09738515901063</v>
+        <v>199.67047216349542</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" si="1"/>
@@ -8976,10 +9593,10 @@
         <v>754</v>
       </c>
       <c r="C40">
-        <v>119</v>
+        <v>196</v>
       </c>
       <c r="D40">
-        <v>215.90162544169613</v>
+        <v>249.17801268498943</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" si="1"/>
@@ -8995,10 +9612,10 @@
         <v>757</v>
       </c>
       <c r="C41">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="D41">
-        <v>217.39420494699647</v>
+        <v>179.31571529245949</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" si="1"/>
@@ -9013,6 +9630,16 @@
       <c r="B42">
         <v>777</v>
       </c>
+      <c r="C42">
+        <v>23</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="1"/>
+        <v>43939</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
@@ -9022,6 +9649,13 @@
       <c r="B43">
         <v>683</v>
       </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="1"/>
+        <v>43940</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">

</xml_diff>

<commit_message>
Update; added ability to parse probables files.
</commit_message>
<xml_diff>
--- a/excelsheets/probables.xlsx
+++ b/excelsheets/probables.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>InfluenzaDate</t>
   </si>
@@ -121,6 +121,21 @@
   </si>
   <si>
     <t>Currently, errors are on the order of magnitude of 1%</t>
+  </si>
+  <si>
+    <t>419est</t>
+  </si>
+  <si>
+    <t>419act</t>
+  </si>
+  <si>
+    <t>419estround</t>
+  </si>
+  <si>
+    <t>(OBSOLETED AS OF 4/20)</t>
+  </si>
+  <si>
+    <t>(NOTE: This became obsolete when NYC started releasing its probables as well as confirmed numbers in spreadsheet form on 4/20)</t>
   </si>
 </sst>
 </file>
@@ -613,7 +628,7 @@
                   <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>205</c:v>
+                  <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>256</c:v>
@@ -625,61 +640,64 @@
                   <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>356</c:v>
+                  <c:v>358</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>401</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>433</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>441</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>446</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>504</c:v>
+                  <c:v>506</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>510</c:v>
+                  <c:v>513</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>529</c:v>
+                  <c:v>533</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>459</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>431</c:v>
+                  <c:v>436</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>412</c:v>
+                  <c:v>417</c:v>
                 </c:pt>
                 <c:pt idx="33">
+                  <c:v>401</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>409</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>393</c:v>
                 </c:pt>
-                <c:pt idx="34">
-                  <c:v>402</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>385</c:v>
-                </c:pt>
                 <c:pt idx="36">
-                  <c:v>311</c:v>
+                  <c:v>326</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>261</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>196</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>94</c:v>
+                  <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>23</c:v>
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -969,107 +987,107 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4735729386892178</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.4735729386892178</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.9823819591261453</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.4735729386892178</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9647639182522907</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.4735729386892178</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16.030303030303031</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13.197040169133192</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.012684989429175</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36.16138125440451</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43.766455250176179</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>62.779140239605354</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>72.844679351656097</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>96.181818181818187</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>96.181818181818187</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>122.50133897110641</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>195.34601832276252</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>195.34601832276252</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>209.95968992248061</c:v>
+                  <c:v>211</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>209.95968992248061</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>265.28287526427061</c:v>
+                  <c:v>263</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>266.77406624383366</c:v>
+                  <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>253.65158562367864</c:v>
+                  <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>260.95842142353769</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>250.6692036645525</c:v>
+                  <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>249.17801268498943</c:v>
+                  <c:v>238</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>257.97603946441154</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>274.0063424947146</c:v>
+                  <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>265.28287526427061</c:v>
+                  <c:v>259</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>199.67047216349542</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>249.17801268498943</c:v>
+                  <c:v>243</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>179.31571529245949</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>0</c:v>
@@ -1088,8 +1106,8 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="289900352"/>
-        <c:axId val="296094416"/>
+        <c:axId val="301431600"/>
+        <c:axId val="301426000"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1630,11 +1648,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="289900352"/>
-        <c:axId val="296094416"/>
+        <c:axId val="301431600"/>
+        <c:axId val="301426000"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="289900352"/>
+        <c:axId val="301431600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1676,7 +1694,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296094416"/>
+        <c:crossAx val="301426000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1685,7 +1703,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="296094416"/>
+        <c:axId val="301426000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1735,7 +1753,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289900352"/>
+        <c:crossAx val="301431600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2675,62 +2693,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3565,15 +3591,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -3592,33 +3618,39 @@
       <c r="G1">
         <v>419</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>316</v>
       </c>
@@ -3647,7 +3679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>317</v>
       </c>
@@ -3675,8 +3707,11 @@
         <f>Raw!G10*Raw!G$3/Raw!G$2</f>
         <v>4.4735729386892178</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>318</v>
       </c>
@@ -3704,8 +3739,11 @@
         <f>Raw!G11*Raw!G$3/Raw!G$2</f>
         <v>4.4735729386892178</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>319</v>
       </c>
@@ -3733,8 +3771,11 @@
         <f>Raw!G12*Raw!G$3/Raw!G$2</f>
         <v>2.9823819591261453</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>320</v>
       </c>
@@ -3762,8 +3803,11 @@
         <f>Raw!G13*Raw!G$3/Raw!G$2</f>
         <v>4.4735729386892178</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>321</v>
       </c>
@@ -3791,8 +3835,11 @@
         <f>Raw!G14*Raw!G$3/Raw!G$2</f>
         <v>5.9647639182522907</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>322</v>
       </c>
@@ -3820,8 +3867,11 @@
         <f>Raw!G15*Raw!G$3/Raw!G$2</f>
         <v>4.4735729386892178</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>323</v>
       </c>
@@ -3849,8 +3899,11 @@
         <f>Raw!G16*Raw!G$3/Raw!G$2</f>
         <v>16.030303030303031</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>324</v>
       </c>
@@ -3878,8 +3931,11 @@
         <f>Raw!G17*Raw!G$3/Raw!G$2</f>
         <v>13.197040169133192</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>325</v>
       </c>
@@ -3907,8 +3963,11 @@
         <f>Raw!G18*Raw!G$3/Raw!G$2</f>
         <v>19.012684989429175</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>326</v>
       </c>
@@ -3936,8 +3995,11 @@
         <f>Raw!G19*Raw!G$3/Raw!G$2</f>
         <v>36.16138125440451</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>327</v>
       </c>
@@ -3965,8 +4027,11 @@
         <f>Raw!G20*Raw!G$3/Raw!G$2</f>
         <v>43.766455250176179</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>328</v>
       </c>
@@ -3994,8 +4059,11 @@
         <f>Raw!G21*Raw!G$3/Raw!G$2</f>
         <v>62.779140239605354</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>329</v>
       </c>
@@ -4023,8 +4091,11 @@
         <f>Raw!G22*Raw!G$3/Raw!G$2</f>
         <v>72.844679351656097</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>330</v>
       </c>
@@ -4052,8 +4123,11 @@
         <f>Raw!G23*Raw!G$3/Raw!G$2</f>
         <v>96.181818181818187</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>331</v>
       </c>
@@ -4081,8 +4155,11 @@
         <f>Raw!G24*Raw!G$3/Raw!G$2</f>
         <v>96.181818181818187</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>401</v>
       </c>
@@ -4110,8 +4187,11 @@
         <f>Raw!G25*Raw!G$3/Raw!G$2</f>
         <v>122.50133897110641</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>402</v>
       </c>
@@ -4139,8 +4219,11 @@
         <f>Raw!G26*Raw!G$3/Raw!G$2</f>
         <v>195.34601832276252</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>403</v>
       </c>
@@ -4168,8 +4251,11 @@
         <f>Raw!G27*Raw!G$3/Raw!G$2</f>
         <v>195.34601832276252</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>404</v>
       </c>
@@ -4197,8 +4283,11 @@
         <f>Raw!G28*Raw!G$3/Raw!G$2</f>
         <v>209.95968992248061</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>405</v>
       </c>
@@ -4226,8 +4315,11 @@
         <f>Raw!G29*Raw!G$3/Raw!G$2</f>
         <v>209.95968992248061</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>406</v>
       </c>
@@ -4255,8 +4347,11 @@
         <f>Raw!G30*Raw!G$3/Raw!G$2</f>
         <v>265.28287526427061</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>407</v>
       </c>
@@ -4284,8 +4379,11 @@
         <f>Raw!G31*Raw!G$3/Raw!G$2</f>
         <v>266.77406624383366</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>408</v>
       </c>
@@ -4313,8 +4411,11 @@
         <f>Raw!G32*Raw!G$3/Raw!G$2</f>
         <v>253.65158562367864</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>409</v>
       </c>
@@ -4342,8 +4443,11 @@
         <f>Raw!G33*Raw!G$3/Raw!G$2</f>
         <v>260.95842142353769</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>410</v>
       </c>
@@ -4371,8 +4475,11 @@
         <f>Raw!G34*Raw!G$3/Raw!G$2</f>
         <v>250.6692036645525</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>411</v>
       </c>
@@ -4400,8 +4507,11 @@
         <f>Raw!G35*Raw!G$3/Raw!G$2</f>
         <v>249.17801268498943</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>412</v>
       </c>
@@ -4429,8 +4539,11 @@
         <f>Raw!G36*Raw!G$3/Raw!G$2</f>
         <v>257.97603946441154</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>413</v>
       </c>
@@ -4458,8 +4571,11 @@
         <f>Raw!G37*Raw!G$3/Raw!G$2</f>
         <v>274.0063424947146</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>414</v>
       </c>
@@ -4483,8 +4599,11 @@
         <f>Raw!G38*Raw!G$3/Raw!G$2</f>
         <v>265.28287526427061</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>415</v>
       </c>
@@ -4504,8 +4623,11 @@
         <f>Raw!G39*Raw!G$3/Raw!G$2</f>
         <v>199.67047216349542</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>416</v>
       </c>
@@ -4521,8 +4643,11 @@
         <f>Raw!G40*Raw!G$3/Raw!G$2</f>
         <v>249.17801268498943</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>417</v>
       </c>
@@ -4534,14 +4659,20 @@
         <f>Raw!G41*Raw!G$3/Raw!G$2</f>
         <v>179.31571529245949</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>418</v>
       </c>
       <c r="G40">
         <f>Raw!G42*Raw!G$3/Raw!G$2</f>
         <v>0</v>
+      </c>
+      <c r="H40">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -4551,15 +4682,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y49"/>
+  <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView topLeftCell="J31" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11:Y49"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>325</v>
       </c>
@@ -4632,8 +4763,11 @@
       <c r="Y1">
         <v>419</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z1">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>302</v>
       </c>
@@ -4709,8 +4843,11 @@
       <c r="Y2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>303</v>
       </c>
@@ -4786,8 +4923,11 @@
       <c r="Y3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>304</v>
       </c>
@@ -4863,8 +5003,11 @@
       <c r="Y4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>305</v>
       </c>
@@ -4940,8 +5083,11 @@
       <c r="Y5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>306</v>
       </c>
@@ -5017,8 +5163,11 @@
       <c r="Y6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>307</v>
       </c>
@@ -5094,8 +5243,11 @@
       <c r="Y7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>308</v>
       </c>
@@ -5171,8 +5323,11 @@
       <c r="Y8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>309</v>
       </c>
@@ -5248,8 +5403,11 @@
       <c r="Y9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>310</v>
       </c>
@@ -5325,8 +5483,11 @@
       <c r="Y10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>311</v>
       </c>
@@ -5402,8 +5563,11 @@
       <c r="Y11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>312</v>
       </c>
@@ -5479,8 +5643,11 @@
       <c r="Y12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>313</v>
       </c>
@@ -5556,8 +5723,11 @@
       <c r="Y13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>314</v>
       </c>
@@ -5633,8 +5803,11 @@
       <c r="Y14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>315</v>
       </c>
@@ -5710,8 +5883,11 @@
       <c r="Y15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>316</v>
       </c>
@@ -5787,8 +5963,11 @@
       <c r="Y16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>317</v>
       </c>
@@ -5864,8 +6043,11 @@
       <c r="Y17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>318</v>
       </c>
@@ -5941,8 +6123,11 @@
       <c r="Y18">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>319</v>
       </c>
@@ -6018,8 +6203,11 @@
       <c r="Y19">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>320</v>
       </c>
@@ -6095,8 +6283,11 @@
       <c r="Y20">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z20">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>321</v>
       </c>
@@ -6172,8 +6363,11 @@
       <c r="Y21">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>322</v>
       </c>
@@ -6249,8 +6443,11 @@
       <c r="Y22">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z22">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>323</v>
       </c>
@@ -6326,8 +6523,11 @@
       <c r="Y23">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z23">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>324</v>
       </c>
@@ -6403,8 +6603,11 @@
       <c r="Y24">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>325</v>
       </c>
@@ -6480,8 +6683,11 @@
       <c r="Y25">
         <v>120</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>326</v>
       </c>
@@ -6554,8 +6760,11 @@
       <c r="Y26">
         <v>185</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z26">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>327</v>
       </c>
@@ -6625,8 +6834,11 @@
       <c r="Y27">
         <v>205</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z27">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>328</v>
       </c>
@@ -6693,8 +6905,11 @@
       <c r="Y28">
         <v>256</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z28">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>329</v>
       </c>
@@ -6761,8 +6976,11 @@
       <c r="Y29">
         <v>274</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z29">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>330</v>
       </c>
@@ -6829,8 +7047,11 @@
       <c r="Y30">
         <v>300</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z30">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>331</v>
       </c>
@@ -6894,8 +7115,11 @@
       <c r="Y31">
         <v>356</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z31">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>401</v>
       </c>
@@ -6956,8 +7180,11 @@
       <c r="Y32">
         <v>401</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z32">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>402</v>
       </c>
@@ -7015,8 +7242,11 @@
       <c r="Y33">
         <v>433</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z33">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>403</v>
       </c>
@@ -7071,8 +7301,11 @@
       <c r="Y34">
         <v>441</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z34">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>404</v>
       </c>
@@ -7124,8 +7357,11 @@
       <c r="Y35">
         <v>446</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z35">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>405</v>
       </c>
@@ -7174,8 +7410,11 @@
       <c r="Y36">
         <v>504</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z36">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>406</v>
       </c>
@@ -7221,8 +7460,11 @@
       <c r="Y37">
         <v>510</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z37">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>407</v>
       </c>
@@ -7265,8 +7507,11 @@
       <c r="Y38">
         <v>529</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z38">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>408</v>
       </c>
@@ -7306,8 +7551,11 @@
       <c r="Y39">
         <v>459</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z39">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>409</v>
       </c>
@@ -7344,8 +7592,11 @@
       <c r="Y40">
         <v>431</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z40">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>410</v>
       </c>
@@ -7379,8 +7630,11 @@
       <c r="Y41">
         <v>412</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z41">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>411</v>
       </c>
@@ -7411,8 +7665,11 @@
       <c r="Y42">
         <v>393</v>
       </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z42">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>412</v>
       </c>
@@ -7440,8 +7697,11 @@
       <c r="Y43">
         <v>402</v>
       </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z43">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>413</v>
       </c>
@@ -7466,8 +7726,11 @@
       <c r="Y44">
         <v>385</v>
       </c>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z44">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>414</v>
       </c>
@@ -7486,8 +7749,11 @@
       <c r="Y45">
         <v>311</v>
       </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z45">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>415</v>
       </c>
@@ -7503,8 +7769,11 @@
       <c r="Y46">
         <v>261</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z46">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>416</v>
       </c>
@@ -7517,8 +7786,11 @@
       <c r="Y47">
         <v>196</v>
       </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z47">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>417</v>
       </c>
@@ -7528,13 +7800,24 @@
       <c r="Y48">
         <v>94</v>
       </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z48">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>418</v>
       </c>
       <c r="Y49">
         <v>23</v>
+      </c>
+      <c r="Z49">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z50">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -7544,15 +7827,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G40" sqref="G40:G41"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -7571,8 +7854,11 @@
       <c r="G1">
         <v>419</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>311</v>
       </c>
@@ -7600,8 +7886,12 @@
         <f>Confirmed!Y11+Daily!G2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <f>Confirmed!Z11+Daily!H2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>312</v>
       </c>
@@ -7629,8 +7919,12 @@
         <f>Confirmed!Y12+Daily!G3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <f>Confirmed!Z12+Daily!H3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>313</v>
       </c>
@@ -7658,8 +7952,12 @@
         <f>Confirmed!Y13+Daily!G4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <f>Confirmed!Z13+Daily!H4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314</v>
       </c>
@@ -7687,8 +7985,12 @@
         <f>Confirmed!Y14+Daily!G5</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <f>Confirmed!Z14+Daily!H5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>315</v>
       </c>
@@ -7716,8 +8018,12 @@
         <f>Confirmed!Y15+Daily!G6</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <f>Confirmed!Z15+Daily!H6</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>316</v>
       </c>
@@ -7745,8 +8051,12 @@
         <f>Confirmed!Y16+Daily!G7</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <f>Confirmed!Z16+Daily!H7</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>317</v>
       </c>
@@ -7774,8 +8084,12 @@
         <f>Confirmed!Y17+Daily!G8</f>
         <v>11.473572938689218</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <f>Confirmed!Z17+Daily!H8</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>318</v>
       </c>
@@ -7803,8 +8117,12 @@
         <f>Confirmed!Y18+Daily!G9</f>
         <v>25.473572938689216</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <f>Confirmed!Z18+Daily!H9</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>319</v>
       </c>
@@ -7832,8 +8150,12 @@
         <f>Confirmed!Y19+Daily!G10</f>
         <v>27.982381959126144</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <f>Confirmed!Z19+Daily!H10</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>320</v>
       </c>
@@ -7861,8 +8183,12 @@
         <f>Confirmed!Y20+Daily!G11</f>
         <v>50.473572938689216</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <f>Confirmed!Z20+Daily!H11</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>321</v>
       </c>
@@ -7890,8 +8216,12 @@
         <f>Confirmed!Y21+Daily!G12</f>
         <v>45.964763918252288</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12">
+        <f>Confirmed!Z21+Daily!H12</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>322</v>
       </c>
@@ -7919,8 +8249,12 @@
         <f>Confirmed!Y22+Daily!G13</f>
         <v>52.473572938689216</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <f>Confirmed!Z22+Daily!H13</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>323</v>
       </c>
@@ -7948,8 +8282,12 @@
         <f>Confirmed!Y23+Daily!G14</f>
         <v>97.030303030303031</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <f>Confirmed!Z23+Daily!H14</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>324</v>
       </c>
@@ -7977,8 +8315,12 @@
         <f>Confirmed!Y24+Daily!G15</f>
         <v>105.19704016913319</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15">
+        <f>Confirmed!Z24+Daily!H15</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>325</v>
       </c>
@@ -8006,8 +8348,12 @@
         <f>Confirmed!Y25+Daily!G16</f>
         <v>139.01268498942918</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <f>Confirmed!Z25+Daily!H16</f>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>326</v>
       </c>
@@ -8035,8 +8381,12 @@
         <f>Confirmed!Y26+Daily!G17</f>
         <v>221.16138125440452</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <f>Confirmed!Z26+Daily!H17</f>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>327</v>
       </c>
@@ -8064,8 +8414,12 @@
         <f>Confirmed!Y27+Daily!G18</f>
         <v>248.76645525017619</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <f>Confirmed!Z27+Daily!H18</f>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>328</v>
       </c>
@@ -8093,8 +8447,12 @@
         <f>Confirmed!Y28+Daily!G19</f>
         <v>318.77914023960534</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <f>Confirmed!Z28+Daily!H19</f>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>329</v>
       </c>
@@ -8122,8 +8480,12 @@
         <f>Confirmed!Y29+Daily!G20</f>
         <v>346.84467935165611</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <f>Confirmed!Z29+Daily!H20</f>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>330</v>
       </c>
@@ -8151,8 +8513,12 @@
         <f>Confirmed!Y30+Daily!G21</f>
         <v>396.18181818181819</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <f>Confirmed!Z30+Daily!H21</f>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>331</v>
       </c>
@@ -8180,8 +8546,12 @@
         <f>Confirmed!Y31+Daily!G22</f>
         <v>452.18181818181819</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <f>Confirmed!Z31+Daily!H22</f>
+        <v>454</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>401</v>
       </c>
@@ -8209,8 +8579,12 @@
         <f>Confirmed!Y32+Daily!G23</f>
         <v>523.50133897110641</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <f>Confirmed!Z32+Daily!H23</f>
+        <v>522</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>402</v>
       </c>
@@ -8238,8 +8612,12 @@
         <f>Confirmed!Y33+Daily!G24</f>
         <v>628.34601832276257</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <f>Confirmed!Z33+Daily!H24</f>
+        <v>628</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>403</v>
       </c>
@@ -8267,8 +8645,12 @@
         <f>Confirmed!Y34+Daily!G25</f>
         <v>636.34601832276257</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <f>Confirmed!Z34+Daily!H25</f>
+        <v>633</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>404</v>
       </c>
@@ -8296,8 +8678,12 @@
         <f>Confirmed!Y35+Daily!G26</f>
         <v>655.95968992248061</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <f>Confirmed!Z35+Daily!H26</f>
+        <v>661</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>405</v>
       </c>
@@ -8325,8 +8711,12 @@
         <f>Confirmed!Y36+Daily!G27</f>
         <v>713.95968992248061</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27">
+        <f>Confirmed!Z36+Daily!H27</f>
+        <v>713</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>406</v>
       </c>
@@ -8354,8 +8744,12 @@
         <f>Confirmed!Y37+Daily!G28</f>
         <v>775.28287526427061</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28">
+        <f>Confirmed!Z37+Daily!H28</f>
+        <v>776</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>407</v>
       </c>
@@ -8383,8 +8777,12 @@
         <f>Confirmed!Y38+Daily!G29</f>
         <v>795.77406624383366</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <f>Confirmed!Z38+Daily!H29</f>
+        <v>799</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>408</v>
       </c>
@@ -8412,8 +8810,12 @@
         <f>Confirmed!Y39+Daily!G30</f>
         <v>712.65158562367867</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30">
+        <f>Confirmed!Z39+Daily!H30</f>
+        <v>713</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>409</v>
       </c>
@@ -8441,8 +8843,12 @@
         <f>Confirmed!Y40+Daily!G31</f>
         <v>691.95842142353763</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31">
+        <f>Confirmed!Z40+Daily!H31</f>
+        <v>692</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>410</v>
       </c>
@@ -8470,8 +8876,12 @@
         <f>Confirmed!Y41+Daily!G32</f>
         <v>662.66920366455247</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32">
+        <f>Confirmed!Z41+Daily!H32</f>
+        <v>661</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>411</v>
       </c>
@@ -8499,8 +8909,12 @@
         <f>Confirmed!Y42+Daily!G33</f>
         <v>642.17801268498943</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33">
+        <f>Confirmed!Z42+Daily!H33</f>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>412</v>
       </c>
@@ -8528,8 +8942,12 @@
         <f>Confirmed!Y43+Daily!G34</f>
         <v>659.97603946441154</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34">
+        <f>Confirmed!Z43+Daily!H34</f>
+        <v>665</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>413</v>
       </c>
@@ -8557,8 +8975,12 @@
         <f>Confirmed!Y44+Daily!G35</f>
         <v>659.00634249471454</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35">
+        <f>Confirmed!Z44+Daily!H35</f>
+        <v>660</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>414</v>
       </c>
@@ -8586,8 +9008,12 @@
         <f>Confirmed!Y45+Daily!G36</f>
         <v>576.28287526427061</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36">
+        <f>Confirmed!Z45+Daily!H36</f>
+        <v>585</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>415</v>
       </c>
@@ -8615,8 +9041,12 @@
         <f>Confirmed!Y46+Daily!G37</f>
         <v>460.67047216349545</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37">
+        <f>Confirmed!Z46+Daily!H37</f>
+        <v>477</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>416</v>
       </c>
@@ -8644,8 +9074,12 @@
         <f>Confirmed!Y47+Daily!G38</f>
         <v>445.17801268498943</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38">
+        <f>Confirmed!Z47+Daily!H38</f>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>417</v>
       </c>
@@ -8673,8 +9107,12 @@
         <f>Confirmed!Y48+Daily!G39</f>
         <v>273.31571529245946</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39">
+        <f>Confirmed!Z48+Daily!H39</f>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>418</v>
       </c>
@@ -8682,14 +9120,22 @@
         <f>Confirmed!Y49+Daily!G40</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40">
+        <f>Confirmed!Z49+Daily!H40</f>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>419</v>
       </c>
       <c r="G41">
         <f>Confirmed!Y50+Daily!G41</f>
         <v>0</v>
+      </c>
+      <c r="H41">
+        <f>Confirmed!Z50+Daily!H41</f>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -8699,15 +9145,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -8735,8 +9181,17 @@
       <c r="J1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>415</v>
       </c>
@@ -8767,8 +9222,17 @@
         <f>(I2)/E2</f>
         <v>1.2987486504153002E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <v>311</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>416</v>
       </c>
@@ -8799,8 +9263,17 @@
         <f>(I3)/E3</f>
         <v>9.4222880118921618E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>312</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>417</v>
       </c>
@@ -8831,8 +9304,17 @@
         <f>(I4)/E4</f>
         <v>1.3222156931243911E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>313</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>418</v>
       </c>
@@ -8862,6 +9344,434 @@
       <c r="J5" s="3">
         <f>(I5)/E5</f>
         <v>5.6529146971275096E-3</v>
+      </c>
+      <c r="L5">
+        <v>314</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>315</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>316</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f>ROUND(M7,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>317</v>
+      </c>
+      <c r="M8">
+        <v>4.4735729386892178</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ref="N8:N40" si="0">ROUND(M8,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>318</v>
+      </c>
+      <c r="M9">
+        <v>4.4735729386892178</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>319</v>
+      </c>
+      <c r="M10">
+        <v>2.9823819591261453</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>320</v>
+      </c>
+      <c r="M11">
+        <v>4.4735729386892178</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>321</v>
+      </c>
+      <c r="M12">
+        <v>5.9647639182522907</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>322</v>
+      </c>
+      <c r="M13">
+        <v>4.4735729386892178</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>323</v>
+      </c>
+      <c r="M14">
+        <v>16.030303030303031</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>324</v>
+      </c>
+      <c r="M15">
+        <v>13.197040169133192</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>325</v>
+      </c>
+      <c r="M16">
+        <v>19.012684989429175</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>326</v>
+      </c>
+      <c r="M17">
+        <v>36.16138125440451</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>327</v>
+      </c>
+      <c r="M18">
+        <v>43.766455250176179</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>328</v>
+      </c>
+      <c r="M19">
+        <v>62.779140239605354</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>329</v>
+      </c>
+      <c r="M20">
+        <v>72.844679351656097</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>330</v>
+      </c>
+      <c r="M21">
+        <v>96.181818181818187</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <v>331</v>
+      </c>
+      <c r="M22">
+        <v>96.181818181818187</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <v>401</v>
+      </c>
+      <c r="M23">
+        <v>122.50133897110641</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <v>402</v>
+      </c>
+      <c r="M24">
+        <v>195.34601832276252</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <v>403</v>
+      </c>
+      <c r="M25">
+        <v>195.34601832276252</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <v>404</v>
+      </c>
+      <c r="M26">
+        <v>209.95968992248061</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <v>405</v>
+      </c>
+      <c r="M27">
+        <v>209.95968992248061</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L28">
+        <v>406</v>
+      </c>
+      <c r="M28">
+        <v>265.28287526427061</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L29">
+        <v>407</v>
+      </c>
+      <c r="M29">
+        <v>266.77406624383366</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="30" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <v>408</v>
+      </c>
+      <c r="M30">
+        <v>253.65158562367864</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="31" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L31">
+        <v>409</v>
+      </c>
+      <c r="M31">
+        <v>260.95842142353769</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L32">
+        <v>410</v>
+      </c>
+      <c r="M32">
+        <v>250.6692036645525</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="33" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <v>411</v>
+      </c>
+      <c r="M33">
+        <v>249.17801268498943</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="0"/>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L34">
+        <v>412</v>
+      </c>
+      <c r="M34">
+        <v>257.97603946441154</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="35" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <v>413</v>
+      </c>
+      <c r="M35">
+        <v>274.0063424947146</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="36" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <v>414</v>
+      </c>
+      <c r="M36">
+        <v>265.28287526427061</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="0"/>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="37" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L37">
+        <v>415</v>
+      </c>
+      <c r="M37">
+        <v>199.67047216349542</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L38">
+        <v>416</v>
+      </c>
+      <c r="M38">
+        <v>249.17801268498943</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="0"/>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="39" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L39">
+        <v>417</v>
+      </c>
+      <c r="M39">
+        <v>179.31571529245949</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L40">
+        <v>418</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8873,8 +9783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8974,6 +9884,9 @@
       <c r="C7">
         <v>2</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
       <c r="E7" s="2">
         <f t="shared" si="1"/>
         <v>43904</v>
@@ -9006,9 +9919,6 @@
       <c r="C9">
         <v>9</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
       <c r="E9" s="2">
         <f t="shared" si="1"/>
         <v>43906</v>
@@ -9026,7 +9936,7 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <v>4.4735729386892178</v>
+        <v>4</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="1"/>
@@ -9045,7 +9955,7 @@
         <v>21</v>
       </c>
       <c r="D11">
-        <v>4.4735729386892178</v>
+        <v>4</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="1"/>
@@ -9064,7 +9974,7 @@
         <v>25</v>
       </c>
       <c r="D12">
-        <v>2.9823819591261453</v>
+        <v>2</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="1"/>
@@ -9083,7 +9993,7 @@
         <v>46</v>
       </c>
       <c r="D13">
-        <v>4.4735729386892178</v>
+        <v>5</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="1"/>
@@ -9102,7 +10012,7 @@
         <v>40</v>
       </c>
       <c r="D14">
-        <v>5.9647639182522907</v>
+        <v>5</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="1"/>
@@ -9121,7 +10031,7 @@
         <v>48</v>
       </c>
       <c r="D15">
-        <v>4.4735729386892178</v>
+        <v>4</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
@@ -9140,7 +10050,7 @@
         <v>81</v>
       </c>
       <c r="D16">
-        <v>16.030303030303031</v>
+        <v>16</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="1"/>
@@ -9159,7 +10069,7 @@
         <v>92</v>
       </c>
       <c r="D17">
-        <v>13.197040169133192</v>
+        <v>13</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="1"/>
@@ -9178,7 +10088,7 @@
         <v>120</v>
       </c>
       <c r="D18">
-        <v>19.012684989429175</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="1"/>
@@ -9197,7 +10107,7 @@
         <v>185</v>
       </c>
       <c r="D19">
-        <v>36.16138125440451</v>
+        <v>38</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="1"/>
@@ -9213,10 +10123,10 @@
         <v>129</v>
       </c>
       <c r="C20">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D20">
-        <v>43.766455250176179</v>
+        <v>46</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="1"/>
@@ -9235,7 +10145,7 @@
         <v>256</v>
       </c>
       <c r="D21">
-        <v>62.779140239605354</v>
+        <v>63</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="1"/>
@@ -9254,7 +10164,7 @@
         <v>274</v>
       </c>
       <c r="D22">
-        <v>72.844679351656097</v>
+        <v>73</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="1"/>
@@ -9273,7 +10183,7 @@
         <v>300</v>
       </c>
       <c r="D23">
-        <v>96.181818181818187</v>
+        <v>96</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="1"/>
@@ -9289,10 +10199,10 @@
         <v>289</v>
       </c>
       <c r="C24">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D24">
-        <v>96.181818181818187</v>
+        <v>96</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="1"/>
@@ -9311,7 +10221,7 @@
         <v>401</v>
       </c>
       <c r="D25">
-        <v>122.50133897110641</v>
+        <v>121</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="1"/>
@@ -9327,10 +10237,10 @@
         <v>374</v>
       </c>
       <c r="C26">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D26">
-        <v>195.34601832276252</v>
+        <v>193</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="1"/>
@@ -9349,7 +10259,7 @@
         <v>441</v>
       </c>
       <c r="D27">
-        <v>195.34601832276252</v>
+        <v>192</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="1"/>
@@ -9365,10 +10275,10 @@
         <v>514</v>
       </c>
       <c r="C28">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D28">
-        <v>209.95968992248061</v>
+        <v>211</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="1"/>
@@ -9384,10 +10294,10 @@
         <v>549</v>
       </c>
       <c r="C29">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D29">
-        <v>209.95968992248061</v>
+        <v>207</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="1"/>
@@ -9403,10 +10313,10 @@
         <v>624</v>
       </c>
       <c r="C30">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="D30">
-        <v>265.28287526427061</v>
+        <v>263</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="1"/>
@@ -9422,10 +10332,10 @@
         <v>599</v>
       </c>
       <c r="C31">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="D31">
-        <v>266.77406624383366</v>
+        <v>266</v>
       </c>
       <c r="E31" s="2">
         <f t="shared" si="1"/>
@@ -9444,7 +10354,7 @@
         <v>459</v>
       </c>
       <c r="D32">
-        <v>253.65158562367864</v>
+        <v>254</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" si="1"/>
@@ -9460,10 +10370,10 @@
         <v>757</v>
       </c>
       <c r="C33">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="D33">
-        <v>260.95842142353769</v>
+        <v>256</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" si="1"/>
@@ -9479,10 +10389,10 @@
         <v>789</v>
       </c>
       <c r="C34">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="D34">
-        <v>250.6692036645525</v>
+        <v>244</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="1"/>
@@ -9498,10 +10408,10 @@
         <v>797</v>
       </c>
       <c r="C35">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="D35">
-        <v>249.17801268498943</v>
+        <v>238</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="1"/>
@@ -9517,10 +10427,10 @@
         <v>729</v>
       </c>
       <c r="C36">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="D36">
-        <v>257.97603946441154</v>
+        <v>256</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="1"/>
@@ -9536,10 +10446,10 @@
         <v>804</v>
       </c>
       <c r="C37">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="D37">
-        <v>274.0063424947146</v>
+        <v>267</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="1"/>
@@ -9555,10 +10465,10 @@
         <v>755</v>
       </c>
       <c r="C38">
-        <v>311</v>
+        <v>326</v>
       </c>
       <c r="D38">
-        <v>265.28287526427061</v>
+        <v>259</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="1"/>
@@ -9574,10 +10484,10 @@
         <v>742</v>
       </c>
       <c r="C39">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="D39">
-        <v>199.67047216349542</v>
+        <v>197</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" si="1"/>
@@ -9593,10 +10503,10 @@
         <v>754</v>
       </c>
       <c r="C40">
-        <v>196</v>
+        <v>226</v>
       </c>
       <c r="D40">
-        <v>249.17801268498943</v>
+        <v>243</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" si="1"/>
@@ -9612,10 +10522,10 @@
         <v>757</v>
       </c>
       <c r="C41">
-        <v>94</v>
+        <v>175</v>
       </c>
       <c r="D41">
-        <v>179.31571529245949</v>
+        <v>198</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" si="1"/>
@@ -9631,10 +10541,10 @@
         <v>777</v>
       </c>
       <c r="C42">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>198</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" si="1"/>
@@ -9649,6 +10559,9 @@
       <c r="B43">
         <v>683</v>
       </c>
+      <c r="C43">
+        <v>18</v>
+      </c>
       <c r="D43">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Update, fix to prevent additional line at top of tsvs.
</commit_message>
<xml_diff>
--- a/excelsheets/probables.xlsx
+++ b/excelsheets/probables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16692" windowHeight="6756"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16692" windowHeight="6756" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="5" r:id="rId1"/>
@@ -610,7 +610,7 @@
                   <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>48</c:v>
@@ -631,73 +631,76 @@
                   <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>256</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>274</c:v>
+                  <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>358</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>401</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>435</c:v>
+                  <c:v>438</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>441</c:v>
+                  <c:v>444</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>453</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>517</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>538</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>462</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="27">
-                  <c:v>506</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>513</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>533</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>459</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>436</c:v>
-                </c:pt>
                 <c:pt idx="32">
-                  <c:v>417</c:v>
+                  <c:v>429</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>401</c:v>
+                  <c:v>423</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>409</c:v>
+                  <c:v>423</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>393</c:v>
+                  <c:v>418</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>326</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>280</c:v>
+                  <c:v>298</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>226</c:v>
+                  <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>175</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>99</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>18</c:v>
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -990,6 +993,12 @@
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="8">
                   <c:v>4</c:v>
                 </c:pt>
@@ -1024,10 +1033,10 @@
                   <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>63</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>73</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>96</c:v>
@@ -1036,61 +1045,61 @@
                   <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>121</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>193</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>192</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>211</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>207</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>263</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>254</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>244</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>238</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>267</c:v>
+                  <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>259</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>197</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>243</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>198</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>198</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1106,8 +1115,8 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="301431600"/>
-        <c:axId val="301426000"/>
+        <c:axId val="294038992"/>
+        <c:axId val="294039552"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1648,11 +1657,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="301431600"/>
-        <c:axId val="301426000"/>
+        <c:axId val="294038992"/>
+        <c:axId val="294039552"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="301431600"/>
+        <c:axId val="294038992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1694,7 +1703,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301426000"/>
+        <c:crossAx val="294039552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1703,7 +1712,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="301426000"/>
+        <c:axId val="294039552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1753,7 +1762,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301431600"/>
+        <c:crossAx val="294038992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2396,7 +2405,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2695,7 +2704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -3591,15 +3600,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H40"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -3621,36 +3630,54 @@
       <c r="H1">
         <v>420</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>311</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>312</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>313</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>315</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>316</v>
       </c>
@@ -3678,8 +3705,11 @@
         <f>Raw!G9*Raw!G$3/Raw!G$2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>317</v>
       </c>
@@ -3710,8 +3740,11 @@
       <c r="H8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>318</v>
       </c>
@@ -3742,8 +3775,11 @@
       <c r="H9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>319</v>
       </c>
@@ -3774,8 +3810,11 @@
       <c r="H10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>320</v>
       </c>
@@ -3806,8 +3845,11 @@
       <c r="H11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>321</v>
       </c>
@@ -3838,8 +3880,11 @@
       <c r="H12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>322</v>
       </c>
@@ -3870,8 +3915,11 @@
       <c r="H13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>323</v>
       </c>
@@ -3902,8 +3950,11 @@
       <c r="H14">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>324</v>
       </c>
@@ -3934,8 +3985,11 @@
       <c r="H15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>325</v>
       </c>
@@ -3966,8 +4020,11 @@
       <c r="H16">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>326</v>
       </c>
@@ -3998,8 +4055,11 @@
       <c r="H17">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>327</v>
       </c>
@@ -4030,8 +4090,11 @@
       <c r="H18">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>328</v>
       </c>
@@ -4062,8 +4125,11 @@
       <c r="H19">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>329</v>
       </c>
@@ -4094,8 +4160,11 @@
       <c r="H20">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>330</v>
       </c>
@@ -4126,8 +4195,11 @@
       <c r="H21">
         <v>96</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>331</v>
       </c>
@@ -4158,8 +4230,11 @@
       <c r="H22">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>401</v>
       </c>
@@ -4190,8 +4265,11 @@
       <c r="H23">
         <v>121</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>402</v>
       </c>
@@ -4222,8 +4300,11 @@
       <c r="H24">
         <v>193</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>403</v>
       </c>
@@ -4254,8 +4335,11 @@
       <c r="H25">
         <v>192</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>404</v>
       </c>
@@ -4286,8 +4370,11 @@
       <c r="H26">
         <v>211</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>405</v>
       </c>
@@ -4318,8 +4405,11 @@
       <c r="H27">
         <v>207</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>406</v>
       </c>
@@ -4350,8 +4440,11 @@
       <c r="H28">
         <v>263</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>407</v>
       </c>
@@ -4382,8 +4475,11 @@
       <c r="H29">
         <v>266</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>408</v>
       </c>
@@ -4414,8 +4510,11 @@
       <c r="H30">
         <v>254</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>409</v>
       </c>
@@ -4446,8 +4545,11 @@
       <c r="H31">
         <v>256</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>410</v>
       </c>
@@ -4478,8 +4580,11 @@
       <c r="H32">
         <v>244</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>411</v>
       </c>
@@ -4510,8 +4615,11 @@
       <c r="H33">
         <v>238</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>412</v>
       </c>
@@ -4542,8 +4650,11 @@
       <c r="H34">
         <v>256</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>413</v>
       </c>
@@ -4574,8 +4685,11 @@
       <c r="H35">
         <v>267</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>414</v>
       </c>
@@ -4602,8 +4716,11 @@
       <c r="H36">
         <v>259</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>415</v>
       </c>
@@ -4626,8 +4743,11 @@
       <c r="H37">
         <v>197</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>416</v>
       </c>
@@ -4646,8 +4766,11 @@
       <c r="H38">
         <v>243</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>417</v>
       </c>
@@ -4662,8 +4785,11 @@
       <c r="H39">
         <v>198</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>418</v>
       </c>
@@ -4673,6 +4799,19 @@
       </c>
       <c r="H40">
         <v>198</v>
+      </c>
+      <c r="I40">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I41">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I42">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4682,15 +4821,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z50"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+    <sheetView topLeftCell="L32" workbookViewId="0">
+      <selection activeCell="AA11" sqref="AA11:AA51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>325</v>
       </c>
@@ -4766,8 +4905,11 @@
       <c r="Z1">
         <v>420</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA1">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>302</v>
       </c>
@@ -4846,8 +4988,11 @@
       <c r="Z2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>303</v>
       </c>
@@ -4926,8 +5071,11 @@
       <c r="Z3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>304</v>
       </c>
@@ -5006,8 +5154,11 @@
       <c r="Z4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>305</v>
       </c>
@@ -5086,8 +5237,11 @@
       <c r="Z5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>306</v>
       </c>
@@ -5166,8 +5320,11 @@
       <c r="Z6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>307</v>
       </c>
@@ -5246,8 +5403,11 @@
       <c r="Z7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>308</v>
       </c>
@@ -5326,8 +5486,11 @@
       <c r="Z8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>309</v>
       </c>
@@ -5406,8 +5569,11 @@
       <c r="Z9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>310</v>
       </c>
@@ -5486,8 +5652,11 @@
       <c r="Z10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>311</v>
       </c>
@@ -5566,8 +5735,11 @@
       <c r="Z11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>312</v>
       </c>
@@ -5646,8 +5818,11 @@
       <c r="Z12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>313</v>
       </c>
@@ -5726,8 +5901,11 @@
       <c r="Z13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>314</v>
       </c>
@@ -5806,8 +5984,11 @@
       <c r="Z14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>315</v>
       </c>
@@ -5886,8 +6067,11 @@
       <c r="Z15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>316</v>
       </c>
@@ -5966,8 +6150,11 @@
       <c r="Z16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>317</v>
       </c>
@@ -6046,8 +6233,11 @@
       <c r="Z17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>318</v>
       </c>
@@ -6126,8 +6316,11 @@
       <c r="Z18">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>319</v>
       </c>
@@ -6206,8 +6399,11 @@
       <c r="Z19">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>320</v>
       </c>
@@ -6286,8 +6482,11 @@
       <c r="Z20">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA20">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>321</v>
       </c>
@@ -6366,8 +6565,11 @@
       <c r="Z21">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA21">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>322</v>
       </c>
@@ -6446,8 +6648,11 @@
       <c r="Z22">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA22">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>323</v>
       </c>
@@ -6526,8 +6731,11 @@
       <c r="Z23">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA23">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>324</v>
       </c>
@@ -6606,8 +6814,11 @@
       <c r="Z24">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>325</v>
       </c>
@@ -6686,8 +6897,11 @@
       <c r="Z25">
         <v>120</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>326</v>
       </c>
@@ -6763,8 +6977,11 @@
       <c r="Z26">
         <v>185</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA26">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>327</v>
       </c>
@@ -6837,8 +7054,11 @@
       <c r="Z27">
         <v>206</v>
       </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA27">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>328</v>
       </c>
@@ -6908,8 +7128,11 @@
       <c r="Z28">
         <v>256</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA28">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>329</v>
       </c>
@@ -6979,8 +7202,11 @@
       <c r="Z29">
         <v>274</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA29">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>330</v>
       </c>
@@ -7050,8 +7276,11 @@
       <c r="Z30">
         <v>300</v>
       </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA30">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>331</v>
       </c>
@@ -7118,8 +7347,11 @@
       <c r="Z31">
         <v>358</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA31">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>401</v>
       </c>
@@ -7183,8 +7415,11 @@
       <c r="Z32">
         <v>401</v>
       </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA32">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>402</v>
       </c>
@@ -7245,8 +7480,11 @@
       <c r="Z33">
         <v>435</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA33">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>403</v>
       </c>
@@ -7304,8 +7542,11 @@
       <c r="Z34">
         <v>441</v>
       </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA34">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>404</v>
       </c>
@@ -7360,8 +7601,11 @@
       <c r="Z35">
         <v>450</v>
       </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA35">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>405</v>
       </c>
@@ -7413,8 +7657,11 @@
       <c r="Z36">
         <v>506</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA36">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>406</v>
       </c>
@@ -7463,8 +7710,11 @@
       <c r="Z37">
         <v>513</v>
       </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA37">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>407</v>
       </c>
@@ -7510,8 +7760,11 @@
       <c r="Z38">
         <v>533</v>
       </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA38">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>408</v>
       </c>
@@ -7554,8 +7807,11 @@
       <c r="Z39">
         <v>459</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA39">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>409</v>
       </c>
@@ -7595,8 +7851,11 @@
       <c r="Z40">
         <v>436</v>
       </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA40">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>410</v>
       </c>
@@ -7633,8 +7892,11 @@
       <c r="Z41">
         <v>417</v>
       </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA41">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>411</v>
       </c>
@@ -7668,8 +7930,11 @@
       <c r="Z42">
         <v>401</v>
       </c>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA42">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>412</v>
       </c>
@@ -7700,8 +7965,11 @@
       <c r="Z43">
         <v>409</v>
       </c>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA43">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>413</v>
       </c>
@@ -7729,8 +7997,11 @@
       <c r="Z44">
         <v>393</v>
       </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA44">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>414</v>
       </c>
@@ -7752,8 +8023,11 @@
       <c r="Z45">
         <v>326</v>
       </c>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA45">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>415</v>
       </c>
@@ -7772,8 +8046,11 @@
       <c r="Z46">
         <v>280</v>
       </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA46">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>416</v>
       </c>
@@ -7789,8 +8066,11 @@
       <c r="Z47">
         <v>226</v>
       </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA47">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>417</v>
       </c>
@@ -7803,8 +8083,11 @@
       <c r="Z48">
         <v>175</v>
       </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA48">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>418</v>
       </c>
@@ -7814,10 +8097,21 @@
       <c r="Z49">
         <v>99</v>
       </c>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA49">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="Z50">
         <v>18</v>
+      </c>
+      <c r="AA50">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA51">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -7827,15 +8121,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H41"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -7857,8 +8151,11 @@
       <c r="H1">
         <v>420</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>311</v>
       </c>
@@ -7890,8 +8187,12 @@
         <f>Confirmed!Z11+Daily!H2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <f>Confirmed!AA11+Daily!I2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>312</v>
       </c>
@@ -7923,8 +8224,12 @@
         <f>Confirmed!Z12+Daily!H3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <f>Confirmed!AA12+Daily!I3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>313</v>
       </c>
@@ -7956,8 +8261,12 @@
         <f>Confirmed!Z13+Daily!H4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <f>Confirmed!AA13+Daily!I4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314</v>
       </c>
@@ -7989,8 +8298,12 @@
         <f>Confirmed!Z14+Daily!H5</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <f>Confirmed!AA14+Daily!I5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>315</v>
       </c>
@@ -8022,8 +8335,12 @@
         <f>Confirmed!Z15+Daily!H6</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <f>Confirmed!AA15+Daily!I6</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>316</v>
       </c>
@@ -8055,8 +8372,12 @@
         <f>Confirmed!Z16+Daily!H7</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <f>Confirmed!AA16+Daily!I7</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>317</v>
       </c>
@@ -8088,8 +8409,12 @@
         <f>Confirmed!Z17+Daily!H8</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <f>Confirmed!AA17+Daily!I8</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>318</v>
       </c>
@@ -8121,8 +8446,12 @@
         <f>Confirmed!Z18+Daily!H9</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <f>Confirmed!AA18+Daily!I9</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>319</v>
       </c>
@@ -8154,8 +8483,12 @@
         <f>Confirmed!Z19+Daily!H10</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <f>Confirmed!AA19+Daily!I10</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>320</v>
       </c>
@@ -8187,8 +8520,12 @@
         <f>Confirmed!Z20+Daily!H11</f>
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <f>Confirmed!AA20+Daily!I11</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>321</v>
       </c>
@@ -8220,8 +8557,12 @@
         <f>Confirmed!Z21+Daily!H12</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <f>Confirmed!AA21+Daily!I12</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>322</v>
       </c>
@@ -8253,8 +8594,12 @@
         <f>Confirmed!Z22+Daily!H13</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <f>Confirmed!AA22+Daily!I13</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>323</v>
       </c>
@@ -8286,8 +8631,12 @@
         <f>Confirmed!Z23+Daily!H14</f>
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <f>Confirmed!AA23+Daily!I14</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>324</v>
       </c>
@@ -8319,8 +8668,12 @@
         <f>Confirmed!Z24+Daily!H15</f>
         <v>105</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <f>Confirmed!AA24+Daily!I15</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>325</v>
       </c>
@@ -8352,8 +8705,12 @@
         <f>Confirmed!Z25+Daily!H16</f>
         <v>139</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <f>Confirmed!AA25+Daily!I16</f>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>326</v>
       </c>
@@ -8385,8 +8742,12 @@
         <f>Confirmed!Z26+Daily!H17</f>
         <v>223</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <f>Confirmed!AA26+Daily!I17</f>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>327</v>
       </c>
@@ -8418,8 +8779,12 @@
         <f>Confirmed!Z27+Daily!H18</f>
         <v>252</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <f>Confirmed!AA27+Daily!I18</f>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>328</v>
       </c>
@@ -8451,8 +8816,12 @@
         <f>Confirmed!Z28+Daily!H19</f>
         <v>319</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <f>Confirmed!AA28+Daily!I19</f>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>329</v>
       </c>
@@ -8484,8 +8853,12 @@
         <f>Confirmed!Z29+Daily!H20</f>
         <v>347</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <f>Confirmed!AA29+Daily!I20</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>330</v>
       </c>
@@ -8517,8 +8890,12 @@
         <f>Confirmed!Z30+Daily!H21</f>
         <v>396</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <f>Confirmed!AA30+Daily!I21</f>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>331</v>
       </c>
@@ -8550,8 +8927,12 @@
         <f>Confirmed!Z31+Daily!H22</f>
         <v>454</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <f>Confirmed!AA31+Daily!I22</f>
+        <v>456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>401</v>
       </c>
@@ -8583,8 +8964,12 @@
         <f>Confirmed!Z32+Daily!H23</f>
         <v>522</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23">
+        <f>Confirmed!AA32+Daily!I23</f>
+        <v>526</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>402</v>
       </c>
@@ -8616,8 +9001,12 @@
         <f>Confirmed!Z33+Daily!H24</f>
         <v>628</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24">
+        <f>Confirmed!AA33+Daily!I24</f>
+        <v>628</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>403</v>
       </c>
@@ -8649,8 +9038,12 @@
         <f>Confirmed!Z34+Daily!H25</f>
         <v>633</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25">
+        <f>Confirmed!AA34+Daily!I25</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>404</v>
       </c>
@@ -8682,8 +9075,12 @@
         <f>Confirmed!Z35+Daily!H26</f>
         <v>661</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26">
+        <f>Confirmed!AA35+Daily!I26</f>
+        <v>665</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>405</v>
       </c>
@@ -8715,8 +9112,12 @@
         <f>Confirmed!Z36+Daily!H27</f>
         <v>713</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27">
+        <f>Confirmed!AA36+Daily!I27</f>
+        <v>719</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>406</v>
       </c>
@@ -8748,8 +9149,12 @@
         <f>Confirmed!Z37+Daily!H28</f>
         <v>776</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28">
+        <f>Confirmed!AA37+Daily!I28</f>
+        <v>782</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>407</v>
       </c>
@@ -8781,8 +9186,12 @@
         <f>Confirmed!Z38+Daily!H29</f>
         <v>799</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29">
+        <f>Confirmed!AA38+Daily!I29</f>
+        <v>804</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>408</v>
       </c>
@@ -8814,8 +9223,12 @@
         <f>Confirmed!Z39+Daily!H30</f>
         <v>713</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30">
+        <f>Confirmed!AA39+Daily!I30</f>
+        <v>717</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>409</v>
       </c>
@@ -8847,8 +9260,12 @@
         <f>Confirmed!Z40+Daily!H31</f>
         <v>692</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31">
+        <f>Confirmed!AA40+Daily!I31</f>
+        <v>706</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>410</v>
       </c>
@@ -8880,8 +9297,12 @@
         <f>Confirmed!Z41+Daily!H32</f>
         <v>661</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32">
+        <f>Confirmed!AA41+Daily!I32</f>
+        <v>675</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>411</v>
       </c>
@@ -8913,8 +9334,12 @@
         <f>Confirmed!Z42+Daily!H33</f>
         <v>639</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33">
+        <f>Confirmed!AA42+Daily!I33</f>
+        <v>657</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>412</v>
       </c>
@@ -8946,8 +9371,12 @@
         <f>Confirmed!Z43+Daily!H34</f>
         <v>665</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34">
+        <f>Confirmed!AA43+Daily!I34</f>
+        <v>679</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>413</v>
       </c>
@@ -8979,8 +9408,12 @@
         <f>Confirmed!Z44+Daily!H35</f>
         <v>660</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35">
+        <f>Confirmed!AA44+Daily!I35</f>
+        <v>684</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>414</v>
       </c>
@@ -9012,8 +9445,12 @@
         <f>Confirmed!Z45+Daily!H36</f>
         <v>585</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36">
+        <f>Confirmed!AA45+Daily!I36</f>
+        <v>606</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>415</v>
       </c>
@@ -9045,8 +9482,12 @@
         <f>Confirmed!Z46+Daily!H37</f>
         <v>477</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37">
+        <f>Confirmed!AA46+Daily!I37</f>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>416</v>
       </c>
@@ -9078,8 +9519,12 @@
         <f>Confirmed!Z47+Daily!H38</f>
         <v>469</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38">
+        <f>Confirmed!AA47+Daily!I38</f>
+        <v>494</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>417</v>
       </c>
@@ -9111,8 +9556,12 @@
         <f>Confirmed!Z48+Daily!H39</f>
         <v>373</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39">
+        <f>Confirmed!AA48+Daily!I39</f>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>418</v>
       </c>
@@ -9124,8 +9573,12 @@
         <f>Confirmed!Z49+Daily!H40</f>
         <v>297</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40">
+        <f>Confirmed!AA49+Daily!I40</f>
+        <v>412</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>419</v>
       </c>
@@ -9136,6 +9589,19 @@
       <c r="H41">
         <f>Confirmed!Z50+Daily!H41</f>
         <v>18</v>
+      </c>
+      <c r="I41">
+        <f>Confirmed!AA50+Daily!I41</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>420</v>
+      </c>
+      <c r="I42">
+        <f>Confirmed!AA51+Daily!I42</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -9783,8 +10249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9853,7 +10319,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E43" si="1">E4+1</f>
+        <f t="shared" ref="C4:E45" si="1">E4+1</f>
         <v>43902</v>
       </c>
     </row>
@@ -9903,6 +10369,9 @@
       <c r="C8">
         <v>6</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="E8" s="2">
         <f t="shared" si="1"/>
         <v>43905</v>
@@ -9919,6 +10388,9 @@
       <c r="C9">
         <v>9</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
       <c r="E9" s="2">
         <f t="shared" si="1"/>
         <v>43906</v>
@@ -10009,7 +10481,7 @@
         <v>45</v>
       </c>
       <c r="C14">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -10142,10 +10614,10 @@
         <v>190</v>
       </c>
       <c r="C21">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D21">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="1"/>
@@ -10161,10 +10633,10 @@
         <v>223</v>
       </c>
       <c r="C22">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D22">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="1"/>
@@ -10199,7 +10671,7 @@
         <v>289</v>
       </c>
       <c r="C24">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D24">
         <v>96</v>
@@ -10221,7 +10693,7 @@
         <v>401</v>
       </c>
       <c r="D25">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="1"/>
@@ -10237,10 +10709,10 @@
         <v>374</v>
       </c>
       <c r="C26">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="D26">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="1"/>
@@ -10256,10 +10728,10 @@
         <v>450</v>
       </c>
       <c r="C27">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D27">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="1"/>
@@ -10275,10 +10747,10 @@
         <v>514</v>
       </c>
       <c r="C28">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="D28">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="1"/>
@@ -10294,10 +10766,10 @@
         <v>549</v>
       </c>
       <c r="C29">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="D29">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="1"/>
@@ -10313,10 +10785,10 @@
         <v>624</v>
       </c>
       <c r="C30">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="D30">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="1"/>
@@ -10332,7 +10804,7 @@
         <v>599</v>
       </c>
       <c r="C31">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="D31">
         <v>266</v>
@@ -10351,10 +10823,10 @@
         <v>628</v>
       </c>
       <c r="C32">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="D32">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" si="1"/>
@@ -10370,7 +10842,7 @@
         <v>757</v>
       </c>
       <c r="C33">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="D33">
         <v>256</v>
@@ -10389,10 +10861,10 @@
         <v>789</v>
       </c>
       <c r="C34">
-        <v>417</v>
+        <v>429</v>
       </c>
       <c r="D34">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="1"/>
@@ -10408,10 +10880,10 @@
         <v>797</v>
       </c>
       <c r="C35">
-        <v>401</v>
+        <v>423</v>
       </c>
       <c r="D35">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="1"/>
@@ -10427,7 +10899,7 @@
         <v>729</v>
       </c>
       <c r="C36">
-        <v>409</v>
+        <v>423</v>
       </c>
       <c r="D36">
         <v>256</v>
@@ -10446,10 +10918,10 @@
         <v>804</v>
       </c>
       <c r="C37">
-        <v>393</v>
+        <v>418</v>
       </c>
       <c r="D37">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="1"/>
@@ -10465,10 +10937,10 @@
         <v>755</v>
       </c>
       <c r="C38">
-        <v>326</v>
+        <v>350</v>
       </c>
       <c r="D38">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="1"/>
@@ -10484,10 +10956,10 @@
         <v>742</v>
       </c>
       <c r="C39">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="D39">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" si="1"/>
@@ -10503,7 +10975,7 @@
         <v>754</v>
       </c>
       <c r="C40">
-        <v>226</v>
+        <v>251</v>
       </c>
       <c r="D40">
         <v>243</v>
@@ -10522,10 +10994,10 @@
         <v>757</v>
       </c>
       <c r="C41">
-        <v>175</v>
+        <v>223</v>
       </c>
       <c r="D41">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" si="1"/>
@@ -10541,10 +11013,10 @@
         <v>777</v>
       </c>
       <c r="C42">
-        <v>99</v>
+        <v>178</v>
       </c>
       <c r="D42">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" si="1"/>
@@ -10560,10 +11032,10 @@
         <v>683</v>
       </c>
       <c r="C43">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="E43" s="2">
         <f t="shared" si="1"/>
@@ -10578,6 +11050,13 @@
       <c r="B44">
         <v>623</v>
       </c>
+      <c r="C44">
+        <v>12</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="1"/>
+        <v>43941</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
@@ -10587,6 +11066,10 @@
       <c r="B45">
         <v>568</v>
       </c>
+      <c r="E45" s="2">
+        <f t="shared" si="1"/>
+        <v>43942</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">

</xml_diff>

<commit_message>
Apr 27 update, tweak combiner to handle bad header.
</commit_message>
<xml_diff>
--- a/excelsheets/probables.xlsx
+++ b/excelsheets/probables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16692" windowHeight="6756" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16692" windowHeight="6756" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="5" r:id="rId1"/>
@@ -619,7 +619,7 @@
                   <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>92</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>121</c:v>
@@ -628,85 +628,94 @@
                   <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>206</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>261</c:v>
+                  <c:v>263</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>277</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>303</c:v>
+                  <c:v>305</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>362</c:v>
+                  <c:v>363</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>402</c:v>
+                  <c:v>408</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>441</c:v>
+                  <c:v>445</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>449</c:v>
+                  <c:v>456</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>463</c:v>
+                  <c:v>469</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>517</c:v>
+                  <c:v>526</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>523</c:v>
+                  <c:v>534</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>546</c:v>
+                  <c:v>555</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>474</c:v>
+                  <c:v>499</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>481</c:v>
+                  <c:v>502</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>453</c:v>
+                  <c:v>477</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>448</c:v>
+                  <c:v>476</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>455</c:v>
+                  <c:v>492</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>453</c:v>
+                  <c:v>487</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>389</c:v>
+                  <c:v>445</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>335</c:v>
+                  <c:v>382</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>274</c:v>
+                  <c:v>334</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>268</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>246</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>221</c:v>
+                  <c:v>283</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>185</c:v>
+                  <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>76</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>15</c:v>
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1024,10 +1033,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>19</c:v>
@@ -1042,79 +1051,88 @@
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>74</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>95</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>124</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>194</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>193</c:v>
+                  <c:v>191</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>212</c:v>
+                  <c:v>211</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>209</c:v>
+                  <c:v>203</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>265</c:v>
+                  <c:v>258</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>263</c:v>
+                  <c:v>257</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>247</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>243</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>233</c:v>
+                  <c:v>222</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>226</c:v>
+                  <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>246</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>253</c:v>
+                  <c:v>239</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>241</c:v>
+                  <c:v>199</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>171</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>230</c:v>
+                  <c:v>191</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>180</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>210</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>205</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>236</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>220</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>30</c:v>
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1130,8 +1148,8 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="509386448"/>
-        <c:axId val="509374688"/>
+        <c:axId val="296040992"/>
+        <c:axId val="296041552"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1672,11 +1690,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="509386448"/>
-        <c:axId val="509374688"/>
+        <c:axId val="296040992"/>
+        <c:axId val="296041552"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="509386448"/>
+        <c:axId val="296040992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1718,7 +1736,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="509374688"/>
+        <c:crossAx val="296041552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1727,7 +1745,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="509374688"/>
+        <c:axId val="296041552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1777,7 +1795,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="509386448"/>
+        <c:crossAx val="296040992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2420,7 +2438,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="58" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2431,7 +2449,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667750" cy="6298406"/>
+    <xdr:ext cx="8657897" cy="6279931"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3615,15 +3633,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K44"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection sqref="A1:N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -3654,8 +3672,17 @@
       <c r="K1">
         <v>423</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1">
+        <v>424</v>
+      </c>
+      <c r="M1">
+        <v>425</v>
+      </c>
+      <c r="N1">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>311</v>
       </c>
@@ -3666,7 +3693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>312</v>
       </c>
@@ -3677,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>313</v>
       </c>
@@ -3688,7 +3715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314</v>
       </c>
@@ -3704,8 +3731,17 @@
       <c r="K5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>315</v>
       </c>
@@ -3718,8 +3754,17 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>316</v>
       </c>
@@ -3756,8 +3801,17 @@
       <c r="K7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>317</v>
       </c>
@@ -3797,8 +3851,17 @@
       <c r="K8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>318</v>
       </c>
@@ -3838,8 +3901,17 @@
       <c r="K9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>319</v>
       </c>
@@ -3879,8 +3951,17 @@
       <c r="K10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>320</v>
       </c>
@@ -3920,8 +4001,17 @@
       <c r="K11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>321</v>
       </c>
@@ -3961,8 +4051,17 @@
       <c r="K12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <v>5</v>
+      </c>
+      <c r="N12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>322</v>
       </c>
@@ -4002,8 +4101,17 @@
       <c r="K13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>323</v>
       </c>
@@ -4043,8 +4151,17 @@
       <c r="K14">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>15</v>
+      </c>
+      <c r="M14">
+        <v>15</v>
+      </c>
+      <c r="N14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>324</v>
       </c>
@@ -4084,8 +4201,17 @@
       <c r="K15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>13</v>
+      </c>
+      <c r="M15">
+        <v>13</v>
+      </c>
+      <c r="N15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>325</v>
       </c>
@@ -4125,8 +4251,17 @@
       <c r="K16">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>19</v>
+      </c>
+      <c r="M16">
+        <v>19</v>
+      </c>
+      <c r="N16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>326</v>
       </c>
@@ -4166,8 +4301,17 @@
       <c r="K17">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>40</v>
+      </c>
+      <c r="M17">
+        <v>40</v>
+      </c>
+      <c r="N17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>327</v>
       </c>
@@ -4207,8 +4351,17 @@
       <c r="K18">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>44</v>
+      </c>
+      <c r="M18">
+        <v>45</v>
+      </c>
+      <c r="N18">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>328</v>
       </c>
@@ -4248,8 +4401,17 @@
       <c r="K19">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>64</v>
+      </c>
+      <c r="M19">
+        <v>65</v>
+      </c>
+      <c r="N19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>329</v>
       </c>
@@ -4289,8 +4451,17 @@
       <c r="K20">
         <v>74</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>74</v>
+      </c>
+      <c r="M20">
+        <v>74</v>
+      </c>
+      <c r="N20">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>330</v>
       </c>
@@ -4330,8 +4501,17 @@
       <c r="K21">
         <v>95</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>96</v>
+      </c>
+      <c r="M21">
+        <v>96</v>
+      </c>
+      <c r="N21">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>331</v>
       </c>
@@ -4371,8 +4551,17 @@
       <c r="K22">
         <v>99</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <v>98</v>
+      </c>
+      <c r="M22">
+        <v>99</v>
+      </c>
+      <c r="N22">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>401</v>
       </c>
@@ -4412,8 +4601,17 @@
       <c r="K23">
         <v>124</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <v>121</v>
+      </c>
+      <c r="M23">
+        <v>121</v>
+      </c>
+      <c r="N23">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>402</v>
       </c>
@@ -4453,8 +4651,17 @@
       <c r="K24">
         <v>194</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <v>192</v>
+      </c>
+      <c r="M24">
+        <v>194</v>
+      </c>
+      <c r="N24">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>403</v>
       </c>
@@ -4494,8 +4701,17 @@
       <c r="K25">
         <v>193</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <v>191</v>
+      </c>
+      <c r="M25">
+        <v>190</v>
+      </c>
+      <c r="N25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>404</v>
       </c>
@@ -4535,8 +4751,17 @@
       <c r="K26">
         <v>212</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <v>211</v>
+      </c>
+      <c r="M26">
+        <v>212</v>
+      </c>
+      <c r="N26">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>405</v>
       </c>
@@ -4576,8 +4801,17 @@
       <c r="K27">
         <v>209</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <v>205</v>
+      </c>
+      <c r="M27">
+        <v>204</v>
+      </c>
+      <c r="N27">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>406</v>
       </c>
@@ -4617,8 +4851,17 @@
       <c r="K28">
         <v>265</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28">
+        <v>264</v>
+      </c>
+      <c r="M28">
+        <v>263</v>
+      </c>
+      <c r="N28">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>407</v>
       </c>
@@ -4658,8 +4901,17 @@
       <c r="K29">
         <v>263</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29">
+        <v>258</v>
+      </c>
+      <c r="M29">
+        <v>258</v>
+      </c>
+      <c r="N29">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>408</v>
       </c>
@@ -4699,8 +4951,17 @@
       <c r="K30">
         <v>247</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <v>238</v>
+      </c>
+      <c r="M30">
+        <v>239</v>
+      </c>
+      <c r="N30">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>409</v>
       </c>
@@ -4740,8 +5001,17 @@
       <c r="K31">
         <v>243</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31">
+        <v>231</v>
+      </c>
+      <c r="M31">
+        <v>226</v>
+      </c>
+      <c r="N31">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>410</v>
       </c>
@@ -4781,8 +5051,17 @@
       <c r="K32">
         <v>233</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32">
+        <v>227</v>
+      </c>
+      <c r="M32">
+        <v>223</v>
+      </c>
+      <c r="N32">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>411</v>
       </c>
@@ -4822,8 +5101,17 @@
       <c r="K33">
         <v>226</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <v>214</v>
+      </c>
+      <c r="M33">
+        <v>209</v>
+      </c>
+      <c r="N33">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>412</v>
       </c>
@@ -4863,8 +5151,17 @@
       <c r="K34">
         <v>246</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34">
+        <v>237</v>
+      </c>
+      <c r="M34">
+        <v>230</v>
+      </c>
+      <c r="N34">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>413</v>
       </c>
@@ -4904,8 +5201,17 @@
       <c r="K35">
         <v>253</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <v>245</v>
+      </c>
+      <c r="M35">
+        <v>246</v>
+      </c>
+      <c r="N35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>414</v>
       </c>
@@ -4941,8 +5247,17 @@
       <c r="K36">
         <v>241</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <v>218</v>
+      </c>
+      <c r="M36">
+        <v>209</v>
+      </c>
+      <c r="N36">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>415</v>
       </c>
@@ -4974,8 +5289,17 @@
       <c r="K37">
         <v>171</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37">
+        <v>158</v>
+      </c>
+      <c r="M37">
+        <v>158</v>
+      </c>
+      <c r="N37">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>416</v>
       </c>
@@ -5003,8 +5327,17 @@
       <c r="K38">
         <v>230</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L38">
+        <v>209</v>
+      </c>
+      <c r="M38">
+        <v>207</v>
+      </c>
+      <c r="N38">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>417</v>
       </c>
@@ -5028,8 +5361,17 @@
       <c r="K39">
         <v>180</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39">
+        <v>168</v>
+      </c>
+      <c r="M39">
+        <v>163</v>
+      </c>
+      <c r="N39">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>418</v>
       </c>
@@ -5049,8 +5391,20 @@
       <c r="K40">
         <v>210</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40">
+        <v>196</v>
+      </c>
+      <c r="M40">
+        <v>195</v>
+      </c>
+      <c r="N40">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>419</v>
+      </c>
       <c r="I41">
         <v>240</v>
       </c>
@@ -5060,8 +5414,20 @@
       <c r="K41">
         <v>205</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41">
+        <v>196</v>
+      </c>
+      <c r="M41">
+        <v>195</v>
+      </c>
+      <c r="N41">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>420</v>
+      </c>
       <c r="I42">
         <v>0</v>
       </c>
@@ -5071,18 +5437,84 @@
       <c r="K42">
         <v>236</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L42">
+        <v>210</v>
+      </c>
+      <c r="M42">
+        <v>211</v>
+      </c>
+      <c r="N42">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>421</v>
+      </c>
       <c r="J43">
         <v>21</v>
       </c>
       <c r="K43">
         <v>220</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L43">
+        <v>196</v>
+      </c>
+      <c r="M43">
+        <v>198</v>
+      </c>
+      <c r="N43">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>422</v>
+      </c>
       <c r="K44">
         <v>30</v>
+      </c>
+      <c r="L44">
+        <v>201</v>
+      </c>
+      <c r="M44">
+        <v>228</v>
+      </c>
+      <c r="N44">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>423</v>
+      </c>
+      <c r="L45">
+        <v>28</v>
+      </c>
+      <c r="M45">
+        <v>218</v>
+      </c>
+      <c r="N45">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>424</v>
+      </c>
+      <c r="M46">
+        <v>21</v>
+      </c>
+      <c r="N46">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>425</v>
+      </c>
+      <c r="N47">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -5092,15 +5524,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC56"/>
+  <dimension ref="A1:AF56"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AC11" sqref="AC11:AC53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AF11" sqref="A1:AF56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>325</v>
       </c>
@@ -5185,8 +5617,17 @@
       <c r="AC1">
         <v>423</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD1">
+        <v>424</v>
+      </c>
+      <c r="AE1">
+        <v>425</v>
+      </c>
+      <c r="AF1">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>302</v>
       </c>
@@ -5272,7 +5713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>303</v>
       </c>
@@ -5358,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>304</v>
       </c>
@@ -5444,7 +5885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>305</v>
       </c>
@@ -5530,7 +5971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>306</v>
       </c>
@@ -5616,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>307</v>
       </c>
@@ -5702,7 +6143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>308</v>
       </c>
@@ -5788,7 +6229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>309</v>
       </c>
@@ -5874,7 +6315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>310</v>
       </c>
@@ -5960,7 +6401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>311</v>
       </c>
@@ -6048,8 +6489,17 @@
       <c r="AC11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AE11">
+        <v>1</v>
+      </c>
+      <c r="AF11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>312</v>
       </c>
@@ -6137,8 +6587,17 @@
       <c r="AC12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD12">
+        <v>1</v>
+      </c>
+      <c r="AE12">
+        <v>1</v>
+      </c>
+      <c r="AF12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>313</v>
       </c>
@@ -6226,8 +6685,17 @@
       <c r="AC13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>314</v>
       </c>
@@ -6315,8 +6783,17 @@
       <c r="AC14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD14">
+        <v>2</v>
+      </c>
+      <c r="AE14">
+        <v>2</v>
+      </c>
+      <c r="AF14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>315</v>
       </c>
@@ -6404,8 +6881,17 @@
       <c r="AC15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD15">
+        <v>6</v>
+      </c>
+      <c r="AE15">
+        <v>6</v>
+      </c>
+      <c r="AF15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>316</v>
       </c>
@@ -6493,8 +6979,17 @@
       <c r="AC16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD16">
+        <v>9</v>
+      </c>
+      <c r="AE16">
+        <v>9</v>
+      </c>
+      <c r="AF16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>317</v>
       </c>
@@ -6582,8 +7077,17 @@
       <c r="AC17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD17">
+        <v>7</v>
+      </c>
+      <c r="AE17">
+        <v>7</v>
+      </c>
+      <c r="AF17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>318</v>
       </c>
@@ -6671,8 +7175,17 @@
       <c r="AC18">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD18">
+        <v>21</v>
+      </c>
+      <c r="AE18">
+        <v>21</v>
+      </c>
+      <c r="AF18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>319</v>
       </c>
@@ -6760,8 +7273,17 @@
       <c r="AC19">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD19">
+        <v>25</v>
+      </c>
+      <c r="AE19">
+        <v>25</v>
+      </c>
+      <c r="AF19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>320</v>
       </c>
@@ -6849,8 +7371,17 @@
       <c r="AC20">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD20">
+        <v>46</v>
+      </c>
+      <c r="AE20">
+        <v>46</v>
+      </c>
+      <c r="AF20">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>321</v>
       </c>
@@ -6938,8 +7469,17 @@
       <c r="AC21">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD21">
+        <v>41</v>
+      </c>
+      <c r="AE21">
+        <v>41</v>
+      </c>
+      <c r="AF21">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>322</v>
       </c>
@@ -7027,8 +7567,17 @@
       <c r="AC22">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD22">
+        <v>48</v>
+      </c>
+      <c r="AE22">
+        <v>48</v>
+      </c>
+      <c r="AF22">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>323</v>
       </c>
@@ -7116,8 +7665,17 @@
       <c r="AC23">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD23">
+        <v>81</v>
+      </c>
+      <c r="AE23">
+        <v>81</v>
+      </c>
+      <c r="AF23">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>324</v>
       </c>
@@ -7205,8 +7763,17 @@
       <c r="AC24">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD24">
+        <v>92</v>
+      </c>
+      <c r="AE24">
+        <v>92</v>
+      </c>
+      <c r="AF24">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>325</v>
       </c>
@@ -7294,8 +7861,17 @@
       <c r="AC25">
         <v>121</v>
       </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD25">
+        <v>121</v>
+      </c>
+      <c r="AE25">
+        <v>121</v>
+      </c>
+      <c r="AF25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>326</v>
       </c>
@@ -7380,8 +7956,17 @@
       <c r="AC26">
         <v>185</v>
       </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD26">
+        <v>185</v>
+      </c>
+      <c r="AE26">
+        <v>185</v>
+      </c>
+      <c r="AF26">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>327</v>
       </c>
@@ -7463,8 +8048,17 @@
       <c r="AC27">
         <v>206</v>
       </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD27">
+        <v>207</v>
+      </c>
+      <c r="AE27">
+        <v>207</v>
+      </c>
+      <c r="AF27">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>328</v>
       </c>
@@ -7543,8 +8137,17 @@
       <c r="AC28">
         <v>261</v>
       </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD28">
+        <v>262</v>
+      </c>
+      <c r="AE28">
+        <v>262</v>
+      </c>
+      <c r="AF28">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>329</v>
       </c>
@@ -7623,8 +8226,17 @@
       <c r="AC29">
         <v>277</v>
       </c>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD29">
+        <v>278</v>
+      </c>
+      <c r="AE29">
+        <v>278</v>
+      </c>
+      <c r="AF29">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>330</v>
       </c>
@@ -7703,8 +8315,17 @@
       <c r="AC30">
         <v>303</v>
       </c>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD30">
+        <v>303</v>
+      </c>
+      <c r="AE30">
+        <v>303</v>
+      </c>
+      <c r="AF30">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>331</v>
       </c>
@@ -7780,8 +8401,17 @@
       <c r="AC31">
         <v>362</v>
       </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD31">
+        <v>362</v>
+      </c>
+      <c r="AE31">
+        <v>362</v>
+      </c>
+      <c r="AF31">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>401</v>
       </c>
@@ -7854,8 +8484,17 @@
       <c r="AC32">
         <v>402</v>
       </c>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD32">
+        <v>405</v>
+      </c>
+      <c r="AE32">
+        <v>405</v>
+      </c>
+      <c r="AF32">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>402</v>
       </c>
@@ -7925,8 +8564,17 @@
       <c r="AC33">
         <v>441</v>
       </c>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD33">
+        <v>444</v>
+      </c>
+      <c r="AE33">
+        <v>445</v>
+      </c>
+      <c r="AF33">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>403</v>
       </c>
@@ -7993,8 +8641,17 @@
       <c r="AC34">
         <v>449</v>
       </c>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD34">
+        <v>453</v>
+      </c>
+      <c r="AE34">
+        <v>455</v>
+      </c>
+      <c r="AF34">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>404</v>
       </c>
@@ -8058,8 +8715,17 @@
       <c r="AC35">
         <v>463</v>
       </c>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD35">
+        <v>464</v>
+      </c>
+      <c r="AE35">
+        <v>466</v>
+      </c>
+      <c r="AF35">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>405</v>
       </c>
@@ -8120,8 +8786,17 @@
       <c r="AC36">
         <v>517</v>
       </c>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD36">
+        <v>521</v>
+      </c>
+      <c r="AE36">
+        <v>523</v>
+      </c>
+      <c r="AF36">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>406</v>
       </c>
@@ -8179,8 +8854,17 @@
       <c r="AC37">
         <v>523</v>
       </c>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD37">
+        <v>527</v>
+      </c>
+      <c r="AE37">
+        <v>529</v>
+      </c>
+      <c r="AF37">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>407</v>
       </c>
@@ -8235,8 +8919,17 @@
       <c r="AC38">
         <v>546</v>
       </c>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD38">
+        <v>550</v>
+      </c>
+      <c r="AE38">
+        <v>552</v>
+      </c>
+      <c r="AF38">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>408</v>
       </c>
@@ -8288,8 +8981,17 @@
       <c r="AC39">
         <v>474</v>
       </c>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD39">
+        <v>491</v>
+      </c>
+      <c r="AE39">
+        <v>492</v>
+      </c>
+      <c r="AF39">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>409</v>
       </c>
@@ -8338,8 +9040,17 @@
       <c r="AC40">
         <v>481</v>
       </c>
-    </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD40">
+        <v>493</v>
+      </c>
+      <c r="AE40">
+        <v>498</v>
+      </c>
+      <c r="AF40">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>410</v>
       </c>
@@ -8385,8 +9096,17 @@
       <c r="AC41">
         <v>453</v>
       </c>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD41">
+        <v>468</v>
+      </c>
+      <c r="AE41">
+        <v>474</v>
+      </c>
+      <c r="AF41">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>411</v>
       </c>
@@ -8429,8 +9149,17 @@
       <c r="AC42">
         <v>448</v>
       </c>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD42">
+        <v>463</v>
+      </c>
+      <c r="AE42">
+        <v>471</v>
+      </c>
+      <c r="AF42">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>412</v>
       </c>
@@ -8470,8 +9199,17 @@
       <c r="AC43">
         <v>455</v>
       </c>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD43">
+        <v>480</v>
+      </c>
+      <c r="AE43">
+        <v>487</v>
+      </c>
+      <c r="AF43">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>413</v>
       </c>
@@ -8508,8 +9246,17 @@
       <c r="AC44">
         <v>453</v>
       </c>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD44">
+        <v>473</v>
+      </c>
+      <c r="AE44">
+        <v>480</v>
+      </c>
+      <c r="AF44">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>414</v>
       </c>
@@ -8540,8 +9287,17 @@
       <c r="AC45">
         <v>389</v>
       </c>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD45">
+        <v>417</v>
+      </c>
+      <c r="AE45">
+        <v>434</v>
+      </c>
+      <c r="AF45">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>415</v>
       </c>
@@ -8569,8 +9325,17 @@
       <c r="AC46">
         <v>335</v>
       </c>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD46">
+        <v>358</v>
+      </c>
+      <c r="AE46">
+        <v>369</v>
+      </c>
+      <c r="AF46">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>416</v>
       </c>
@@ -8595,8 +9360,17 @@
       <c r="AC47">
         <v>274</v>
       </c>
-    </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD47">
+        <v>311</v>
+      </c>
+      <c r="AE47">
+        <v>316</v>
+      </c>
+      <c r="AF47">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>417</v>
       </c>
@@ -8618,8 +9392,17 @@
       <c r="AC48">
         <v>268</v>
       </c>
-    </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD48">
+        <v>283</v>
+      </c>
+      <c r="AE48">
+        <v>289</v>
+      </c>
+      <c r="AF48">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="49" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>418</v>
       </c>
@@ -8638,8 +9421,17 @@
       <c r="AC49">
         <v>246</v>
       </c>
-    </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD49">
+        <v>263</v>
+      </c>
+      <c r="AE49">
+        <v>270</v>
+      </c>
+      <c r="AF49">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>419</v>
       </c>
@@ -8655,8 +9447,17 @@
       <c r="AC50">
         <v>221</v>
       </c>
-    </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD50">
+        <v>243</v>
+      </c>
+      <c r="AE50">
+        <v>249</v>
+      </c>
+      <c r="AF50">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="51" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>420</v>
       </c>
@@ -8669,8 +9470,17 @@
       <c r="AC51">
         <v>185</v>
       </c>
-    </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD51">
+        <v>216</v>
+      </c>
+      <c r="AE51">
+        <v>223</v>
+      </c>
+      <c r="AF51">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="52" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>421</v>
       </c>
@@ -8680,28 +9490,64 @@
       <c r="AC52">
         <v>76</v>
       </c>
-    </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD52">
+        <v>158</v>
+      </c>
+      <c r="AE52">
+        <v>162</v>
+      </c>
+      <c r="AF52">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>422</v>
       </c>
       <c r="AC53">
         <v>15</v>
       </c>
-    </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD53">
+        <v>78</v>
+      </c>
+      <c r="AE53">
+        <v>107</v>
+      </c>
+      <c r="AF53">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="54" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>423</v>
       </c>
-    </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD54">
+        <v>12</v>
+      </c>
+      <c r="AE54">
+        <v>76</v>
+      </c>
+      <c r="AF54">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="55" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>424</v>
       </c>
-    </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AE55">
+        <v>11</v>
+      </c>
+      <c r="AF55">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>425</v>
+      </c>
+      <c r="AF56">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -8711,15 +9557,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D29" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K44"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -8751,8 +9597,17 @@
       <c r="K1">
         <v>423</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1">
+        <v>424</v>
+      </c>
+      <c r="M1">
+        <v>425</v>
+      </c>
+      <c r="N1">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>311</v>
       </c>
@@ -8796,8 +9651,20 @@
         <f>Confirmed!AC11+Daily!K2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <f>Confirmed!AD11+Daily!L2</f>
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <f>Confirmed!AE11+Daily!M2</f>
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <f>Confirmed!AF11+Daily!N2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>312</v>
       </c>
@@ -8841,8 +9708,20 @@
         <f>Confirmed!AC12+Daily!K3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <f>Confirmed!AD12+Daily!L3</f>
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <f>Confirmed!AE12+Daily!M3</f>
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <f>Confirmed!AF12+Daily!N3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>313</v>
       </c>
@@ -8886,8 +9765,20 @@
         <f>Confirmed!AC13+Daily!K4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <f>Confirmed!AD13+Daily!L4</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>Confirmed!AE13+Daily!M4</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f>Confirmed!AF13+Daily!N4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314</v>
       </c>
@@ -8931,8 +9822,20 @@
         <f>Confirmed!AC14+Daily!K5</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <f>Confirmed!AD14+Daily!L5</f>
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <f>Confirmed!AE14+Daily!M5</f>
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <f>Confirmed!AF14+Daily!N5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>315</v>
       </c>
@@ -8976,8 +9879,20 @@
         <f>Confirmed!AC15+Daily!K6</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <f>Confirmed!AD15+Daily!L6</f>
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <f>Confirmed!AE15+Daily!M6</f>
+        <v>6</v>
+      </c>
+      <c r="N6">
+        <f>Confirmed!AF15+Daily!N6</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>316</v>
       </c>
@@ -9021,8 +9936,20 @@
         <f>Confirmed!AC16+Daily!K7</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <f>Confirmed!AD16+Daily!L7</f>
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <f>Confirmed!AE16+Daily!M7</f>
+        <v>10</v>
+      </c>
+      <c r="N7">
+        <f>Confirmed!AF16+Daily!N7</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>317</v>
       </c>
@@ -9066,8 +9993,20 @@
         <f>Confirmed!AC17+Daily!K8</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <f>Confirmed!AD17+Daily!L8</f>
+        <v>11</v>
+      </c>
+      <c r="M8">
+        <f>Confirmed!AE17+Daily!M8</f>
+        <v>11</v>
+      </c>
+      <c r="N8">
+        <f>Confirmed!AF17+Daily!N8</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>318</v>
       </c>
@@ -9111,8 +10050,20 @@
         <f>Confirmed!AC18+Daily!K9</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <f>Confirmed!AD18+Daily!L9</f>
+        <v>25</v>
+      </c>
+      <c r="M9">
+        <f>Confirmed!AE18+Daily!M9</f>
+        <v>25</v>
+      </c>
+      <c r="N9">
+        <f>Confirmed!AF18+Daily!N9</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>319</v>
       </c>
@@ -9156,8 +10107,20 @@
         <f>Confirmed!AC19+Daily!K10</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <f>Confirmed!AD19+Daily!L10</f>
+        <v>27</v>
+      </c>
+      <c r="M10">
+        <f>Confirmed!AE19+Daily!M10</f>
+        <v>27</v>
+      </c>
+      <c r="N10">
+        <f>Confirmed!AF19+Daily!N10</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>320</v>
       </c>
@@ -9201,8 +10164,20 @@
         <f>Confirmed!AC20+Daily!K11</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <f>Confirmed!AD20+Daily!L11</f>
+        <v>50</v>
+      </c>
+      <c r="M11">
+        <f>Confirmed!AE20+Daily!M11</f>
+        <v>50</v>
+      </c>
+      <c r="N11">
+        <f>Confirmed!AF20+Daily!N11</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>321</v>
       </c>
@@ -9246,8 +10221,20 @@
         <f>Confirmed!AC21+Daily!K12</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <f>Confirmed!AD21+Daily!L12</f>
+        <v>46</v>
+      </c>
+      <c r="M12">
+        <f>Confirmed!AE21+Daily!M12</f>
+        <v>46</v>
+      </c>
+      <c r="N12">
+        <f>Confirmed!AF21+Daily!N12</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>322</v>
       </c>
@@ -9291,8 +10278,20 @@
         <f>Confirmed!AC22+Daily!K13</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <f>Confirmed!AD22+Daily!L13</f>
+        <v>52</v>
+      </c>
+      <c r="M13">
+        <f>Confirmed!AE22+Daily!M13</f>
+        <v>52</v>
+      </c>
+      <c r="N13">
+        <f>Confirmed!AF22+Daily!N13</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>323</v>
       </c>
@@ -9336,8 +10335,20 @@
         <f>Confirmed!AC23+Daily!K14</f>
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <f>Confirmed!AD23+Daily!L14</f>
+        <v>96</v>
+      </c>
+      <c r="M14">
+        <f>Confirmed!AE23+Daily!M14</f>
+        <v>96</v>
+      </c>
+      <c r="N14">
+        <f>Confirmed!AF23+Daily!N14</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>324</v>
       </c>
@@ -9381,8 +10392,20 @@
         <f>Confirmed!AC24+Daily!K15</f>
         <v>105</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <f>Confirmed!AD24+Daily!L15</f>
+        <v>105</v>
+      </c>
+      <c r="M15">
+        <f>Confirmed!AE24+Daily!M15</f>
+        <v>105</v>
+      </c>
+      <c r="N15">
+        <f>Confirmed!AF24+Daily!N15</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>325</v>
       </c>
@@ -9426,8 +10449,20 @@
         <f>Confirmed!AC25+Daily!K16</f>
         <v>140</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <f>Confirmed!AD25+Daily!L16</f>
+        <v>140</v>
+      </c>
+      <c r="M16">
+        <f>Confirmed!AE25+Daily!M16</f>
+        <v>140</v>
+      </c>
+      <c r="N16">
+        <f>Confirmed!AF25+Daily!N16</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>326</v>
       </c>
@@ -9471,8 +10506,20 @@
         <f>Confirmed!AC26+Daily!K17</f>
         <v>225</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <f>Confirmed!AD26+Daily!L17</f>
+        <v>225</v>
+      </c>
+      <c r="M17">
+        <f>Confirmed!AE26+Daily!M17</f>
+        <v>225</v>
+      </c>
+      <c r="N17">
+        <f>Confirmed!AF26+Daily!N17</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>327</v>
       </c>
@@ -9516,8 +10563,20 @@
         <f>Confirmed!AC27+Daily!K18</f>
         <v>251</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <f>Confirmed!AD27+Daily!L18</f>
+        <v>251</v>
+      </c>
+      <c r="M18">
+        <f>Confirmed!AE27+Daily!M18</f>
+        <v>252</v>
+      </c>
+      <c r="N18">
+        <f>Confirmed!AF27+Daily!N18</f>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>328</v>
       </c>
@@ -9561,8 +10620,20 @@
         <f>Confirmed!AC28+Daily!K19</f>
         <v>325</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <f>Confirmed!AD28+Daily!L19</f>
+        <v>326</v>
+      </c>
+      <c r="M19">
+        <f>Confirmed!AE28+Daily!M19</f>
+        <v>327</v>
+      </c>
+      <c r="N19">
+        <f>Confirmed!AF28+Daily!N19</f>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>329</v>
       </c>
@@ -9606,8 +10677,20 @@
         <f>Confirmed!AC29+Daily!K20</f>
         <v>351</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <f>Confirmed!AD29+Daily!L20</f>
+        <v>352</v>
+      </c>
+      <c r="M20">
+        <f>Confirmed!AE29+Daily!M20</f>
+        <v>352</v>
+      </c>
+      <c r="N20">
+        <f>Confirmed!AF29+Daily!N20</f>
+        <v>353</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>330</v>
       </c>
@@ -9651,8 +10734,20 @@
         <f>Confirmed!AC30+Daily!K21</f>
         <v>398</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <f>Confirmed!AD30+Daily!L21</f>
+        <v>399</v>
+      </c>
+      <c r="M21">
+        <f>Confirmed!AE30+Daily!M21</f>
+        <v>399</v>
+      </c>
+      <c r="N21">
+        <f>Confirmed!AF30+Daily!N21</f>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>331</v>
       </c>
@@ -9696,8 +10791,20 @@
         <f>Confirmed!AC31+Daily!K22</f>
         <v>461</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <f>Confirmed!AD31+Daily!L22</f>
+        <v>460</v>
+      </c>
+      <c r="M22">
+        <f>Confirmed!AE31+Daily!M22</f>
+        <v>461</v>
+      </c>
+      <c r="N22">
+        <f>Confirmed!AF31+Daily!N22</f>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>401</v>
       </c>
@@ -9741,8 +10848,20 @@
         <f>Confirmed!AC32+Daily!K23</f>
         <v>526</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <f>Confirmed!AD32+Daily!L23</f>
+        <v>526</v>
+      </c>
+      <c r="M23">
+        <f>Confirmed!AE32+Daily!M23</f>
+        <v>526</v>
+      </c>
+      <c r="N23">
+        <f>Confirmed!AF32+Daily!N23</f>
+        <v>527</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>402</v>
       </c>
@@ -9786,8 +10905,20 @@
         <f>Confirmed!AC33+Daily!K24</f>
         <v>635</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <f>Confirmed!AD33+Daily!L24</f>
+        <v>636</v>
+      </c>
+      <c r="M24">
+        <f>Confirmed!AE33+Daily!M24</f>
+        <v>639</v>
+      </c>
+      <c r="N24">
+        <f>Confirmed!AF33+Daily!N24</f>
+        <v>641</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>403</v>
       </c>
@@ -9831,8 +10962,20 @@
         <f>Confirmed!AC34+Daily!K25</f>
         <v>642</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <f>Confirmed!AD34+Daily!L25</f>
+        <v>644</v>
+      </c>
+      <c r="M25">
+        <f>Confirmed!AE34+Daily!M25</f>
+        <v>645</v>
+      </c>
+      <c r="N25">
+        <f>Confirmed!AF34+Daily!N25</f>
+        <v>647</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>404</v>
       </c>
@@ -9876,8 +11019,20 @@
         <f>Confirmed!AC35+Daily!K26</f>
         <v>675</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <f>Confirmed!AD35+Daily!L26</f>
+        <v>675</v>
+      </c>
+      <c r="M26">
+        <f>Confirmed!AE35+Daily!M26</f>
+        <v>678</v>
+      </c>
+      <c r="N26">
+        <f>Confirmed!AF35+Daily!N26</f>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>405</v>
       </c>
@@ -9921,8 +11076,20 @@
         <f>Confirmed!AC36+Daily!K27</f>
         <v>726</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <f>Confirmed!AD36+Daily!L27</f>
+        <v>726</v>
+      </c>
+      <c r="M27">
+        <f>Confirmed!AE36+Daily!M27</f>
+        <v>727</v>
+      </c>
+      <c r="N27">
+        <f>Confirmed!AF36+Daily!N27</f>
+        <v>729</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>406</v>
       </c>
@@ -9966,8 +11133,20 @@
         <f>Confirmed!AC37+Daily!K28</f>
         <v>788</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28">
+        <f>Confirmed!AD37+Daily!L28</f>
+        <v>791</v>
+      </c>
+      <c r="M28">
+        <f>Confirmed!AE37+Daily!M28</f>
+        <v>792</v>
+      </c>
+      <c r="N28">
+        <f>Confirmed!AF37+Daily!N28</f>
+        <v>792</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>407</v>
       </c>
@@ -10011,8 +11190,20 @@
         <f>Confirmed!AC38+Daily!K29</f>
         <v>809</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29">
+        <f>Confirmed!AD38+Daily!L29</f>
+        <v>808</v>
+      </c>
+      <c r="M29">
+        <f>Confirmed!AE38+Daily!M29</f>
+        <v>810</v>
+      </c>
+      <c r="N29">
+        <f>Confirmed!AF38+Daily!N29</f>
+        <v>812</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>408</v>
       </c>
@@ -10056,8 +11247,20 @@
         <f>Confirmed!AC39+Daily!K30</f>
         <v>721</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <f>Confirmed!AD39+Daily!L30</f>
+        <v>729</v>
+      </c>
+      <c r="M30">
+        <f>Confirmed!AE39+Daily!M30</f>
+        <v>731</v>
+      </c>
+      <c r="N30">
+        <f>Confirmed!AF39+Daily!N30</f>
+        <v>732</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>409</v>
       </c>
@@ -10101,8 +11304,20 @@
         <f>Confirmed!AC40+Daily!K31</f>
         <v>724</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31">
+        <f>Confirmed!AD40+Daily!L31</f>
+        <v>724</v>
+      </c>
+      <c r="M31">
+        <f>Confirmed!AE40+Daily!M31</f>
+        <v>724</v>
+      </c>
+      <c r="N31">
+        <f>Confirmed!AF40+Daily!N31</f>
+        <v>729</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>410</v>
       </c>
@@ -10146,8 +11361,20 @@
         <f>Confirmed!AC41+Daily!K32</f>
         <v>686</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32">
+        <f>Confirmed!AD41+Daily!L32</f>
+        <v>695</v>
+      </c>
+      <c r="M32">
+        <f>Confirmed!AE41+Daily!M32</f>
+        <v>697</v>
+      </c>
+      <c r="N32">
+        <f>Confirmed!AF41+Daily!N32</f>
+        <v>699</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>411</v>
       </c>
@@ -10191,8 +11418,20 @@
         <f>Confirmed!AC42+Daily!K33</f>
         <v>674</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <f>Confirmed!AD42+Daily!L33</f>
+        <v>677</v>
+      </c>
+      <c r="M33">
+        <f>Confirmed!AE42+Daily!M33</f>
+        <v>680</v>
+      </c>
+      <c r="N33">
+        <f>Confirmed!AF42+Daily!N33</f>
+        <v>682</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>412</v>
       </c>
@@ -10236,8 +11475,20 @@
         <f>Confirmed!AC43+Daily!K34</f>
         <v>701</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34">
+        <f>Confirmed!AD43+Daily!L34</f>
+        <v>717</v>
+      </c>
+      <c r="M34">
+        <f>Confirmed!AE43+Daily!M34</f>
+        <v>717</v>
+      </c>
+      <c r="N34">
+        <f>Confirmed!AF43+Daily!N34</f>
+        <v>717</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>413</v>
       </c>
@@ -10281,8 +11532,20 @@
         <f>Confirmed!AC44+Daily!K35</f>
         <v>706</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <f>Confirmed!AD44+Daily!L35</f>
+        <v>718</v>
+      </c>
+      <c r="M35">
+        <f>Confirmed!AE44+Daily!M35</f>
+        <v>726</v>
+      </c>
+      <c r="N35">
+        <f>Confirmed!AF44+Daily!N35</f>
+        <v>726</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>414</v>
       </c>
@@ -10326,8 +11589,20 @@
         <f>Confirmed!AC45+Daily!K36</f>
         <v>630</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <f>Confirmed!AD45+Daily!L36</f>
+        <v>635</v>
+      </c>
+      <c r="M36">
+        <f>Confirmed!AE45+Daily!M36</f>
+        <v>643</v>
+      </c>
+      <c r="N36">
+        <f>Confirmed!AF45+Daily!N36</f>
+        <v>644</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>415</v>
       </c>
@@ -10371,8 +11646,20 @@
         <f>Confirmed!AC46+Daily!K37</f>
         <v>506</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37">
+        <f>Confirmed!AD46+Daily!L37</f>
+        <v>516</v>
+      </c>
+      <c r="M37">
+        <f>Confirmed!AE46+Daily!M37</f>
+        <v>527</v>
+      </c>
+      <c r="N37">
+        <f>Confirmed!AF46+Daily!N37</f>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>416</v>
       </c>
@@ -10416,8 +11703,20 @@
         <f>Confirmed!AC47+Daily!K38</f>
         <v>504</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L38">
+        <f>Confirmed!AD47+Daily!L38</f>
+        <v>520</v>
+      </c>
+      <c r="M38">
+        <f>Confirmed!AE47+Daily!M38</f>
+        <v>523</v>
+      </c>
+      <c r="N38">
+        <f>Confirmed!AF47+Daily!N38</f>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>417</v>
       </c>
@@ -10461,8 +11760,20 @@
         <f>Confirmed!AC48+Daily!K39</f>
         <v>448</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39">
+        <f>Confirmed!AD48+Daily!L39</f>
+        <v>451</v>
+      </c>
+      <c r="M39">
+        <f>Confirmed!AE48+Daily!M39</f>
+        <v>452</v>
+      </c>
+      <c r="N39">
+        <f>Confirmed!AF48+Daily!N39</f>
+        <v>453</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>418</v>
       </c>
@@ -10486,8 +11797,20 @@
         <f>Confirmed!AC49+Daily!K40</f>
         <v>456</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40">
+        <f>Confirmed!AD49+Daily!L40</f>
+        <v>459</v>
+      </c>
+      <c r="M40">
+        <f>Confirmed!AE49+Daily!M40</f>
+        <v>465</v>
+      </c>
+      <c r="N40">
+        <f>Confirmed!AF49+Daily!N40</f>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>419</v>
       </c>
@@ -10511,8 +11834,20 @@
         <f>Confirmed!AC50+Daily!K41</f>
         <v>426</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41">
+        <f>Confirmed!AD50+Daily!L41</f>
+        <v>439</v>
+      </c>
+      <c r="M41">
+        <f>Confirmed!AE50+Daily!M41</f>
+        <v>444</v>
+      </c>
+      <c r="N41">
+        <f>Confirmed!AF50+Daily!N41</f>
+        <v>448</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>420</v>
       </c>
@@ -10528,8 +11863,20 @@
         <f>Confirmed!AC51+Daily!K42</f>
         <v>421</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L42">
+        <f>Confirmed!AD51+Daily!L42</f>
+        <v>426</v>
+      </c>
+      <c r="M42">
+        <f>Confirmed!AE51+Daily!M42</f>
+        <v>434</v>
+      </c>
+      <c r="N42">
+        <f>Confirmed!AF51+Daily!N42</f>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>421</v>
       </c>
@@ -10541,8 +11888,20 @@
         <f>Confirmed!AC52+Daily!K43</f>
         <v>296</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L43">
+        <f>Confirmed!AD52+Daily!L43</f>
+        <v>354</v>
+      </c>
+      <c r="M43">
+        <f>Confirmed!AE52+Daily!M43</f>
+        <v>360</v>
+      </c>
+      <c r="N43">
+        <f>Confirmed!AF52+Daily!N43</f>
+        <v>379</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>422</v>
       </c>
@@ -10554,8 +11913,20 @@
         <f>Confirmed!AC53+Daily!K44</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L44">
+        <f>Confirmed!AD53+Daily!L44</f>
+        <v>279</v>
+      </c>
+      <c r="M44">
+        <f>Confirmed!AE53+Daily!M44</f>
+        <v>335</v>
+      </c>
+      <c r="N44">
+        <f>Confirmed!AF53+Daily!N44</f>
+        <v>357</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>423</v>
       </c>
@@ -10563,8 +11934,20 @@
         <f>Confirmed!AC54+Daily!K45</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L45">
+        <f>Confirmed!AD54+Daily!L45</f>
+        <v>40</v>
+      </c>
+      <c r="M45">
+        <f>Confirmed!AE54+Daily!M45</f>
+        <v>294</v>
+      </c>
+      <c r="N45">
+        <f>Confirmed!AF54+Daily!N45</f>
+        <v>352</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>424</v>
       </c>
@@ -10572,13 +11955,43 @@
         <f>Confirmed!AC55+Daily!K46</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L46">
+        <f>Confirmed!AD55+Daily!L46</f>
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <f>Confirmed!AE55+Daily!M46</f>
+        <v>32</v>
+      </c>
+      <c r="N46">
+        <f>Confirmed!AF55+Daily!N46</f>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>425</v>
       </c>
       <c r="K47">
         <f>Confirmed!AC56+Daily!K47</f>
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <f>Confirmed!AD56+Daily!L47</f>
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <f>Confirmed!AE56+Daily!M47</f>
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <f>Confirmed!AF56+Daily!N47</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N48">
+        <f>Confirmed!AF57+Daily!N48</f>
         <v>0</v>
       </c>
     </row>
@@ -11227,8 +12640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11337,7 +12750,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" ref="E9:E52" si="1">E8+1</f>
+        <f t="shared" ref="E9:E53" si="1">E8+1</f>
         <v>43902</v>
       </c>
     </row>
@@ -11540,7 +12953,7 @@
         <v>81</v>
       </c>
       <c r="D20">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="1"/>
@@ -11556,10 +12969,10 @@
         <v>190</v>
       </c>
       <c r="C21">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D21">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="1"/>
@@ -11613,7 +13026,7 @@
         <v>289</v>
       </c>
       <c r="C24">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D24">
         <v>45</v>
@@ -11632,7 +13045,7 @@
         <v>319</v>
       </c>
       <c r="C25">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D25">
         <v>64</v>
@@ -11651,10 +13064,10 @@
         <v>374</v>
       </c>
       <c r="C26">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D26">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="1"/>
@@ -11670,10 +13083,10 @@
         <v>450</v>
       </c>
       <c r="C27">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D27">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="1"/>
@@ -11689,7 +13102,7 @@
         <v>514</v>
       </c>
       <c r="C28">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D28">
         <v>99</v>
@@ -11708,10 +13121,10 @@
         <v>549</v>
       </c>
       <c r="C29">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="D29">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="1"/>
@@ -11727,10 +13140,10 @@
         <v>624</v>
       </c>
       <c r="C30">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="D30">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="1"/>
@@ -11746,10 +13159,10 @@
         <v>599</v>
       </c>
       <c r="C31">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="D31">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E31" s="2">
         <f t="shared" si="1"/>
@@ -11765,10 +13178,10 @@
         <v>628</v>
       </c>
       <c r="C32">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="D32">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" si="1"/>
@@ -11784,10 +13197,10 @@
         <v>757</v>
       </c>
       <c r="C33">
-        <v>517</v>
+        <v>526</v>
       </c>
       <c r="D33">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" si="1"/>
@@ -11803,10 +13216,10 @@
         <v>789</v>
       </c>
       <c r="C34">
-        <v>523</v>
+        <v>534</v>
       </c>
       <c r="D34">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="1"/>
@@ -11822,10 +13235,10 @@
         <v>797</v>
       </c>
       <c r="C35">
-        <v>546</v>
+        <v>555</v>
       </c>
       <c r="D35">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="1"/>
@@ -11841,10 +13254,10 @@
         <v>729</v>
       </c>
       <c r="C36">
-        <v>474</v>
+        <v>499</v>
       </c>
       <c r="D36">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="1"/>
@@ -11860,10 +13273,10 @@
         <v>804</v>
       </c>
       <c r="C37">
-        <v>481</v>
+        <v>502</v>
       </c>
       <c r="D37">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="1"/>
@@ -11879,10 +13292,10 @@
         <v>755</v>
       </c>
       <c r="C38">
-        <v>453</v>
+        <v>477</v>
       </c>
       <c r="D38">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="1"/>
@@ -11898,10 +13311,10 @@
         <v>742</v>
       </c>
       <c r="C39">
-        <v>448</v>
+        <v>476</v>
       </c>
       <c r="D39">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" si="1"/>
@@ -11917,10 +13330,10 @@
         <v>754</v>
       </c>
       <c r="C40">
-        <v>455</v>
+        <v>492</v>
       </c>
       <c r="D40">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" si="1"/>
@@ -11936,10 +13349,10 @@
         <v>757</v>
       </c>
       <c r="C41">
-        <v>453</v>
+        <v>487</v>
       </c>
       <c r="D41">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" si="1"/>
@@ -11955,10 +13368,10 @@
         <v>777</v>
       </c>
       <c r="C42">
-        <v>389</v>
+        <v>445</v>
       </c>
       <c r="D42">
-        <v>241</v>
+        <v>199</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" si="1"/>
@@ -11974,10 +13387,10 @@
         <v>683</v>
       </c>
       <c r="C43">
-        <v>335</v>
+        <v>382</v>
       </c>
       <c r="D43">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="E43" s="2">
         <f t="shared" si="1"/>
@@ -11993,10 +13406,10 @@
         <v>623</v>
       </c>
       <c r="C44">
-        <v>274</v>
+        <v>334</v>
       </c>
       <c r="D44">
-        <v>230</v>
+        <v>191</v>
       </c>
       <c r="E44" s="2">
         <f t="shared" si="1"/>
@@ -12012,10 +13425,10 @@
         <v>568</v>
       </c>
       <c r="C45">
-        <v>268</v>
+        <v>302</v>
       </c>
       <c r="D45">
-        <v>180</v>
+        <v>151</v>
       </c>
       <c r="E45" s="2">
         <f t="shared" si="1"/>
@@ -12031,10 +13444,10 @@
         <v>527</v>
       </c>
       <c r="C46">
-        <v>246</v>
+        <v>295</v>
       </c>
       <c r="D46">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="E46" s="2">
         <f t="shared" si="1"/>
@@ -12050,10 +13463,10 @@
         <v>522</v>
       </c>
       <c r="C47">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="D47">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="E47" s="2">
         <f t="shared" si="1"/>
@@ -12069,10 +13482,10 @@
         <v>459</v>
       </c>
       <c r="C48">
-        <v>185</v>
+        <v>264</v>
       </c>
       <c r="D48">
-        <v>236</v>
+        <v>177</v>
       </c>
       <c r="E48" s="2">
         <f t="shared" si="1"/>
@@ -12088,10 +13501,10 @@
         <v>378</v>
       </c>
       <c r="C49">
-        <v>76</v>
+        <v>215</v>
       </c>
       <c r="D49">
-        <v>220</v>
+        <v>164</v>
       </c>
       <c r="E49" s="2">
         <f t="shared" si="1"/>
@@ -12107,10 +13520,10 @@
         <v>365</v>
       </c>
       <c r="C50">
-        <v>15</v>
+        <v>192</v>
       </c>
       <c r="D50">
-        <v>30</v>
+        <v>165</v>
       </c>
       <c r="E50" s="2">
         <f t="shared" si="1"/>
@@ -12125,6 +13538,12 @@
       <c r="B51">
         <v>328</v>
       </c>
+      <c r="C51">
+        <v>161</v>
+      </c>
+      <c r="D51">
+        <v>191</v>
+      </c>
       <c r="E51" s="2">
         <f t="shared" si="1"/>
         <v>43944</v>
@@ -12138,6 +13557,12 @@
       <c r="B52">
         <v>323</v>
       </c>
+      <c r="C52">
+        <v>81</v>
+      </c>
+      <c r="D52">
+        <v>200</v>
+      </c>
       <c r="E52" s="2">
         <f t="shared" si="1"/>
         <v>43945</v>
@@ -12151,6 +13576,16 @@
       <c r="B53">
         <v>353</v>
       </c>
+      <c r="C53">
+        <v>10</v>
+      </c>
+      <c r="D53">
+        <v>14</v>
+      </c>
+      <c r="E53" s="2">
+        <f t="shared" si="1"/>
+        <v>43946</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1">

</xml_diff>

<commit_message>
Fix to account for changed fieldname PROBABLE_COUNT
</commit_message>
<xml_diff>
--- a/excelsheets/probables.xlsx
+++ b/excelsheets/probables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16692" windowHeight="6756" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16692" windowHeight="6756" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="5" r:id="rId1"/>
@@ -252,7 +252,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1148,8 +1147,8 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="296040992"/>
-        <c:axId val="296041552"/>
+        <c:axId val="295107600"/>
+        <c:axId val="295108160"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1690,11 +1689,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="296040992"/>
-        <c:axId val="296041552"/>
+        <c:axId val="295107600"/>
+        <c:axId val="295108160"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="296040992"/>
+        <c:axId val="295107600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1736,7 +1735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296041552"/>
+        <c:crossAx val="295108160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1745,7 +1744,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="296041552"/>
+        <c:axId val="295108160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1795,7 +1794,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296040992"/>
+        <c:crossAx val="295107600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1809,7 +1808,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3633,15 +3631,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection sqref="A1:N47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -3681,8 +3679,11 @@
       <c r="N1">
         <v>426</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>311</v>
       </c>
@@ -3693,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>312</v>
       </c>
@@ -3704,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>313</v>
       </c>
@@ -3715,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314</v>
       </c>
@@ -3741,7 +3742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>315</v>
       </c>
@@ -3764,7 +3765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>316</v>
       </c>
@@ -3811,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>317</v>
       </c>
@@ -3861,7 +3862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>318</v>
       </c>
@@ -3911,7 +3912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>319</v>
       </c>
@@ -3961,7 +3962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>320</v>
       </c>
@@ -4011,7 +4012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>321</v>
       </c>
@@ -4061,7 +4062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>322</v>
       </c>
@@ -4111,7 +4112,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>323</v>
       </c>
@@ -4161,7 +4162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>324</v>
       </c>
@@ -4211,7 +4212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>325</v>
       </c>
@@ -12640,7 +12641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11:D53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed one coding issue w/clinicaltrials spreadsheet
</commit_message>
<xml_diff>
--- a/excelsheets/probables.xlsx
+++ b/excelsheets/probables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16692" windowHeight="6756" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16692" windowHeight="6756" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="5" r:id="rId1"/>
@@ -252,6 +252,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -618,7 +619,7 @@
                   <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>93</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>121</c:v>
@@ -627,22 +628,22 @@
                   <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>207</c:v>
+                  <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>263</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>278</c:v>
+                  <c:v>277</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>305</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>363</c:v>
+                  <c:v>365</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>408</c:v>
+                  <c:v>411</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>445</c:v>
@@ -651,70 +652,73 @@
                   <c:v>456</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>469</c:v>
+                  <c:v>463</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>526</c:v>
+                  <c:v>520</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>534</c:v>
+                  <c:v>538</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>555</c:v>
+                  <c:v>556</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>499</c:v>
+                  <c:v>502</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>502</c:v>
+                  <c:v>505</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>477</c:v>
+                  <c:v>478</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>476</c:v>
+                  <c:v>479</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>492</c:v>
+                  <c:v>494</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>487</c:v>
+                  <c:v>488</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>445</c:v>
+                  <c:v>453</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>382</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>334</c:v>
+                  <c:v>338</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>302</c:v>
+                  <c:v>308</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>295</c:v>
+                  <c:v>301</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>283</c:v>
+                  <c:v>292</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>264</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>215</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>192</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>161</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>81</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>10</c:v>
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1004,12 +1008,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1035,7 +1033,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>19</c:v>
@@ -1044,22 +1042,22 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>75</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>99</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>119</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>196</c:v>
@@ -1068,16 +1066,16 @@
                   <c:v>191</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>211</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>203</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>258</c:v>
+                  <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>257</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>233</c:v>
@@ -1086,52 +1084,55 @@
                   <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>222</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>206</c:v>
+                  <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>225</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>239</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>199</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>148</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>191</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>151</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>174</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>165</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>177</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>164</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>165</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>191</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>200</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>14</c:v>
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1147,8 +1148,8 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="295107600"/>
-        <c:axId val="295108160"/>
+        <c:axId val="295113200"/>
+        <c:axId val="108548784"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1689,11 +1690,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="295107600"/>
-        <c:axId val="295108160"/>
+        <c:axId val="295113200"/>
+        <c:axId val="108548784"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="295107600"/>
+        <c:axId val="295113200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1735,7 +1736,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295108160"/>
+        <c:crossAx val="108548784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1744,7 +1745,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="295108160"/>
+        <c:axId val="108548784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1794,7 +1795,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295107600"/>
+        <c:crossAx val="295113200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1808,6 +1809,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3631,10 +3633,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5:O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3811,6 +3813,9 @@
       <c r="N7">
         <v>1</v>
       </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -3861,6 +3866,9 @@
       <c r="N8">
         <v>4</v>
       </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -3911,6 +3919,9 @@
       <c r="N9">
         <v>4</v>
       </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -3961,6 +3972,9 @@
       <c r="N10">
         <v>2</v>
       </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -4011,6 +4025,9 @@
       <c r="N11">
         <v>4</v>
       </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -4061,6 +4078,9 @@
       <c r="N12">
         <v>5</v>
       </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -4111,6 +4131,9 @@
       <c r="N13">
         <v>4</v>
       </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -4161,6 +4184,9 @@
       <c r="N14">
         <v>15</v>
       </c>
+      <c r="O14">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -4211,6 +4237,9 @@
       <c r="N15">
         <v>12</v>
       </c>
+      <c r="O15">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -4261,8 +4290,11 @@
       <c r="N16">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>326</v>
       </c>
@@ -4311,8 +4343,11 @@
       <c r="N17">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>327</v>
       </c>
@@ -4361,8 +4396,11 @@
       <c r="N18">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O18">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>328</v>
       </c>
@@ -4411,8 +4449,11 @@
       <c r="N19">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>329</v>
       </c>
@@ -4461,8 +4502,11 @@
       <c r="N20">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O20">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>330</v>
       </c>
@@ -4511,8 +4555,11 @@
       <c r="N21">
         <v>93</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O21">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>331</v>
       </c>
@@ -4561,8 +4608,11 @@
       <c r="N22">
         <v>99</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O22">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>401</v>
       </c>
@@ -4611,8 +4661,11 @@
       <c r="N23">
         <v>119</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O23">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>402</v>
       </c>
@@ -4661,8 +4714,11 @@
       <c r="N24">
         <v>196</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O24">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>403</v>
       </c>
@@ -4711,8 +4767,11 @@
       <c r="N25">
         <v>191</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>404</v>
       </c>
@@ -4761,8 +4820,11 @@
       <c r="N26">
         <v>211</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O26">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>405</v>
       </c>
@@ -4811,8 +4873,11 @@
       <c r="N27">
         <v>203</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O27">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>406</v>
       </c>
@@ -4861,8 +4926,11 @@
       <c r="N28">
         <v>258</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O28">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>407</v>
       </c>
@@ -4911,8 +4979,11 @@
       <c r="N29">
         <v>257</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O29">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>408</v>
       </c>
@@ -4961,8 +5032,11 @@
       <c r="N30">
         <v>233</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O30">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>409</v>
       </c>
@@ -5011,8 +5085,11 @@
       <c r="N31">
         <v>227</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O31">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>410</v>
       </c>
@@ -5061,8 +5138,11 @@
       <c r="N32">
         <v>222</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O32">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>411</v>
       </c>
@@ -5111,8 +5191,11 @@
       <c r="N33">
         <v>206</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O33">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>412</v>
       </c>
@@ -5161,8 +5244,11 @@
       <c r="N34">
         <v>225</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O34">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>413</v>
       </c>
@@ -5211,8 +5297,11 @@
       <c r="N35">
         <v>239</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>414</v>
       </c>
@@ -5257,8 +5346,11 @@
       <c r="N36">
         <v>199</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O36">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>415</v>
       </c>
@@ -5299,8 +5391,11 @@
       <c r="N37">
         <v>148</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O37">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>416</v>
       </c>
@@ -5337,8 +5432,11 @@
       <c r="N38">
         <v>191</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O38">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>417</v>
       </c>
@@ -5371,8 +5469,11 @@
       <c r="N39">
         <v>151</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O39">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>418</v>
       </c>
@@ -5401,8 +5502,11 @@
       <c r="N40">
         <v>174</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O40">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>419</v>
       </c>
@@ -5424,8 +5528,11 @@
       <c r="N41">
         <v>165</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O41">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>420</v>
       </c>
@@ -5447,8 +5554,11 @@
       <c r="N42">
         <v>177</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O42">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>421</v>
       </c>
@@ -5467,8 +5577,11 @@
       <c r="N43">
         <v>164</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O43">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>422</v>
       </c>
@@ -5484,8 +5597,11 @@
       <c r="N44">
         <v>165</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O44">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>423</v>
       </c>
@@ -5498,8 +5614,11 @@
       <c r="N45">
         <v>191</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O45">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>424</v>
       </c>
@@ -5509,13 +5628,24 @@
       <c r="N46">
         <v>200</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O46">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>425</v>
       </c>
       <c r="N47">
         <v>14</v>
+      </c>
+      <c r="O47">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O48">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -5525,15 +5655,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF56"/>
+  <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AF11" sqref="A1:AF56"/>
+    <sheetView topLeftCell="S41" workbookViewId="0">
+      <selection activeCell="AG11" sqref="AG11:AG57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>325</v>
       </c>
@@ -5628,7 +5758,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>302</v>
       </c>
@@ -5714,7 +5844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>303</v>
       </c>
@@ -5800,7 +5930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>304</v>
       </c>
@@ -5886,7 +6016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>305</v>
       </c>
@@ -5972,7 +6102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>306</v>
       </c>
@@ -6058,7 +6188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>307</v>
       </c>
@@ -6144,7 +6274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>308</v>
       </c>
@@ -6230,7 +6360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>309</v>
       </c>
@@ -6316,7 +6446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>310</v>
       </c>
@@ -6402,7 +6532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>311</v>
       </c>
@@ -6499,8 +6629,11 @@
       <c r="AF11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>312</v>
       </c>
@@ -6597,8 +6730,11 @@
       <c r="AF12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>313</v>
       </c>
@@ -6695,8 +6831,11 @@
       <c r="AF13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>314</v>
       </c>
@@ -6793,8 +6932,11 @@
       <c r="AF14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>315</v>
       </c>
@@ -6891,8 +7033,11 @@
       <c r="AF15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>316</v>
       </c>
@@ -6989,8 +7134,11 @@
       <c r="AF16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>317</v>
       </c>
@@ -7087,8 +7235,11 @@
       <c r="AF17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>318</v>
       </c>
@@ -7185,8 +7336,11 @@
       <c r="AF18">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>319</v>
       </c>
@@ -7283,8 +7437,11 @@
       <c r="AF19">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>320</v>
       </c>
@@ -7381,8 +7538,11 @@
       <c r="AF20">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG20">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>321</v>
       </c>
@@ -7479,8 +7639,11 @@
       <c r="AF21">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG21">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>322</v>
       </c>
@@ -7577,8 +7740,11 @@
       <c r="AF22">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG22">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>323</v>
       </c>
@@ -7675,8 +7841,11 @@
       <c r="AF23">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG23">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>324</v>
       </c>
@@ -7773,8 +7942,11 @@
       <c r="AF24">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>325</v>
       </c>
@@ -7871,8 +8043,11 @@
       <c r="AF25">
         <v>121</v>
       </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>326</v>
       </c>
@@ -7966,8 +8141,11 @@
       <c r="AF26">
         <v>185</v>
       </c>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG26">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>327</v>
       </c>
@@ -8058,8 +8236,11 @@
       <c r="AF27">
         <v>207</v>
       </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG27">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>328</v>
       </c>
@@ -8147,8 +8328,11 @@
       <c r="AF28">
         <v>263</v>
       </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG28">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>329</v>
       </c>
@@ -8236,8 +8420,11 @@
       <c r="AF29">
         <v>278</v>
       </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG29">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>330</v>
       </c>
@@ -8325,8 +8512,11 @@
       <c r="AF30">
         <v>305</v>
       </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG30">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>331</v>
       </c>
@@ -8411,8 +8601,11 @@
       <c r="AF31">
         <v>363</v>
       </c>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG31">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>401</v>
       </c>
@@ -8494,8 +8687,11 @@
       <c r="AF32">
         <v>408</v>
       </c>
-    </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG32">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>402</v>
       </c>
@@ -8574,8 +8770,11 @@
       <c r="AF33">
         <v>445</v>
       </c>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG33">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>403</v>
       </c>
@@ -8651,8 +8850,11 @@
       <c r="AF34">
         <v>456</v>
       </c>
-    </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG34">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>404</v>
       </c>
@@ -8725,8 +8927,11 @@
       <c r="AF35">
         <v>469</v>
       </c>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG35">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>405</v>
       </c>
@@ -8796,8 +9001,11 @@
       <c r="AF36">
         <v>526</v>
       </c>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG36">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>406</v>
       </c>
@@ -8864,8 +9072,11 @@
       <c r="AF37">
         <v>534</v>
       </c>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG37">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>407</v>
       </c>
@@ -8929,8 +9140,11 @@
       <c r="AF38">
         <v>555</v>
       </c>
-    </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG38">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>408</v>
       </c>
@@ -8991,8 +9205,11 @@
       <c r="AF39">
         <v>499</v>
       </c>
-    </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG39">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>409</v>
       </c>
@@ -9050,8 +9267,11 @@
       <c r="AF40">
         <v>502</v>
       </c>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG40">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>410</v>
       </c>
@@ -9106,8 +9326,11 @@
       <c r="AF41">
         <v>477</v>
       </c>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG41">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>411</v>
       </c>
@@ -9159,8 +9382,11 @@
       <c r="AF42">
         <v>476</v>
       </c>
-    </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG42">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>412</v>
       </c>
@@ -9209,8 +9435,11 @@
       <c r="AF43">
         <v>492</v>
       </c>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG43">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>413</v>
       </c>
@@ -9256,8 +9485,11 @@
       <c r="AF44">
         <v>487</v>
       </c>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG44">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>414</v>
       </c>
@@ -9297,8 +9529,11 @@
       <c r="AF45">
         <v>445</v>
       </c>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG45">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>415</v>
       </c>
@@ -9335,8 +9570,11 @@
       <c r="AF46">
         <v>382</v>
       </c>
-    </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG46">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>416</v>
       </c>
@@ -9370,8 +9608,11 @@
       <c r="AF47">
         <v>334</v>
       </c>
-    </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG47">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>417</v>
       </c>
@@ -9402,8 +9643,11 @@
       <c r="AF48">
         <v>302</v>
       </c>
-    </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG48">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>418</v>
       </c>
@@ -9431,8 +9675,11 @@
       <c r="AF49">
         <v>295</v>
       </c>
-    </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG49">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>419</v>
       </c>
@@ -9457,8 +9704,11 @@
       <c r="AF50">
         <v>283</v>
       </c>
-    </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG50">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>420</v>
       </c>
@@ -9480,8 +9730,11 @@
       <c r="AF51">
         <v>264</v>
       </c>
-    </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG51">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>421</v>
       </c>
@@ -9500,8 +9753,11 @@
       <c r="AF52">
         <v>215</v>
       </c>
-    </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG52">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>422</v>
       </c>
@@ -9517,8 +9773,11 @@
       <c r="AF53">
         <v>192</v>
       </c>
-    </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG53">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>423</v>
       </c>
@@ -9531,8 +9790,11 @@
       <c r="AF54">
         <v>161</v>
       </c>
-    </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG54">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>424</v>
       </c>
@@ -9542,13 +9804,24 @@
       <c r="AF55">
         <v>81</v>
       </c>
-    </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG55">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>425</v>
       </c>
       <c r="AF56">
         <v>10</v>
+      </c>
+      <c r="AG56">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AG57">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -9558,15 +9831,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="N47" sqref="N47"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -9607,8 +9880,11 @@
       <c r="N1">
         <v>426</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>311</v>
       </c>
@@ -9664,8 +9940,12 @@
         <f>Confirmed!AF11+Daily!N2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2">
+        <f>Confirmed!AG11+Daily!O2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>312</v>
       </c>
@@ -9721,8 +10001,12 @@
         <f>Confirmed!AF12+Daily!N3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3">
+        <f>Confirmed!AG12+Daily!O3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>313</v>
       </c>
@@ -9778,8 +10062,12 @@
         <f>Confirmed!AF13+Daily!N4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4">
+        <f>Confirmed!AG13+Daily!O4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314</v>
       </c>
@@ -9835,8 +10123,12 @@
         <f>Confirmed!AF14+Daily!N5</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5">
+        <f>Confirmed!AG14+Daily!O5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>315</v>
       </c>
@@ -9892,8 +10184,12 @@
         <f>Confirmed!AF15+Daily!N6</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6">
+        <f>Confirmed!AG15+Daily!O6</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>316</v>
       </c>
@@ -9949,8 +10245,12 @@
         <f>Confirmed!AF16+Daily!N7</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7">
+        <f>Confirmed!AG16+Daily!O7</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>317</v>
       </c>
@@ -10006,8 +10306,12 @@
         <f>Confirmed!AF17+Daily!N8</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O8">
+        <f>Confirmed!AG17+Daily!O8</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>318</v>
       </c>
@@ -10063,8 +10367,12 @@
         <f>Confirmed!AF18+Daily!N9</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9">
+        <f>Confirmed!AG18+Daily!O9</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>319</v>
       </c>
@@ -10120,8 +10428,12 @@
         <f>Confirmed!AF19+Daily!N10</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O10">
+        <f>Confirmed!AG19+Daily!O10</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>320</v>
       </c>
@@ -10177,8 +10489,12 @@
         <f>Confirmed!AF20+Daily!N11</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O11">
+        <f>Confirmed!AG20+Daily!O11</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>321</v>
       </c>
@@ -10234,8 +10550,12 @@
         <f>Confirmed!AF21+Daily!N12</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O12">
+        <f>Confirmed!AG21+Daily!O12</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>322</v>
       </c>
@@ -10291,8 +10611,12 @@
         <f>Confirmed!AF22+Daily!N13</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O13">
+        <f>Confirmed!AG22+Daily!O13</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>323</v>
       </c>
@@ -10348,8 +10672,12 @@
         <f>Confirmed!AF23+Daily!N14</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O14">
+        <f>Confirmed!AG23+Daily!O14</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>324</v>
       </c>
@@ -10405,8 +10733,12 @@
         <f>Confirmed!AF24+Daily!N15</f>
         <v>105</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O15">
+        <f>Confirmed!AG24+Daily!O15</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>325</v>
       </c>
@@ -10462,8 +10794,12 @@
         <f>Confirmed!AF25+Daily!N16</f>
         <v>140</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O16">
+        <f>Confirmed!AG25+Daily!O16</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>326</v>
       </c>
@@ -10519,8 +10855,12 @@
         <f>Confirmed!AF26+Daily!N17</f>
         <v>225</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O17">
+        <f>Confirmed!AG26+Daily!O17</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>327</v>
       </c>
@@ -10576,8 +10916,12 @@
         <f>Confirmed!AF27+Daily!N18</f>
         <v>252</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O18">
+        <f>Confirmed!AG27+Daily!O18</f>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>328</v>
       </c>
@@ -10633,8 +10977,12 @@
         <f>Confirmed!AF28+Daily!N19</f>
         <v>327</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O19">
+        <f>Confirmed!AG28+Daily!O19</f>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>329</v>
       </c>
@@ -10690,8 +11038,12 @@
         <f>Confirmed!AF29+Daily!N20</f>
         <v>353</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O20">
+        <f>Confirmed!AG29+Daily!O20</f>
+        <v>353</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>330</v>
       </c>
@@ -10747,8 +11099,12 @@
         <f>Confirmed!AF30+Daily!N21</f>
         <v>398</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O21">
+        <f>Confirmed!AG30+Daily!O21</f>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>331</v>
       </c>
@@ -10804,8 +11160,12 @@
         <f>Confirmed!AF31+Daily!N22</f>
         <v>462</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O22">
+        <f>Confirmed!AG31+Daily!O22</f>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>401</v>
       </c>
@@ -10861,8 +11221,12 @@
         <f>Confirmed!AF32+Daily!N23</f>
         <v>527</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O23">
+        <f>Confirmed!AG32+Daily!O23</f>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>402</v>
       </c>
@@ -10918,8 +11282,12 @@
         <f>Confirmed!AF33+Daily!N24</f>
         <v>641</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O24">
+        <f>Confirmed!AG33+Daily!O24</f>
+        <v>641</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>403</v>
       </c>
@@ -10975,8 +11343,12 @@
         <f>Confirmed!AF34+Daily!N25</f>
         <v>647</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O25">
+        <f>Confirmed!AG34+Daily!O25</f>
+        <v>647</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>404</v>
       </c>
@@ -11032,8 +11404,12 @@
         <f>Confirmed!AF35+Daily!N26</f>
         <v>680</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O26">
+        <f>Confirmed!AG35+Daily!O26</f>
+        <v>679</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>405</v>
       </c>
@@ -11089,8 +11465,12 @@
         <f>Confirmed!AF36+Daily!N27</f>
         <v>729</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O27">
+        <f>Confirmed!AG36+Daily!O27</f>
+        <v>728</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>406</v>
       </c>
@@ -11146,8 +11526,12 @@
         <f>Confirmed!AF37+Daily!N28</f>
         <v>792</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O28">
+        <f>Confirmed!AG37+Daily!O28</f>
+        <v>792</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>407</v>
       </c>
@@ -11203,8 +11587,12 @@
         <f>Confirmed!AF38+Daily!N29</f>
         <v>812</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O29">
+        <f>Confirmed!AG38+Daily!O29</f>
+        <v>811</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>408</v>
       </c>
@@ -11260,8 +11648,12 @@
         <f>Confirmed!AF39+Daily!N30</f>
         <v>732</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O30">
+        <f>Confirmed!AG39+Daily!O30</f>
+        <v>735</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>409</v>
       </c>
@@ -11317,8 +11709,12 @@
         <f>Confirmed!AF40+Daily!N31</f>
         <v>729</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O31">
+        <f>Confirmed!AG40+Daily!O31</f>
+        <v>732</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>410</v>
       </c>
@@ -11374,8 +11770,12 @@
         <f>Confirmed!AF41+Daily!N32</f>
         <v>699</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O32">
+        <f>Confirmed!AG41+Daily!O32</f>
+        <v>699</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>411</v>
       </c>
@@ -11431,8 +11831,12 @@
         <f>Confirmed!AF42+Daily!N33</f>
         <v>682</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O33">
+        <f>Confirmed!AG42+Daily!O33</f>
+        <v>684</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>412</v>
       </c>
@@ -11488,8 +11892,12 @@
         <f>Confirmed!AF43+Daily!N34</f>
         <v>717</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O34">
+        <f>Confirmed!AG43+Daily!O34</f>
+        <v>718</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>413</v>
       </c>
@@ -11545,8 +11953,12 @@
         <f>Confirmed!AF44+Daily!N35</f>
         <v>726</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O35">
+        <f>Confirmed!AG44+Daily!O35</f>
+        <v>727</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>414</v>
       </c>
@@ -11602,8 +12014,12 @@
         <f>Confirmed!AF45+Daily!N36</f>
         <v>644</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O36">
+        <f>Confirmed!AG45+Daily!O36</f>
+        <v>645</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>415</v>
       </c>
@@ -11659,8 +12075,12 @@
         <f>Confirmed!AF46+Daily!N37</f>
         <v>530</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O37">
+        <f>Confirmed!AG46+Daily!O37</f>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>416</v>
       </c>
@@ -11716,8 +12136,12 @@
         <f>Confirmed!AF47+Daily!N38</f>
         <v>525</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O38">
+        <f>Confirmed!AG47+Daily!O38</f>
+        <v>526</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>417</v>
       </c>
@@ -11773,8 +12197,12 @@
         <f>Confirmed!AF48+Daily!N39</f>
         <v>453</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O39">
+        <f>Confirmed!AG48+Daily!O39</f>
+        <v>453</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>418</v>
       </c>
@@ -11810,8 +12238,12 @@
         <f>Confirmed!AF49+Daily!N40</f>
         <v>469</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O40">
+        <f>Confirmed!AG49+Daily!O40</f>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>419</v>
       </c>
@@ -11847,8 +12279,12 @@
         <f>Confirmed!AF50+Daily!N41</f>
         <v>448</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O41">
+        <f>Confirmed!AG50+Daily!O41</f>
+        <v>449</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>420</v>
       </c>
@@ -11876,8 +12312,12 @@
         <f>Confirmed!AF51+Daily!N42</f>
         <v>441</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O42">
+        <f>Confirmed!AG51+Daily!O42</f>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>421</v>
       </c>
@@ -11901,8 +12341,12 @@
         <f>Confirmed!AF52+Daily!N43</f>
         <v>379</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O43">
+        <f>Confirmed!AG52+Daily!O43</f>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>422</v>
       </c>
@@ -11926,8 +12370,12 @@
         <f>Confirmed!AF53+Daily!N44</f>
         <v>357</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O44">
+        <f>Confirmed!AG53+Daily!O44</f>
+        <v>362</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>423</v>
       </c>
@@ -11947,8 +12395,12 @@
         <f>Confirmed!AF54+Daily!N45</f>
         <v>352</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O45">
+        <f>Confirmed!AG54+Daily!O45</f>
+        <v>357</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>424</v>
       </c>
@@ -11968,8 +12420,12 @@
         <f>Confirmed!AF55+Daily!N46</f>
         <v>281</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O46">
+        <f>Confirmed!AG55+Daily!O46</f>
+        <v>321</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>425</v>
       </c>
@@ -11989,10 +12445,27 @@
         <f>Confirmed!AF56+Daily!N47</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O47">
+        <f>Confirmed!AG56+Daily!O47</f>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>426</v>
+      </c>
       <c r="N48">
         <f>Confirmed!AF57+Daily!N48</f>
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <f>Confirmed!AG57+Daily!O48</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O49">
+        <f>Confirmed!AG58+Daily!O49</f>
         <v>0</v>
       </c>
     </row>
@@ -12641,8 +13114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D53"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12751,7 +13224,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" ref="E9:E53" si="1">E8+1</f>
+        <f t="shared" ref="E9:E54" si="1">E8+1</f>
         <v>43902</v>
       </c>
     </row>
@@ -12782,9 +13255,6 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
       <c r="E11" s="2">
         <f t="shared" si="1"/>
         <v>43904</v>
@@ -12801,9 +13271,6 @@
       <c r="C12">
         <v>6</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
       <c r="E12" s="2">
         <f t="shared" si="1"/>
         <v>43905</v>
@@ -12970,10 +13437,10 @@
         <v>190</v>
       </c>
       <c r="C21">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D21">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="1"/>
@@ -13027,10 +13494,10 @@
         <v>289</v>
       </c>
       <c r="C24">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D24">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="1"/>
@@ -13065,10 +13532,10 @@
         <v>374</v>
       </c>
       <c r="C26">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D26">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="1"/>
@@ -13084,7 +13551,7 @@
         <v>450</v>
       </c>
       <c r="C27">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D27">
         <v>93</v>
@@ -13103,10 +13570,10 @@
         <v>514</v>
       </c>
       <c r="C28">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D28">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="1"/>
@@ -13122,10 +13589,10 @@
         <v>549</v>
       </c>
       <c r="C29">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="D29">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="1"/>
@@ -13179,10 +13646,10 @@
         <v>628</v>
       </c>
       <c r="C32">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="D32">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" si="1"/>
@@ -13198,10 +13665,10 @@
         <v>757</v>
       </c>
       <c r="C33">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="D33">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" si="1"/>
@@ -13217,10 +13684,10 @@
         <v>789</v>
       </c>
       <c r="C34">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="D34">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="1"/>
@@ -13236,10 +13703,10 @@
         <v>797</v>
       </c>
       <c r="C35">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D35">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="1"/>
@@ -13255,7 +13722,7 @@
         <v>729</v>
       </c>
       <c r="C36">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="D36">
         <v>233</v>
@@ -13274,7 +13741,7 @@
         <v>804</v>
       </c>
       <c r="C37">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="D37">
         <v>227</v>
@@ -13293,10 +13760,10 @@
         <v>755</v>
       </c>
       <c r="C38">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D38">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="1"/>
@@ -13312,10 +13779,10 @@
         <v>742</v>
       </c>
       <c r="C39">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="D39">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" si="1"/>
@@ -13331,10 +13798,10 @@
         <v>754</v>
       </c>
       <c r="C40">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="D40">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" si="1"/>
@@ -13350,7 +13817,7 @@
         <v>757</v>
       </c>
       <c r="C41">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D41">
         <v>239</v>
@@ -13369,10 +13836,10 @@
         <v>777</v>
       </c>
       <c r="C42">
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="D42">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" si="1"/>
@@ -13388,10 +13855,10 @@
         <v>683</v>
       </c>
       <c r="C43">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="D43">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E43" s="2">
         <f t="shared" si="1"/>
@@ -13407,10 +13874,10 @@
         <v>623</v>
       </c>
       <c r="C44">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="D44">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E44" s="2">
         <f t="shared" si="1"/>
@@ -13426,10 +13893,10 @@
         <v>568</v>
       </c>
       <c r="C45">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="D45">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E45" s="2">
         <f t="shared" si="1"/>
@@ -13445,10 +13912,10 @@
         <v>527</v>
       </c>
       <c r="C46">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="D46">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E46" s="2">
         <f t="shared" si="1"/>
@@ -13464,10 +13931,10 @@
         <v>522</v>
       </c>
       <c r="C47">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="D47">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E47" s="2">
         <f t="shared" si="1"/>
@@ -13483,10 +13950,10 @@
         <v>459</v>
       </c>
       <c r="C48">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="D48">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E48" s="2">
         <f t="shared" si="1"/>
@@ -13502,10 +13969,10 @@
         <v>378</v>
       </c>
       <c r="C49">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="D49">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E49" s="2">
         <f t="shared" si="1"/>
@@ -13521,10 +13988,10 @@
         <v>365</v>
       </c>
       <c r="C50">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="D50">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="E50" s="2">
         <f t="shared" si="1"/>
@@ -13540,10 +14007,10 @@
         <v>328</v>
       </c>
       <c r="C51">
-        <v>161</v>
+        <v>201</v>
       </c>
       <c r="D51">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="E51" s="2">
         <f t="shared" si="1"/>
@@ -13559,10 +14026,10 @@
         <v>323</v>
       </c>
       <c r="C52">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="D52">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="E52" s="2">
         <f t="shared" si="1"/>
@@ -13578,10 +14045,10 @@
         <v>353</v>
       </c>
       <c r="C53">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="D53">
-        <v>14</v>
+        <v>142</v>
       </c>
       <c r="E53" s="2">
         <f t="shared" si="1"/>
@@ -13596,6 +14063,16 @@
       <c r="B54">
         <v>221</v>
       </c>
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="D54">
+        <v>17</v>
+      </c>
+      <c r="E54" s="2">
+        <f t="shared" si="1"/>
+        <v>43947</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1">

</xml_diff>

<commit_message>
Apr 28 update, delete of extraneous files.
</commit_message>
<xml_diff>
--- a/excelsheets/probables.xlsx
+++ b/excelsheets/probables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16692" windowHeight="6756" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16692" windowHeight="6756" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="5" r:id="rId1"/>
@@ -628,43 +628,43 @@
                   <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>205</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>263</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>277</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>306</c:v>
+                  <c:v>305</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>365</c:v>
+                  <c:v>364</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>411</c:v>
+                  <c:v>412</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>445</c:v>
+                  <c:v>446</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>456</c:v>
+                  <c:v>454</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>463</c:v>
+                  <c:v>470</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>520</c:v>
+                  <c:v>524</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>538</c:v>
+                  <c:v>539</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>556</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>502</c:v>
+                  <c:v>501</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>505</c:v>
@@ -679,25 +679,25 @@
                   <c:v>494</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>488</c:v>
+                  <c:v>487</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>453</c:v>
+                  <c:v>454</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>386</c:v>
+                  <c:v>388</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>338</c:v>
+                  <c:v>339</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>308</c:v>
+                  <c:v>309</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>301</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>292</c:v>
+                  <c:v>293</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>275</c:v>
@@ -706,19 +706,22 @@
                   <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>217</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>201</c:v>
+                  <c:v>203</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>57</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>7</c:v>
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1042,7 +1045,7 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>47</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>64</c:v>
@@ -1051,88 +1054,91 @@
                   <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>93</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>97</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>118</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>196</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>191</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>216</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>208</c:v>
+                  <c:v>203</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>254</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>255</c:v>
-                </c:pt>
                 <c:pt idx="34">
-                  <c:v>233</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>221</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>224</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>239</c:v>
+                  <c:v>238</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>192</c:v>
+                  <c:v>191</c:v>
                 </c:pt>
                 <c:pt idx="41">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>144</c:v>
                 </c:pt>
-                <c:pt idx="42">
-                  <c:v>188</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>145</c:v>
-                </c:pt>
                 <c:pt idx="44">
-                  <c:v>168</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>166</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>145</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>156</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>176</c:v>
+                  <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>142</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>17</c:v>
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1148,8 +1154,8 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="295113200"/>
-        <c:axId val="108548784"/>
+        <c:axId val="290811040"/>
+        <c:axId val="290811600"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1690,11 +1696,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="295113200"/>
-        <c:axId val="108548784"/>
+        <c:axId val="290811040"/>
+        <c:axId val="290811600"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="295113200"/>
+        <c:axId val="290811040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1736,7 +1742,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108548784"/>
+        <c:crossAx val="290811600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1745,7 +1751,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="108548784"/>
+        <c:axId val="290811600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1795,7 +1801,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295113200"/>
+        <c:crossAx val="290811040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2438,7 +2444,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="58" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3633,15 +3639,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O48"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5:O48"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7:P49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -3684,8 +3690,11 @@
       <c r="O1">
         <v>427</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>311</v>
       </c>
@@ -3696,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>312</v>
       </c>
@@ -3707,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>313</v>
       </c>
@@ -3718,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314</v>
       </c>
@@ -3744,7 +3753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>315</v>
       </c>
@@ -3767,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>316</v>
       </c>
@@ -3816,8 +3825,11 @@
       <c r="O7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>317</v>
       </c>
@@ -3869,8 +3881,11 @@
       <c r="O8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>318</v>
       </c>
@@ -3922,8 +3937,11 @@
       <c r="O9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>319</v>
       </c>
@@ -3975,8 +3993,11 @@
       <c r="O10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>320</v>
       </c>
@@ -4028,8 +4049,11 @@
       <c r="O11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>321</v>
       </c>
@@ -4081,8 +4105,11 @@
       <c r="O12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>322</v>
       </c>
@@ -4134,8 +4161,11 @@
       <c r="O13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>323</v>
       </c>
@@ -4187,8 +4217,11 @@
       <c r="O14">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>324</v>
       </c>
@@ -4240,8 +4273,11 @@
       <c r="O15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>325</v>
       </c>
@@ -4293,8 +4329,11 @@
       <c r="O16">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>326</v>
       </c>
@@ -4346,8 +4385,11 @@
       <c r="O17">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>327</v>
       </c>
@@ -4399,8 +4441,11 @@
       <c r="O18">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>328</v>
       </c>
@@ -4452,8 +4497,11 @@
       <c r="O19">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>329</v>
       </c>
@@ -4505,8 +4553,11 @@
       <c r="O20">
         <v>76</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>330</v>
       </c>
@@ -4558,8 +4609,11 @@
       <c r="O21">
         <v>93</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>331</v>
       </c>
@@ -4611,8 +4665,11 @@
       <c r="O22">
         <v>97</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>401</v>
       </c>
@@ -4664,8 +4721,11 @@
       <c r="O23">
         <v>118</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>402</v>
       </c>
@@ -4717,8 +4777,11 @@
       <c r="O24">
         <v>196</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>403</v>
       </c>
@@ -4770,8 +4833,11 @@
       <c r="O25">
         <v>191</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>404</v>
       </c>
@@ -4823,8 +4889,11 @@
       <c r="O26">
         <v>216</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>405</v>
       </c>
@@ -4876,8 +4945,11 @@
       <c r="O27">
         <v>208</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>406</v>
       </c>
@@ -4929,8 +5001,11 @@
       <c r="O28">
         <v>254</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P28">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>407</v>
       </c>
@@ -4982,8 +5057,11 @@
       <c r="O29">
         <v>255</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P29">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>408</v>
       </c>
@@ -5035,8 +5113,11 @@
       <c r="O30">
         <v>233</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P30">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>409</v>
       </c>
@@ -5088,8 +5169,11 @@
       <c r="O31">
         <v>227</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P31">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>410</v>
       </c>
@@ -5141,8 +5225,11 @@
       <c r="O32">
         <v>221</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P32">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>411</v>
       </c>
@@ -5194,8 +5281,11 @@
       <c r="O33">
         <v>205</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P33">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>412</v>
       </c>
@@ -5247,8 +5337,11 @@
       <c r="O34">
         <v>224</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P34">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>413</v>
       </c>
@@ -5300,8 +5393,11 @@
       <c r="O35">
         <v>239</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>414</v>
       </c>
@@ -5349,8 +5445,11 @@
       <c r="O36">
         <v>192</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P36">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>415</v>
       </c>
@@ -5394,8 +5493,11 @@
       <c r="O37">
         <v>144</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P37">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>416</v>
       </c>
@@ -5435,8 +5537,11 @@
       <c r="O38">
         <v>188</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P38">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>417</v>
       </c>
@@ -5472,8 +5577,11 @@
       <c r="O39">
         <v>145</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P39">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>418</v>
       </c>
@@ -5505,8 +5613,11 @@
       <c r="O40">
         <v>168</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P40">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>419</v>
       </c>
@@ -5531,8 +5642,11 @@
       <c r="O41">
         <v>157</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P41">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>420</v>
       </c>
@@ -5557,8 +5671,11 @@
       <c r="O42">
         <v>166</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P42">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>421</v>
       </c>
@@ -5580,8 +5697,11 @@
       <c r="O43">
         <v>156</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P43">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>422</v>
       </c>
@@ -5600,8 +5720,11 @@
       <c r="O44">
         <v>145</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P44">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>423</v>
       </c>
@@ -5617,8 +5740,11 @@
       <c r="O45">
         <v>156</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P45">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>424</v>
       </c>
@@ -5631,8 +5757,11 @@
       <c r="O46">
         <v>176</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P46">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>425</v>
       </c>
@@ -5642,10 +5771,21 @@
       <c r="O47">
         <v>142</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P47">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O48">
         <v>17</v>
+      </c>
+      <c r="P48">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="16:16" x14ac:dyDescent="0.3">
+      <c r="P49">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -5655,15 +5795,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG57"/>
+  <dimension ref="A1:AH58"/>
   <sheetViews>
-    <sheetView topLeftCell="S41" workbookViewId="0">
-      <selection activeCell="AG11" sqref="AG11:AG57"/>
+    <sheetView topLeftCell="V41" workbookViewId="0">
+      <selection activeCell="AH11" sqref="AH11:AH58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>325</v>
       </c>
@@ -5757,8 +5897,14 @@
       <c r="AF1">
         <v>426</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AG1">
+        <v>427</v>
+      </c>
+      <c r="AH1">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>302</v>
       </c>
@@ -5844,7 +5990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>303</v>
       </c>
@@ -5930,7 +6076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>304</v>
       </c>
@@ -6016,7 +6162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>305</v>
       </c>
@@ -6102,7 +6248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>306</v>
       </c>
@@ -6188,7 +6334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>307</v>
       </c>
@@ -6274,7 +6420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>308</v>
       </c>
@@ -6360,7 +6506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>309</v>
       </c>
@@ -6446,7 +6592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>310</v>
       </c>
@@ -6532,7 +6678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>311</v>
       </c>
@@ -6632,8 +6778,11 @@
       <c r="AG11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>312</v>
       </c>
@@ -6733,8 +6882,11 @@
       <c r="AG12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>313</v>
       </c>
@@ -6834,8 +6986,11 @@
       <c r="AG13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>314</v>
       </c>
@@ -6935,8 +7090,11 @@
       <c r="AG14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>315</v>
       </c>
@@ -7036,8 +7194,11 @@
       <c r="AG15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>316</v>
       </c>
@@ -7137,8 +7298,11 @@
       <c r="AG16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>317</v>
       </c>
@@ -7238,8 +7402,11 @@
       <c r="AG17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>318</v>
       </c>
@@ -7339,8 +7506,11 @@
       <c r="AG18">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>319</v>
       </c>
@@ -7440,8 +7610,11 @@
       <c r="AG19">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>320</v>
       </c>
@@ -7541,8 +7714,11 @@
       <c r="AG20">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH20">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>321</v>
       </c>
@@ -7642,8 +7818,11 @@
       <c r="AG21">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH21">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>322</v>
       </c>
@@ -7743,8 +7922,11 @@
       <c r="AG22">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH22">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>323</v>
       </c>
@@ -7844,8 +8026,11 @@
       <c r="AG23">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH23">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>324</v>
       </c>
@@ -7945,8 +8130,11 @@
       <c r="AG24">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>325</v>
       </c>
@@ -8046,8 +8234,11 @@
       <c r="AG25">
         <v>121</v>
       </c>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>326</v>
       </c>
@@ -8144,8 +8335,11 @@
       <c r="AG26">
         <v>185</v>
       </c>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH26">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>327</v>
       </c>
@@ -8239,8 +8433,11 @@
       <c r="AG27">
         <v>205</v>
       </c>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH27">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>328</v>
       </c>
@@ -8331,8 +8528,11 @@
       <c r="AG28">
         <v>263</v>
       </c>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH28">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>329</v>
       </c>
@@ -8423,8 +8623,11 @@
       <c r="AG29">
         <v>277</v>
       </c>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH29">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>330</v>
       </c>
@@ -8515,8 +8718,11 @@
       <c r="AG30">
         <v>306</v>
       </c>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH30">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>331</v>
       </c>
@@ -8604,8 +8810,11 @@
       <c r="AG31">
         <v>365</v>
       </c>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH31">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>401</v>
       </c>
@@ -8690,8 +8899,11 @@
       <c r="AG32">
         <v>411</v>
       </c>
-    </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH32">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>402</v>
       </c>
@@ -8773,8 +8985,11 @@
       <c r="AG33">
         <v>445</v>
       </c>
-    </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH33">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>403</v>
       </c>
@@ -8853,8 +9068,11 @@
       <c r="AG34">
         <v>456</v>
       </c>
-    </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH34">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>404</v>
       </c>
@@ -8930,8 +9148,11 @@
       <c r="AG35">
         <v>463</v>
       </c>
-    </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH35">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>405</v>
       </c>
@@ -9004,8 +9225,11 @@
       <c r="AG36">
         <v>520</v>
       </c>
-    </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH36">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>406</v>
       </c>
@@ -9075,8 +9299,11 @@
       <c r="AG37">
         <v>538</v>
       </c>
-    </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH37">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>407</v>
       </c>
@@ -9143,8 +9370,11 @@
       <c r="AG38">
         <v>556</v>
       </c>
-    </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH38">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>408</v>
       </c>
@@ -9208,8 +9438,11 @@
       <c r="AG39">
         <v>502</v>
       </c>
-    </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH39">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>409</v>
       </c>
@@ -9270,8 +9503,11 @@
       <c r="AG40">
         <v>505</v>
       </c>
-    </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH40">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>410</v>
       </c>
@@ -9329,8 +9565,11 @@
       <c r="AG41">
         <v>478</v>
       </c>
-    </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH41">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>411</v>
       </c>
@@ -9385,8 +9624,11 @@
       <c r="AG42">
         <v>479</v>
       </c>
-    </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH42">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>412</v>
       </c>
@@ -9438,8 +9680,11 @@
       <c r="AG43">
         <v>494</v>
       </c>
-    </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH43">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>413</v>
       </c>
@@ -9488,8 +9733,11 @@
       <c r="AG44">
         <v>488</v>
       </c>
-    </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH44">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>414</v>
       </c>
@@ -9532,8 +9780,11 @@
       <c r="AG45">
         <v>453</v>
       </c>
-    </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH45">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>415</v>
       </c>
@@ -9573,8 +9824,11 @@
       <c r="AG46">
         <v>386</v>
       </c>
-    </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH46">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="47" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>416</v>
       </c>
@@ -9611,8 +9865,11 @@
       <c r="AG47">
         <v>338</v>
       </c>
-    </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH47">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="48" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>417</v>
       </c>
@@ -9646,8 +9903,11 @@
       <c r="AG48">
         <v>308</v>
       </c>
-    </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH48">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="49" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>418</v>
       </c>
@@ -9678,8 +9938,11 @@
       <c r="AG49">
         <v>301</v>
       </c>
-    </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH49">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>419</v>
       </c>
@@ -9707,8 +9970,11 @@
       <c r="AG50">
         <v>292</v>
       </c>
-    </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH50">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="51" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>420</v>
       </c>
@@ -9733,8 +9999,11 @@
       <c r="AG51">
         <v>275</v>
       </c>
-    </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH51">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="52" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>421</v>
       </c>
@@ -9756,8 +10025,11 @@
       <c r="AG52">
         <v>226</v>
       </c>
-    </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH52">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>422</v>
       </c>
@@ -9776,8 +10048,11 @@
       <c r="AG53">
         <v>217</v>
       </c>
-    </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH53">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>423</v>
       </c>
@@ -9793,8 +10068,11 @@
       <c r="AG54">
         <v>201</v>
       </c>
-    </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH54">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>424</v>
       </c>
@@ -9807,8 +10085,11 @@
       <c r="AG55">
         <v>145</v>
       </c>
-    </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH55">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>425</v>
       </c>
@@ -9818,10 +10099,21 @@
       <c r="AG56">
         <v>57</v>
       </c>
-    </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH56">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
       <c r="AG57">
         <v>7</v>
+      </c>
+      <c r="AH57">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="AH58">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -9831,15 +10123,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O49"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="P49" sqref="P49:P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>414</v>
       </c>
@@ -9883,8 +10175,11 @@
       <c r="O1">
         <v>427</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>311</v>
       </c>
@@ -9944,8 +10239,12 @@
         <f>Confirmed!AG11+Daily!O2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2">
+        <f>Confirmed!AH11+Daily!P2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>312</v>
       </c>
@@ -10005,8 +10304,12 @@
         <f>Confirmed!AG12+Daily!O3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3">
+        <f>Confirmed!AH12+Daily!P3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>313</v>
       </c>
@@ -10066,8 +10369,12 @@
         <f>Confirmed!AG13+Daily!O4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <f>Confirmed!AH13+Daily!P4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>314</v>
       </c>
@@ -10127,8 +10434,12 @@
         <f>Confirmed!AG14+Daily!O5</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5">
+        <f>Confirmed!AH14+Daily!P5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>315</v>
       </c>
@@ -10188,8 +10499,12 @@
         <f>Confirmed!AG15+Daily!O6</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <f>Confirmed!AH15+Daily!P6</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>316</v>
       </c>
@@ -10249,8 +10564,12 @@
         <f>Confirmed!AG16+Daily!O7</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <f>Confirmed!AH16+Daily!P7</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>317</v>
       </c>
@@ -10310,8 +10629,12 @@
         <f>Confirmed!AG17+Daily!O8</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <f>Confirmed!AH17+Daily!P8</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>318</v>
       </c>
@@ -10371,8 +10694,12 @@
         <f>Confirmed!AG18+Daily!O9</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9">
+        <f>Confirmed!AH18+Daily!P9</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>319</v>
       </c>
@@ -10432,8 +10759,12 @@
         <f>Confirmed!AG19+Daily!O10</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10">
+        <f>Confirmed!AH19+Daily!P10</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>320</v>
       </c>
@@ -10493,8 +10824,12 @@
         <f>Confirmed!AG20+Daily!O11</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11">
+        <f>Confirmed!AH20+Daily!P11</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>321</v>
       </c>
@@ -10554,8 +10889,12 @@
         <f>Confirmed!AG21+Daily!O12</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <f>Confirmed!AH21+Daily!P12</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>322</v>
       </c>
@@ -10615,8 +10954,12 @@
         <f>Confirmed!AG22+Daily!O13</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13">
+        <f>Confirmed!AH22+Daily!P13</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>323</v>
       </c>
@@ -10676,8 +11019,12 @@
         <f>Confirmed!AG23+Daily!O14</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <f>Confirmed!AH23+Daily!P14</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>324</v>
       </c>
@@ -10737,8 +11084,12 @@
         <f>Confirmed!AG24+Daily!O15</f>
         <v>105</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <f>Confirmed!AH24+Daily!P15</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>325</v>
       </c>
@@ -10798,8 +11149,12 @@
         <f>Confirmed!AG25+Daily!O16</f>
         <v>140</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <f>Confirmed!AH25+Daily!P16</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>326</v>
       </c>
@@ -10859,8 +11214,12 @@
         <f>Confirmed!AG26+Daily!O17</f>
         <v>225</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <f>Confirmed!AH26+Daily!P17</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>327</v>
       </c>
@@ -10920,8 +11279,12 @@
         <f>Confirmed!AG27+Daily!O18</f>
         <v>252</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18">
+        <f>Confirmed!AH27+Daily!P18</f>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>328</v>
       </c>
@@ -10981,8 +11344,12 @@
         <f>Confirmed!AG28+Daily!O19</f>
         <v>327</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <f>Confirmed!AH28+Daily!P19</f>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>329</v>
       </c>
@@ -11042,8 +11409,12 @@
         <f>Confirmed!AG29+Daily!O20</f>
         <v>353</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20">
+        <f>Confirmed!AH29+Daily!P20</f>
+        <v>353</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>330</v>
       </c>
@@ -11103,8 +11474,12 @@
         <f>Confirmed!AG30+Daily!O21</f>
         <v>399</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21">
+        <f>Confirmed!AH30+Daily!P21</f>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>331</v>
       </c>
@@ -11164,8 +11539,12 @@
         <f>Confirmed!AG31+Daily!O22</f>
         <v>462</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22">
+        <f>Confirmed!AH31+Daily!P22</f>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>401</v>
       </c>
@@ -11225,8 +11604,12 @@
         <f>Confirmed!AG32+Daily!O23</f>
         <v>529</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23">
+        <f>Confirmed!AH32+Daily!P23</f>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>402</v>
       </c>
@@ -11286,8 +11669,12 @@
         <f>Confirmed!AG33+Daily!O24</f>
         <v>641</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24">
+        <f>Confirmed!AH33+Daily!P24</f>
+        <v>641</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>403</v>
       </c>
@@ -11347,8 +11734,12 @@
         <f>Confirmed!AG34+Daily!O25</f>
         <v>647</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25">
+        <f>Confirmed!AH34+Daily!P25</f>
+        <v>647</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>404</v>
       </c>
@@ -11408,8 +11799,12 @@
         <f>Confirmed!AG35+Daily!O26</f>
         <v>679</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26">
+        <f>Confirmed!AH35+Daily!P26</f>
+        <v>679</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>405</v>
       </c>
@@ -11469,8 +11864,12 @@
         <f>Confirmed!AG36+Daily!O27</f>
         <v>728</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27">
+        <f>Confirmed!AH36+Daily!P27</f>
+        <v>727</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>406</v>
       </c>
@@ -11530,8 +11929,12 @@
         <f>Confirmed!AG37+Daily!O28</f>
         <v>792</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P28">
+        <f>Confirmed!AH37+Daily!P28</f>
+        <v>790</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>407</v>
       </c>
@@ -11591,8 +11994,12 @@
         <f>Confirmed!AG38+Daily!O29</f>
         <v>811</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P29">
+        <f>Confirmed!AH38+Daily!P29</f>
+        <v>810</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>408</v>
       </c>
@@ -11652,8 +12059,12 @@
         <f>Confirmed!AG39+Daily!O30</f>
         <v>735</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P30">
+        <f>Confirmed!AH39+Daily!P30</f>
+        <v>735</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>409</v>
       </c>
@@ -11713,8 +12124,12 @@
         <f>Confirmed!AG40+Daily!O31</f>
         <v>732</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P31">
+        <f>Confirmed!AH40+Daily!P31</f>
+        <v>732</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>410</v>
       </c>
@@ -11774,8 +12189,12 @@
         <f>Confirmed!AG41+Daily!O32</f>
         <v>699</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P32">
+        <f>Confirmed!AH41+Daily!P32</f>
+        <v>698</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>411</v>
       </c>
@@ -11835,8 +12254,12 @@
         <f>Confirmed!AG42+Daily!O33</f>
         <v>684</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P33">
+        <f>Confirmed!AH42+Daily!P33</f>
+        <v>684</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>412</v>
       </c>
@@ -11896,8 +12319,12 @@
         <f>Confirmed!AG43+Daily!O34</f>
         <v>718</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P34">
+        <f>Confirmed!AH43+Daily!P34</f>
+        <v>717</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>413</v>
       </c>
@@ -11957,8 +12384,12 @@
         <f>Confirmed!AG44+Daily!O35</f>
         <v>727</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P35">
+        <f>Confirmed!AH44+Daily!P35</f>
+        <v>725</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>414</v>
       </c>
@@ -12018,8 +12449,12 @@
         <f>Confirmed!AG45+Daily!O36</f>
         <v>645</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P36">
+        <f>Confirmed!AH45+Daily!P36</f>
+        <v>645</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>415</v>
       </c>
@@ -12079,8 +12514,12 @@
         <f>Confirmed!AG46+Daily!O37</f>
         <v>530</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P37">
+        <f>Confirmed!AH46+Daily!P37</f>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>416</v>
       </c>
@@ -12140,8 +12579,12 @@
         <f>Confirmed!AG47+Daily!O38</f>
         <v>526</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P38">
+        <f>Confirmed!AH47+Daily!P38</f>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>417</v>
       </c>
@@ -12201,8 +12644,12 @@
         <f>Confirmed!AG48+Daily!O39</f>
         <v>453</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P39">
+        <f>Confirmed!AH48+Daily!P39</f>
+        <v>453</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>418</v>
       </c>
@@ -12242,8 +12689,12 @@
         <f>Confirmed!AG49+Daily!O40</f>
         <v>469</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P40">
+        <f>Confirmed!AH49+Daily!P40</f>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>419</v>
       </c>
@@ -12283,8 +12734,12 @@
         <f>Confirmed!AG50+Daily!O41</f>
         <v>449</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P41">
+        <f>Confirmed!AH50+Daily!P41</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>420</v>
       </c>
@@ -12316,8 +12771,12 @@
         <f>Confirmed!AG51+Daily!O42</f>
         <v>441</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P42">
+        <f>Confirmed!AH51+Daily!P42</f>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>421</v>
       </c>
@@ -12345,8 +12804,12 @@
         <f>Confirmed!AG52+Daily!O43</f>
         <v>382</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P43">
+        <f>Confirmed!AH52+Daily!P43</f>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>422</v>
       </c>
@@ -12374,8 +12837,12 @@
         <f>Confirmed!AG53+Daily!O44</f>
         <v>362</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P44">
+        <f>Confirmed!AH53+Daily!P44</f>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>423</v>
       </c>
@@ -12399,8 +12866,12 @@
         <f>Confirmed!AG54+Daily!O45</f>
         <v>357</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P45">
+        <f>Confirmed!AH54+Daily!P45</f>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>424</v>
       </c>
@@ -12424,8 +12895,12 @@
         <f>Confirmed!AG55+Daily!O46</f>
         <v>321</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P46">
+        <f>Confirmed!AH55+Daily!P46</f>
+        <v>329</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>425</v>
       </c>
@@ -12449,8 +12924,12 @@
         <f>Confirmed!AG56+Daily!O47</f>
         <v>199</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P47">
+        <f>Confirmed!AH56+Daily!P47</f>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>426</v>
       </c>
@@ -12462,10 +12941,24 @@
         <f>Confirmed!AG57+Daily!O48</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="49" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="P48">
+        <f>Confirmed!AH57+Daily!P48</f>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="49" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O49">
         <f>Confirmed!AG58+Daily!O49</f>
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <f>Confirmed!AH58+Daily!P49</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="P50">
+        <f>Confirmed!AH59+Daily!P50</f>
         <v>0</v>
       </c>
     </row>
@@ -13114,8 +13607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13224,7 +13717,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" ref="E9:E54" si="1">E8+1</f>
+        <f t="shared" ref="E9:E55" si="1">E8+1</f>
         <v>43902</v>
       </c>
     </row>
@@ -13494,10 +13987,10 @@
         <v>289</v>
       </c>
       <c r="C24">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D24">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="1"/>
@@ -13513,7 +14006,7 @@
         <v>319</v>
       </c>
       <c r="C25">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D25">
         <v>64</v>
@@ -13551,10 +14044,10 @@
         <v>450</v>
       </c>
       <c r="C27">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D27">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="1"/>
@@ -13570,10 +14063,10 @@
         <v>514</v>
       </c>
       <c r="C28">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D28">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="1"/>
@@ -13589,10 +14082,10 @@
         <v>549</v>
       </c>
       <c r="C29">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D29">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="1"/>
@@ -13608,10 +14101,10 @@
         <v>624</v>
       </c>
       <c r="C30">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D30">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="1"/>
@@ -13627,10 +14120,10 @@
         <v>599</v>
       </c>
       <c r="C31">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D31">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E31" s="2">
         <f t="shared" si="1"/>
@@ -13646,10 +14139,10 @@
         <v>628</v>
       </c>
       <c r="C32">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="D32">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" si="1"/>
@@ -13665,10 +14158,10 @@
         <v>757</v>
       </c>
       <c r="C33">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="D33">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" si="1"/>
@@ -13684,10 +14177,10 @@
         <v>789</v>
       </c>
       <c r="C34">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D34">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="1"/>
@@ -13706,7 +14199,7 @@
         <v>556</v>
       </c>
       <c r="D35">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="1"/>
@@ -13722,10 +14215,10 @@
         <v>729</v>
       </c>
       <c r="C36">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D36">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="1"/>
@@ -13763,7 +14256,7 @@
         <v>478</v>
       </c>
       <c r="D38">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="1"/>
@@ -13801,7 +14294,7 @@
         <v>494</v>
       </c>
       <c r="D40">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" si="1"/>
@@ -13817,10 +14310,10 @@
         <v>757</v>
       </c>
       <c r="C41">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D41">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" si="1"/>
@@ -13836,10 +14329,10 @@
         <v>777</v>
       </c>
       <c r="C42">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D42">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" si="1"/>
@@ -13855,10 +14348,10 @@
         <v>683</v>
       </c>
       <c r="C43">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D43">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E43" s="2">
         <f t="shared" si="1"/>
@@ -13874,10 +14367,10 @@
         <v>623</v>
       </c>
       <c r="C44">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D44">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E44" s="2">
         <f t="shared" si="1"/>
@@ -13893,10 +14386,10 @@
         <v>568</v>
       </c>
       <c r="C45">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D45">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E45" s="2">
         <f t="shared" si="1"/>
@@ -13915,7 +14408,7 @@
         <v>301</v>
       </c>
       <c r="D46">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E46" s="2">
         <f t="shared" si="1"/>
@@ -13931,7 +14424,7 @@
         <v>522</v>
       </c>
       <c r="C47">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D47">
         <v>157</v>
@@ -13953,7 +14446,7 @@
         <v>275</v>
       </c>
       <c r="D48">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E48" s="2">
         <f t="shared" si="1"/>
@@ -13988,10 +14481,10 @@
         <v>365</v>
       </c>
       <c r="C50">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D50">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E50" s="2">
         <f t="shared" si="1"/>
@@ -14007,10 +14500,10 @@
         <v>328</v>
       </c>
       <c r="C51">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D51">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E51" s="2">
         <f t="shared" si="1"/>
@@ -14029,7 +14522,7 @@
         <v>145</v>
       </c>
       <c r="D52">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E52" s="2">
         <f t="shared" si="1"/>
@@ -14045,10 +14538,10 @@
         <v>353</v>
       </c>
       <c r="C53">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="D53">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="E53" s="2">
         <f t="shared" si="1"/>
@@ -14064,10 +14557,10 @@
         <v>221</v>
       </c>
       <c r="C54">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="D54">
-        <v>17</v>
+        <v>151</v>
       </c>
       <c r="E54" s="2">
         <f t="shared" si="1"/>
@@ -14082,6 +14575,16 @@
       <c r="B55">
         <v>214</v>
       </c>
+      <c r="C55">
+        <v>10</v>
+      </c>
+      <c r="D55">
+        <v>19</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="1"/>
+        <v>43948</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">

</xml_diff>